<commit_message>
i363--Apollo eit2 suite added
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/radiant/silicon_07_apollo.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/radiant/silicon_07_apollo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\update\07_Apollo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="pSvbrBtM5D7J1tTbaFvNMFAx+gsFF1+zjWgivCK1irAkzVtGcdIaviGYDMewqTuAFCctlIpswoSn4Z8ezPPc6w==" workbookSaltValue="fuR2EkRIGc7n0eTkIKsWWA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="6300" windowWidth="28830" windowHeight="6240"/>
+    <workbookView xWindow="-15" yWindow="6300" windowWidth="28830" windowHeight="6240" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="suite" sheetId="1" r:id="rId1"/>
@@ -27,16 +27,16 @@
   </definedNames>
   <calcPr calcId="122211"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jeffrey Ye - Personal View" guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="3"/>
+    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
+    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
     <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
-    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
-    <customWorkbookView name="Jeffrey Ye - Personal View" guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="3"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="464">
   <si>
     <t>[suite_info]</t>
   </si>
@@ -864,6 +864,9 @@
     <t>Author column added</t>
   </si>
   <si>
+    <t>group = rna_regression_group</t>
+  </si>
+  <si>
     <t>Jeffrey</t>
   </si>
   <si>
@@ -888,9 +891,6 @@
     <t>=Primitive</t>
   </si>
   <si>
-    <t>cmd = python DEV/bin/run_radiant.py  --run-map-trce --run-par-trce  --run-export-bitstream</t>
-  </si>
-  <si>
     <t>=impl</t>
   </si>
   <si>
@@ -1017,33 +1017,15 @@
     <t>34</t>
   </si>
   <si>
-    <t>01_Logic/01_impl/101_LUT4</t>
-  </si>
-  <si>
     <t>inistantiate LUT4 and INIT="AB91"</t>
   </si>
   <si>
-    <t>01_Logic/01_impl/103_WIDEFN9</t>
-  </si>
-  <si>
     <t>inistantiate WIDEFN9:INIT1="AB91",INIT2="8899"</t>
   </si>
   <si>
-    <t>01_Logic/03_sim/101_LUT4</t>
-  </si>
-  <si>
-    <t>01_Logic/03_sim/103_WIDEFN9</t>
-  </si>
-  <si>
-    <t>02_CCU2/01_impl/202_CCU2_SUB</t>
-  </si>
-  <si>
     <t>Primitive: CCU2C with Substractor function</t>
   </si>
   <si>
-    <t>02_CCU2/03_sim/201_CCU2_ADD</t>
-  </si>
-  <si>
     <t xml:space="preserve">CCU2 mode: Addition </t>
   </si>
   <si>
@@ -1059,69 +1041,30 @@
     <t>FD1P3JX, basic function</t>
   </si>
   <si>
-    <t>04_Dist_RAM/01_impl/401_DPR16X4A_impl</t>
-  </si>
-  <si>
     <t>implemetation check, resource/clock/clock enable</t>
   </si>
   <si>
-    <t>04_Dist_RAM/01_impl/402_DPR32X2_impl</t>
-  </si>
-  <si>
-    <t>04_Dist_RAM/01_impl/403_SPR16X4A_impl</t>
-  </si>
-  <si>
-    <t>04_Dist_RAM/01_impl/404_SPR32X2_impl</t>
-  </si>
-  <si>
-    <t>04_Dist_RAM/03_sim/402_DPR16X4A_initial</t>
-  </si>
-  <si>
     <t>Instantiate 1 DPR16X4A with initial, check the read out data</t>
   </si>
   <si>
-    <t>04_Dist_RAM/03_sim/412_DPR32X2_initial</t>
-  </si>
-  <si>
     <t>Instantiate 1 DPR32X2 with initial, check the read out data</t>
   </si>
   <si>
-    <t>04_Dist_RAM/03_sim/422_SPR16X4A_initial</t>
-  </si>
-  <si>
     <t>Instantiate 1 SPR16X4A with initial, check the read out data</t>
   </si>
   <si>
-    <t>04_Dist_RAM/03_sim/432_SPR32X2_initial</t>
-  </si>
-  <si>
     <t>Instantiate 1 SPR32X2 with initial, check the read out data</t>
   </si>
   <si>
     <t>Clock</t>
   </si>
   <si>
-    <t>06_others/01_clcok/01_4_Clocks</t>
-  </si>
-  <si>
     <t>Infer 4 clcoks: A4, A8, C12 and C16</t>
   </si>
   <si>
     <t>primitive</t>
   </si>
   <si>
-    <t>08_IO/03_sim_cov/01_IB</t>
-  </si>
-  <si>
-    <t>08_IO/03_sim_cov/02_OB</t>
-  </si>
-  <si>
-    <t>08_IO/03_sim_cov/03_BB</t>
-  </si>
-  <si>
-    <t>08_IO/03_sim_cov/04_OBZ</t>
-  </si>
-  <si>
     <t>Mix</t>
   </si>
   <si>
@@ -1161,114 +1104,9 @@
     <t>cmd = --check-conf=sim.conf --synthesis=synplify --sim-rtl --sim-syn-vlg  --sim-par-vlg</t>
   </si>
   <si>
-    <t>06_others/02_mix/03_sim/01_SLICEMUX</t>
-  </si>
-  <si>
-    <t>06_others/02_mix/03_sim/02_VLO</t>
-  </si>
-  <si>
-    <t>06_others/02_mix/03_sim/03_VHI</t>
-  </si>
-  <si>
-    <t>06_others/02_mix/03_sim/04_INV</t>
-  </si>
-  <si>
-    <t>06_others/02_mix/03_sim/05_BUF</t>
-  </si>
-  <si>
-    <t>06_others/02_mix/03_sim/06_PUR</t>
-  </si>
-  <si>
-    <t>06_others/02_mix/03_sim/08_GSRA</t>
-  </si>
-  <si>
-    <t>suite_path = ITR1;</t>
-  </si>
-  <si>
-    <t>repository = http://lsh-tmp/radiant/trunk/silicon/07_Apollo</t>
-  </si>
-  <si>
-    <t>03_FF/03_sim/301_FD1P3BX</t>
-  </si>
-  <si>
-    <t>03_FF/03_sim/302_FD1P3DX</t>
-  </si>
-  <si>
-    <t>03_FF/03_sim/303_FD1P3IX</t>
-  </si>
-  <si>
-    <t>03_FF/03_sim/304_FD1P3JX</t>
-  </si>
-  <si>
-    <t>03_FF/01_impl/301_FD1P3BX</t>
-  </si>
-  <si>
-    <t>03_FF/01_impl/302_FD1P3DX</t>
-  </si>
-  <si>
-    <t>03_FF/01_impl/303_FD1P3IX</t>
-  </si>
-  <si>
-    <t>03_FF/01_impl/304_FD1P3JX</t>
-  </si>
-  <si>
     <t>radiant=sd_ng3_1.103</t>
   </si>
   <si>
-    <t>silicon_07_apollo_v1.01</t>
-  </si>
-  <si>
-    <t>07_SoftIP/01_Adder/101_Adder_16bit_Signed</t>
-  </si>
-  <si>
-    <t>07_SoftIP/02_Adder_Substractor/101_Adder_Sub_16bit_Unsign</t>
-  </si>
-  <si>
-    <t>07_SoftIP/03_Barrel_Shifter/101_Barrel_Shifter_default</t>
-  </si>
-  <si>
-    <t>07_SoftIP/04_Comparator/101_Comparator_8bit_Unsign_A_notequal_B</t>
-  </si>
-  <si>
-    <t>07_SoftIP/400_Distributed_DPRAM/401_Dist_DPRAM_default</t>
-  </si>
-  <si>
-    <t>07_SoftIP/410_Distributed_ROM/412_Dist_ROM_a2x4_bin</t>
-  </si>
-  <si>
-    <t>07_SoftIP/420_Distributed_SPRAM/422_Dist_SPRAM_a2x4</t>
-  </si>
-  <si>
-    <t>07_SoftIP/430_Mult_Add_Sub_Sum/431_Mult_Add_Sub_Sum_default</t>
-  </si>
-  <si>
-    <t>07_SoftIP/440_Multiplier/441_Multiplier_default</t>
-  </si>
-  <si>
-    <t>07_SoftIP/450_Sin_Cos_Table/452_Sincos_i3_o4_cos_lut_p2</t>
-  </si>
-  <si>
-    <t>07_SoftIP/460_Subtractor/461_Subtractor_default</t>
-  </si>
-  <si>
-    <t>07_SoftIP/301_FFT_Butterfly/301_FFT_2T_L_1_08_08_01_11</t>
-  </si>
-  <si>
-    <t>07_SoftIP/302_Convert/301_Cvt_8_0_S_8_0_T_W</t>
-  </si>
-  <si>
-    <t>07_SoftIP/304_LFSR/301_LFSR_F_XO_8_00_01_10</t>
-  </si>
-  <si>
-    <t>07_SoftIP/305_Complex_Mult/301_CpM_8_8_U_11_1_L</t>
-  </si>
-  <si>
-    <t>07_SoftIP/306_Mult_Accumulate/301_MA_A_18_18_37_SS_01_1_L</t>
-  </si>
-  <si>
-    <t>07_SoftIP/307_Mult_Add_Sub/301_MAS_A_9_9_SS_11_1_L</t>
-  </si>
-  <si>
     <t>SoftIP</t>
   </si>
   <si>
@@ -1332,9 +1170,6 @@
     <t>21_softIP_LSE</t>
   </si>
   <si>
-    <t>07_SoftIP/303_Counter/302_Cnt_1_U_0_1_0</t>
-  </si>
-  <si>
     <t>FOUNDRY_DRC_DISABLE=1;MA_PIO_LCT_NOT_READY=1;purBypassSpeedModelError=1</t>
   </si>
   <si>
@@ -1345,6 +1180,285 @@
   </si>
   <si>
     <t>=SoftIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cmd = python DEV/bin/run_radiant.py  --run-map-trce --run-par-trce  --run-export-bitstream --set-strategy="{par_disable_timing_driven=True}" </t>
+  </si>
+  <si>
+    <t>ITR1/01_Logic/01_impl/101_LUT4</t>
+  </si>
+  <si>
+    <t>ITR1/01_Logic/01_impl/103_WIDEFN9</t>
+  </si>
+  <si>
+    <t>ITR1/01_Logic/03_sim/101_LUT4</t>
+  </si>
+  <si>
+    <t>ITR1/01_Logic/03_sim/103_WIDEFN9</t>
+  </si>
+  <si>
+    <t>ITR1/02_CCU2/01_impl/202_CCU2_SUB</t>
+  </si>
+  <si>
+    <t>ITR1/02_CCU2/03_sim/201_CCU2_ADD</t>
+  </si>
+  <si>
+    <t>ITR1/03_FF/03_sim/301_FD1P3BX</t>
+  </si>
+  <si>
+    <t>ITR1/03_FF/03_sim/302_FD1P3DX</t>
+  </si>
+  <si>
+    <t>ITR1/03_FF/03_sim/303_FD1P3IX</t>
+  </si>
+  <si>
+    <t>ITR1/03_FF/03_sim/304_FD1P3JX</t>
+  </si>
+  <si>
+    <t>ITR1/03_FF/01_impl/301_FD1P3BX</t>
+  </si>
+  <si>
+    <t>ITR1/03_FF/01_impl/302_FD1P3DX</t>
+  </si>
+  <si>
+    <t>ITR1/03_FF/01_impl/303_FD1P3IX</t>
+  </si>
+  <si>
+    <t>ITR1/03_FF/01_impl/304_FD1P3JX</t>
+  </si>
+  <si>
+    <t>ITR1/04_Dist_RAM/01_impl/401_DPR16X4A_impl</t>
+  </si>
+  <si>
+    <t>ITR1/04_Dist_RAM/01_impl/402_DPR32X2_impl</t>
+  </si>
+  <si>
+    <t>ITR1/04_Dist_RAM/01_impl/403_SPR16X4A_impl</t>
+  </si>
+  <si>
+    <t>ITR1/04_Dist_RAM/01_impl/404_SPR32X2_impl</t>
+  </si>
+  <si>
+    <t>ITR1/04_Dist_RAM/03_sim/402_DPR16X4A_initial</t>
+  </si>
+  <si>
+    <t>ITR1/04_Dist_RAM/03_sim/412_DPR32X2_initial</t>
+  </si>
+  <si>
+    <t>ITR1/04_Dist_RAM/03_sim/422_SPR16X4A_initial</t>
+  </si>
+  <si>
+    <t>ITR1/04_Dist_RAM/03_sim/432_SPR32X2_initial</t>
+  </si>
+  <si>
+    <t>ITR1/06_others/01_clcok/01_4_Clocks</t>
+  </si>
+  <si>
+    <t>ITR1/06_others/02_mix/03_sim/01_SLICEMUX</t>
+  </si>
+  <si>
+    <t>ITR1/06_others/02_mix/03_sim/02_VLO</t>
+  </si>
+  <si>
+    <t>ITR1/06_others/02_mix/03_sim/03_VHI</t>
+  </si>
+  <si>
+    <t>ITR1/06_others/02_mix/03_sim/04_INV</t>
+  </si>
+  <si>
+    <t>ITR1/06_others/02_mix/03_sim/05_BUF</t>
+  </si>
+  <si>
+    <t>ITR1/06_others/02_mix/03_sim/06_PUR</t>
+  </si>
+  <si>
+    <t>ITR1/06_others/02_mix/03_sim/08_GSRA</t>
+  </si>
+  <si>
+    <t>ITR1/08_IO/03_sim_cov/01_IB</t>
+  </si>
+  <si>
+    <t>ITR1/08_IO/03_sim_cov/02_OB</t>
+  </si>
+  <si>
+    <t>ITR1/08_IO/03_sim_cov/03_BB</t>
+  </si>
+  <si>
+    <t>ITR1/08_IO/03_sim_cov/04_OBZ</t>
+  </si>
+  <si>
+    <t>ITR1/07_SoftIP/01_Adder/101_Adder_16bit_Signed</t>
+  </si>
+  <si>
+    <t>ITR1/07_SoftIP/02_Adder_Substractor/101_Adder_Sub_16bit_Unsign</t>
+  </si>
+  <si>
+    <t>ITR1/07_SoftIP/03_Barrel_Shifter/101_Barrel_Shifter_default</t>
+  </si>
+  <si>
+    <t>ITR1/07_SoftIP/04_Comparator/101_Comparator_8bit_Unsign_A_notequal_B</t>
+  </si>
+  <si>
+    <t>ITR1/07_SoftIP/400_Distributed_DPRAM/401_Dist_DPRAM_default</t>
+  </si>
+  <si>
+    <t>ITR1/07_SoftIP/410_Distributed_ROM/412_Dist_ROM_a2x4_bin</t>
+  </si>
+  <si>
+    <t>ITR1/07_SoftIP/420_Distributed_SPRAM/422_Dist_SPRAM_a2x4</t>
+  </si>
+  <si>
+    <t>ITR1/07_SoftIP/430_Mult_Add_Sub_Sum/431_Mult_Add_Sub_Sum_default</t>
+  </si>
+  <si>
+    <t>ITR1/07_SoftIP/440_Multiplier/441_Multiplier_default</t>
+  </si>
+  <si>
+    <t>ITR1/07_SoftIP/450_Sin_Cos_Table/452_Sincos_i3_o4_cos_lut_p2</t>
+  </si>
+  <si>
+    <t>ITR1/07_SoftIP/460_Subtractor/461_Subtractor_default</t>
+  </si>
+  <si>
+    <t>ITR1/07_SoftIP/301_FFT_Butterfly/301_FFT_2T_L_1_08_08_01_11</t>
+  </si>
+  <si>
+    <t>ITR1/07_SoftIP/302_Convert/301_Cvt_8_0_S_8_0_T_W</t>
+  </si>
+  <si>
+    <t>ITR1/07_SoftIP/303_Counter/302_Cnt_1_U_0_1_0</t>
+  </si>
+  <si>
+    <t>ITR1/07_SoftIP/304_LFSR/301_LFSR_F_XO_8_00_01_10</t>
+  </si>
+  <si>
+    <t>ITR1/07_SoftIP/305_Complex_Mult/301_CpM_8_8_U_11_1_L</t>
+  </si>
+  <si>
+    <t>ITR1/07_SoftIP/306_Mult_Accumulate/301_MA_A_18_18_37_SS_01_1_L</t>
+  </si>
+  <si>
+    <t>ITR1/07_SoftIP/307_Mult_Add_Sub/301_MAS_A_9_9_SS_11_1_L</t>
+  </si>
+  <si>
+    <t>ITR2/EIT2/DSP/101_MULT8_REG_REG_REG</t>
+  </si>
+  <si>
+    <t>ITR2/EIT2/DSP/201_MULT9A_REG_REG_REG</t>
+  </si>
+  <si>
+    <t>ITR2/EIT2/DSP/301_MULT18X18A_rega_regb_rego</t>
+  </si>
+  <si>
+    <t>ITR2/EIT2/DSP/400_MULTADDSUB18X18A_default</t>
+  </si>
+  <si>
+    <t>ITR2/EIT2/DSP/501_DOT9_INREG_REG1</t>
+  </si>
+  <si>
+    <t>ITR2/EIT2/DSP/601_DOT9A_INREG_REG1</t>
+  </si>
+  <si>
+    <t>ITR2/EIT2/EBR/105_SP16KA_1Kx18</t>
+  </si>
+  <si>
+    <t>ITR2/EIT2/EBR/201_SP32K_32Kx1</t>
+  </si>
+  <si>
+    <t>ITR2/EIT2/EBR/301_DP32K_1K_X36</t>
+  </si>
+  <si>
+    <t>ITR2/EIT2/EBR/401_pdp32k_1x32k</t>
+  </si>
+  <si>
+    <t>ITR2/EIT2/EBR/501_pdpsc32k_1x32k</t>
+  </si>
+  <si>
+    <t>ITR2/EIT2/EBR/602_FIFO32K_16KX2</t>
+  </si>
+  <si>
+    <t>Primitive MULT8              sim and flow check</t>
+  </si>
+  <si>
+    <t>Primitive MULT9A             sim and flow check</t>
+  </si>
+  <si>
+    <t>Primitive MULT18X18A         sim and flow check</t>
+  </si>
+  <si>
+    <t>Primitive MULTADDSUB18X18A   sim and flow check</t>
+  </si>
+  <si>
+    <t>Primitive DOT9               sim and flow check</t>
+  </si>
+  <si>
+    <t>Primitive DOT9A              sim and flow check</t>
+  </si>
+  <si>
+    <t>Primitive SP16KA             sim and flow check</t>
+  </si>
+  <si>
+    <t>Primitive SP32K              sim and flow check</t>
+  </si>
+  <si>
+    <t>Primitive DP32K              sim and flow check</t>
+  </si>
+  <si>
+    <t>Primitive pdp32k             sim and flow check</t>
+  </si>
+  <si>
+    <t>Primitive pdpsc32k           sim and flow check</t>
+  </si>
+  <si>
+    <t>Primitive FIFO32K            sim and flow check</t>
+  </si>
+  <si>
+    <t>sim;impl</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>silicon_07_apollo_v1.02</t>
+  </si>
+  <si>
+    <t>repository = http://lsh-tmp/radiant/trunk/silicon</t>
+  </si>
+  <si>
+    <t>suite_path = 07_Apollo</t>
   </si>
 </sst>
 </file>
@@ -2435,7 +2549,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="12" fillId="7" borderId="7" xfId="13" applyNumberFormat="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -2641,6 +2755,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="12" fillId="7" borderId="27" xfId="13" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2653,20 +2770,59 @@
     <xf numFmtId="49" fontId="12" fillId="7" borderId="7" xfId="13" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2674,12 +2830,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2689,13 +2839,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
@@ -2715,44 +2859,17 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="48" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -5594,8 +5711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -5610,7 +5727,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>360</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -5626,7 +5743,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>382</v>
+        <v>461</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -5634,12 +5751,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>372</v>
+        <v>462</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="B5" s="2" t="s">
-        <v>371</v>
+        <v>463</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -5647,7 +5764,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>422</v>
+        <v>367</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -5655,7 +5772,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>273</v>
+        <v>371</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -5663,7 +5780,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>381</v>
+        <v>345</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -5675,124 +5792,127 @@
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="B10" s="2" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>114</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>362</v>
+        <v>343</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>114</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>361</v>
+        <v>342</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>363</v>
+        <v>344</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>114</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>122</v>
@@ -5803,18 +5923,18 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>359</v>
+        <v>340</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>5</v>
@@ -5825,78 +5945,78 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>114</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>425</v>
+        <v>370</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>420</v>
+        <v>366</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>419</v>
+        <v>365</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>114</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>425</v>
+        <v>370</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>424</v>
+        <v>369</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>423</v>
+        <v>368</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -5907,23 +6027,23 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="G15" sqref="G15"/>
+    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" topLeftCell="A2">
+      <selection activeCell="C52" sqref="C52"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="B4" sqref="B4"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="B35" sqref="B35"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-    </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="B4" sqref="B4"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" topLeftCell="A2">
-      <selection activeCell="C52" sqref="C52"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
@@ -5936,14 +6056,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE54"/>
+  <dimension ref="A1:AE66"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B46" sqref="B46"/>
+      <selection pane="bottomRight" activeCell="D62" sqref="D62:D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -5976,41 +6096,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-      <c r="R1" s="70"/>
-      <c r="S1" s="70"/>
-      <c r="T1" s="70"/>
-      <c r="U1" s="70"/>
-      <c r="V1" s="70"/>
-      <c r="W1" s="71"/>
-      <c r="X1" s="72" t="s">
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
+      <c r="P1" s="71"/>
+      <c r="Q1" s="71"/>
+      <c r="R1" s="71"/>
+      <c r="S1" s="71"/>
+      <c r="T1" s="71"/>
+      <c r="U1" s="71"/>
+      <c r="V1" s="71"/>
+      <c r="W1" s="72"/>
+      <c r="X1" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="Y1" s="72"/>
-      <c r="Z1" s="72"/>
-      <c r="AA1" s="72"/>
-      <c r="AB1" s="72"/>
-      <c r="AC1" s="72"/>
-      <c r="AD1" s="72"/>
-      <c r="AE1" s="72"/>
+      <c r="Y1" s="73"/>
+      <c r="Z1" s="73"/>
+      <c r="AA1" s="73"/>
+      <c r="AB1" s="73"/>
+      <c r="AC1" s="73"/>
+      <c r="AD1" s="73"/>
+      <c r="AE1" s="73"/>
     </row>
     <row r="2" spans="1:31" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -6115,7 +6235,7 @@
         <v>298</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>316</v>
+        <v>372</v>
       </c>
       <c r="F3" s="2">
         <v>1</v>
@@ -6124,7 +6244,7 @@
         <v>305</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>303</v>
@@ -6144,7 +6264,7 @@
         <v>298</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>318</v>
+        <v>373</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
@@ -6153,7 +6273,7 @@
         <v>305</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>303</v>
@@ -6173,7 +6293,7 @@
         <v>298</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>320</v>
+        <v>374</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>40</v>
@@ -6182,7 +6302,7 @@
         <v>305</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="S5" s="2" t="s">
         <v>303</v>
@@ -6202,7 +6322,7 @@
         <v>298</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>321</v>
+        <v>375</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>40</v>
@@ -6211,7 +6331,7 @@
         <v>305</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="S6" s="2" t="s">
         <v>303</v>
@@ -6231,7 +6351,7 @@
         <v>298</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>322</v>
+        <v>376</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>40</v>
@@ -6240,7 +6360,7 @@
         <v>306</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="S7" s="2" t="s">
         <v>303</v>
@@ -6260,7 +6380,7 @@
         <v>298</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>324</v>
+        <v>377</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>40</v>
@@ -6269,7 +6389,7 @@
         <v>306</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="S8" s="2" t="s">
         <v>303</v>
@@ -6289,7 +6409,7 @@
         <v>298</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>40</v>
@@ -6298,7 +6418,7 @@
         <v>308</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="S9" s="2" t="s">
         <v>303</v>
@@ -6312,13 +6432,13 @@
     </row>
     <row r="10" spans="1:31">
       <c r="A10" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>298</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>40</v>
@@ -6327,7 +6447,7 @@
         <v>308</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="S10" s="2" t="s">
         <v>303</v>
@@ -6347,7 +6467,7 @@
         <v>298</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>40</v>
@@ -6356,7 +6476,7 @@
         <v>308</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="S11" s="2" t="s">
         <v>303</v>
@@ -6376,7 +6496,7 @@
         <v>298</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>40</v>
@@ -6385,7 +6505,7 @@
         <v>308</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="S12" s="2" t="s">
         <v>303</v>
@@ -6405,7 +6525,7 @@
         <v>298</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>40</v>
@@ -6414,7 +6534,7 @@
         <v>308</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="S13" s="2" t="s">
         <v>303</v>
@@ -6434,7 +6554,7 @@
         <v>298</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>378</v>
+        <v>383</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>40</v>
@@ -6443,7 +6563,7 @@
         <v>308</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="S14" s="2" t="s">
         <v>303</v>
@@ -6463,7 +6583,7 @@
         <v>298</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>40</v>
@@ -6472,7 +6592,7 @@
         <v>308</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="S15" s="2" t="s">
         <v>303</v>
@@ -6492,7 +6612,7 @@
         <v>298</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>380</v>
+        <v>385</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>40</v>
@@ -6501,7 +6621,7 @@
         <v>308</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="S16" s="2" t="s">
         <v>303</v>
@@ -6521,7 +6641,7 @@
         <v>298</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>330</v>
+        <v>386</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>40</v>
@@ -6530,7 +6650,7 @@
         <v>307</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="S17" s="2" t="s">
         <v>303</v>
@@ -6550,7 +6670,7 @@
         <v>298</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>332</v>
+        <v>387</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>40</v>
@@ -6559,7 +6679,7 @@
         <v>307</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="S18" s="2" t="s">
         <v>303</v>
@@ -6579,7 +6699,7 @@
         <v>298</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>333</v>
+        <v>388</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>40</v>
@@ -6588,7 +6708,7 @@
         <v>307</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="S19" s="2" t="s">
         <v>303</v>
@@ -6608,7 +6728,7 @@
         <v>298</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>334</v>
+        <v>389</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>40</v>
@@ -6617,7 +6737,7 @@
         <v>307</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="S20" s="2" t="s">
         <v>303</v>
@@ -6637,7 +6757,7 @@
         <v>298</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>335</v>
+        <v>390</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>40</v>
@@ -6646,7 +6766,7 @@
         <v>307</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
       <c r="S21" s="2" t="s">
         <v>303</v>
@@ -6666,7 +6786,7 @@
         <v>298</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>337</v>
+        <v>391</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>40</v>
@@ -6675,7 +6795,7 @@
         <v>307</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="S22" s="2" t="s">
         <v>303</v>
@@ -6695,7 +6815,7 @@
         <v>298</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>339</v>
+        <v>392</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>40</v>
@@ -6704,7 +6824,7 @@
         <v>307</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
       <c r="S23" s="2" t="s">
         <v>303</v>
@@ -6724,7 +6844,7 @@
         <v>298</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>341</v>
+        <v>393</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>40</v>
@@ -6733,7 +6853,7 @@
         <v>307</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
       <c r="S24" s="2" t="s">
         <v>303</v>
@@ -6750,25 +6870,25 @@
         <v>291</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>344</v>
+        <v>394</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>345</v>
+        <v>330</v>
       </c>
       <c r="S25" s="2" t="s">
         <v>303</v>
       </c>
       <c r="T25" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AE25" s="2" t="s">
         <v>309</v>
@@ -6779,22 +6899,22 @@
         <v>292</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>351</v>
+        <v>332</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>364</v>
+        <v>395</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>352</v>
+        <v>333</v>
       </c>
       <c r="S26" s="2" t="s">
         <v>303</v>
       </c>
       <c r="T26" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AE26" s="2" t="s">
         <v>309</v>
@@ -6805,22 +6925,22 @@
         <v>293</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>351</v>
+        <v>332</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>365</v>
+        <v>396</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>353</v>
+        <v>334</v>
       </c>
       <c r="S27" s="2" t="s">
         <v>303</v>
       </c>
       <c r="T27" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AE27" s="2" t="s">
         <v>309</v>
@@ -6831,22 +6951,22 @@
         <v>294</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>351</v>
+        <v>332</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>366</v>
+        <v>397</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>354</v>
+        <v>335</v>
       </c>
       <c r="S28" s="2" t="s">
         <v>303</v>
       </c>
       <c r="T28" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AE28" s="2" t="s">
         <v>309</v>
@@ -6857,22 +6977,22 @@
         <v>295</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>351</v>
+        <v>332</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>367</v>
+        <v>398</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>355</v>
+        <v>336</v>
       </c>
       <c r="S29" s="2" t="s">
         <v>303</v>
       </c>
       <c r="T29" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AE29" s="2" t="s">
         <v>309</v>
@@ -6883,22 +7003,22 @@
         <v>296</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>351</v>
+        <v>332</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>368</v>
+        <v>399</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>356</v>
+        <v>337</v>
       </c>
       <c r="S30" s="2" t="s">
         <v>303</v>
       </c>
       <c r="T30" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AE30" s="2" t="s">
         <v>309</v>
@@ -6909,22 +7029,22 @@
         <v>297</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>351</v>
+        <v>332</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>369</v>
+        <v>400</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="S31" s="2" t="s">
         <v>303</v>
       </c>
       <c r="T31" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AE31" s="2" t="s">
         <v>309</v>
@@ -6935,22 +7055,22 @@
         <v>311</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>351</v>
+        <v>332</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>370</v>
+        <v>401</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="S32" s="2" t="s">
         <v>303</v>
       </c>
       <c r="T32" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AE32" s="2" t="s">
         <v>309</v>
@@ -6961,10 +7081,10 @@
         <v>312</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>347</v>
+        <v>402</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>40</v>
@@ -6984,10 +7104,10 @@
         <v>313</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>348</v>
+        <v>403</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>40</v>
@@ -7007,10 +7127,10 @@
         <v>314</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>349</v>
+        <v>404</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>40</v>
@@ -7030,10 +7150,10 @@
         <v>315</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>350</v>
+        <v>405</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>40</v>
@@ -7050,22 +7170,22 @@
     </row>
     <row r="37" spans="1:31">
       <c r="A37" s="2" t="s">
-        <v>401</v>
+        <v>347</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>383</v>
+        <v>406</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>40</v>
       </c>
       <c r="S37" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="T37" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AE37" s="2" t="s">
         <v>309</v>
@@ -7073,22 +7193,22 @@
     </row>
     <row r="38" spans="1:31">
       <c r="A38" s="2" t="s">
-        <v>402</v>
+        <v>348</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>384</v>
+        <v>407</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>40</v>
       </c>
       <c r="S38" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="T38" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AE38" s="2" t="s">
         <v>309</v>
@@ -7096,22 +7216,22 @@
     </row>
     <row r="39" spans="1:31">
       <c r="A39" s="2" t="s">
-        <v>403</v>
+        <v>349</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>385</v>
+        <v>408</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>40</v>
       </c>
       <c r="S39" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="T39" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AE39" s="2" t="s">
         <v>309</v>
@@ -7119,22 +7239,22 @@
     </row>
     <row r="40" spans="1:31">
       <c r="A40" s="2" t="s">
-        <v>404</v>
+        <v>350</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>386</v>
+        <v>409</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>40</v>
       </c>
       <c r="S40" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="T40" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AE40" s="2" t="s">
         <v>309</v>
@@ -7142,22 +7262,22 @@
     </row>
     <row r="41" spans="1:31">
       <c r="A41" s="2" t="s">
-        <v>405</v>
+        <v>351</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>387</v>
+        <v>410</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>40</v>
       </c>
       <c r="S41" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="T41" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AE41" s="2" t="s">
         <v>309</v>
@@ -7165,22 +7285,22 @@
     </row>
     <row r="42" spans="1:31">
       <c r="A42" s="2" t="s">
-        <v>406</v>
+        <v>352</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>388</v>
+        <v>411</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>40</v>
       </c>
       <c r="S42" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="T42" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AE42" s="2" t="s">
         <v>309</v>
@@ -7188,22 +7308,22 @@
     </row>
     <row r="43" spans="1:31">
       <c r="A43" s="2" t="s">
-        <v>407</v>
+        <v>353</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>389</v>
+        <v>412</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>40</v>
       </c>
       <c r="S43" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="T43" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AE43" s="2" t="s">
         <v>309</v>
@@ -7211,22 +7331,22 @@
     </row>
     <row r="44" spans="1:31">
       <c r="A44" s="2" t="s">
-        <v>408</v>
+        <v>354</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>390</v>
+        <v>413</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>40</v>
       </c>
       <c r="S44" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="T44" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AE44" s="2" t="s">
         <v>309</v>
@@ -7234,22 +7354,22 @@
     </row>
     <row r="45" spans="1:31">
       <c r="A45" s="2" t="s">
-        <v>409</v>
+        <v>355</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>391</v>
+        <v>414</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>40</v>
       </c>
       <c r="S45" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="T45" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AE45" s="2" t="s">
         <v>309</v>
@@ -7257,22 +7377,22 @@
     </row>
     <row r="46" spans="1:31">
       <c r="A46" s="2" t="s">
-        <v>410</v>
+        <v>356</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>392</v>
+        <v>415</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>40</v>
       </c>
       <c r="S46" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="T46" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AE46" s="2" t="s">
         <v>309</v>
@@ -7280,22 +7400,22 @@
     </row>
     <row r="47" spans="1:31">
       <c r="A47" s="2" t="s">
-        <v>411</v>
+        <v>357</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>393</v>
+        <v>416</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>40</v>
       </c>
       <c r="S47" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="T47" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AE47" s="2" t="s">
         <v>309</v>
@@ -7303,22 +7423,22 @@
     </row>
     <row r="48" spans="1:31">
       <c r="A48" s="2" t="s">
-        <v>412</v>
+        <v>358</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>394</v>
+        <v>417</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>40</v>
       </c>
       <c r="S48" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="T48" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AE48" s="2" t="s">
         <v>309</v>
@@ -7326,22 +7446,22 @@
     </row>
     <row r="49" spans="1:31">
       <c r="A49" s="2" t="s">
-        <v>413</v>
+        <v>359</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>395</v>
+        <v>418</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>40</v>
       </c>
       <c r="S49" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="T49" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AE49" s="2" t="s">
         <v>309</v>
@@ -7349,22 +7469,22 @@
     </row>
     <row r="50" spans="1:31">
       <c r="A50" s="2" t="s">
-        <v>414</v>
+        <v>360</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>40</v>
       </c>
       <c r="S50" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="T50" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AE50" s="2" t="s">
         <v>309</v>
@@ -7372,22 +7492,22 @@
     </row>
     <row r="51" spans="1:31">
       <c r="A51" s="2" t="s">
-        <v>415</v>
+        <v>361</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>396</v>
+        <v>420</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>40</v>
       </c>
       <c r="S51" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="T51" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AE51" s="2" t="s">
         <v>309</v>
@@ -7395,22 +7515,22 @@
     </row>
     <row r="52" spans="1:31">
       <c r="A52" s="2" t="s">
-        <v>416</v>
+        <v>362</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>397</v>
+        <v>421</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>40</v>
       </c>
       <c r="S52" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="T52" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AE52" s="2" t="s">
         <v>309</v>
@@ -7418,22 +7538,22 @@
     </row>
     <row r="53" spans="1:31">
       <c r="A53" s="2" t="s">
-        <v>417</v>
+        <v>363</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>398</v>
+        <v>422</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>40</v>
       </c>
       <c r="S53" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="T53" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AE53" s="2" t="s">
         <v>309</v>
@@ -7441,25 +7561,301 @@
     </row>
     <row r="54" spans="1:31">
       <c r="A54" s="2" t="s">
-        <v>418</v>
+        <v>364</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>399</v>
+        <v>423</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>40</v>
       </c>
       <c r="S54" s="2" t="s">
-        <v>400</v>
+        <v>346</v>
       </c>
       <c r="T54" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AE54" s="2" t="s">
         <v>309</v>
+      </c>
+    </row>
+    <row r="55" spans="1:31">
+      <c r="A55" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="H55" s="69" t="s">
+        <v>436</v>
+      </c>
+      <c r="S55" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T55" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="AE55" s="69" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="56" spans="1:31">
+      <c r="A56" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="H56" s="69" t="s">
+        <v>437</v>
+      </c>
+      <c r="S56" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T56" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="AE56" s="69" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="57" spans="1:31">
+      <c r="A57" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="H57" s="69" t="s">
+        <v>438</v>
+      </c>
+      <c r="S57" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T57" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="AE57" s="69" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="58" spans="1:31">
+      <c r="A58" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="H58" s="69" t="s">
+        <v>439</v>
+      </c>
+      <c r="S58" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T58" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="AE58" s="69" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="59" spans="1:31">
+      <c r="A59" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="H59" s="69" t="s">
+        <v>440</v>
+      </c>
+      <c r="S59" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T59" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="AE59" s="69" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="60" spans="1:31">
+      <c r="A60" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="H60" s="69" t="s">
+        <v>441</v>
+      </c>
+      <c r="S60" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T60" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="AE60" s="69" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="61" spans="1:31">
+      <c r="A61" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="H61" s="69" t="s">
+        <v>442</v>
+      </c>
+      <c r="S61" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T61" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="AE61" s="69" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="62" spans="1:31">
+      <c r="A62" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="H62" s="69" t="s">
+        <v>443</v>
+      </c>
+      <c r="S62" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T62" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="AE62" s="69" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="63" spans="1:31">
+      <c r="A63" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="H63" s="69" t="s">
+        <v>444</v>
+      </c>
+      <c r="S63" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T63" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="AE63" s="69" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="64" spans="1:31">
+      <c r="A64" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H64" s="69" t="s">
+        <v>445</v>
+      </c>
+      <c r="S64" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T64" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="AE64" s="69" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="65" spans="1:31">
+      <c r="A65" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="H65" s="69" t="s">
+        <v>446</v>
+      </c>
+      <c r="S65" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T65" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="AE65" s="69" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="66" spans="1:31">
+      <c r="A66" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="H66" s="69" t="s">
+        <v>447</v>
+      </c>
+      <c r="S66" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T66" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="AE66" s="69" t="s">
+        <v>448</v>
       </c>
     </row>
   </sheetData>
@@ -7599,17 +7995,17 @@
       <c r="E111" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F111" s="75" t="s">
+      <c r="F111" s="107" t="s">
         <v>87</v>
       </c>
-      <c r="G111" s="76"/>
-      <c r="H111" s="76"/>
-      <c r="I111" s="76"/>
-      <c r="J111" s="76"/>
-      <c r="K111" s="76"/>
-      <c r="L111" s="76"/>
-      <c r="M111" s="76"/>
-      <c r="N111" s="77"/>
+      <c r="G111" s="108"/>
+      <c r="H111" s="108"/>
+      <c r="I111" s="108"/>
+      <c r="J111" s="108"/>
+      <c r="K111" s="108"/>
+      <c r="L111" s="108"/>
+      <c r="M111" s="108"/>
+      <c r="N111" s="109"/>
     </row>
     <row r="112" spans="1:14">
       <c r="A112" s="11" t="s">
@@ -8499,7 +8895,7 @@
       <c r="A148" s="26">
         <v>1</v>
       </c>
-      <c r="B148" s="78" t="s">
+      <c r="B148" s="92" t="s">
         <v>3</v>
       </c>
       <c r="C148" s="27" t="s">
@@ -8525,7 +8921,7 @@
       <c r="A149" s="26">
         <v>2</v>
       </c>
-      <c r="B149" s="79"/>
+      <c r="B149" s="93"/>
       <c r="C149" s="28" t="s">
         <v>136</v>
       </c>
@@ -8547,7 +8943,7 @@
       <c r="A150" s="26">
         <v>3</v>
       </c>
-      <c r="B150" s="79"/>
+      <c r="B150" s="93"/>
       <c r="C150" s="28" t="s">
         <v>9</v>
       </c>
@@ -8567,7 +8963,7 @@
       <c r="A151" s="26">
         <v>4</v>
       </c>
-      <c r="B151" s="79"/>
+      <c r="B151" s="93"/>
       <c r="C151" s="28" t="s">
         <v>138</v>
       </c>
@@ -8591,7 +8987,7 @@
       <c r="A152" s="26">
         <v>5</v>
       </c>
-      <c r="B152" s="79"/>
+      <c r="B152" s="93"/>
       <c r="C152" s="27" t="s">
         <v>140</v>
       </c>
@@ -8615,7 +9011,7 @@
       <c r="A153" s="26">
         <v>6</v>
       </c>
-      <c r="B153" s="79"/>
+      <c r="B153" s="93"/>
       <c r="C153" s="27" t="s">
         <v>144</v>
       </c>
@@ -8639,7 +9035,7 @@
       <c r="A154" s="26">
         <v>7</v>
       </c>
-      <c r="B154" s="79"/>
+      <c r="B154" s="93"/>
       <c r="C154" s="28" t="s">
         <v>147</v>
       </c>
@@ -8661,7 +9057,7 @@
       <c r="A155" s="26">
         <v>8</v>
       </c>
-      <c r="B155" s="79"/>
+      <c r="B155" s="93"/>
       <c r="C155" s="27" t="s">
         <v>148</v>
       </c>
@@ -8685,7 +9081,7 @@
       <c r="A156" s="26">
         <v>9</v>
       </c>
-      <c r="B156" s="79"/>
+      <c r="B156" s="93"/>
       <c r="C156" s="27" t="s">
         <v>149</v>
       </c>
@@ -8709,7 +9105,7 @@
       <c r="A157" s="26">
         <v>10</v>
       </c>
-      <c r="B157" s="79"/>
+      <c r="B157" s="93"/>
       <c r="C157" s="28" t="s">
         <v>150</v>
       </c>
@@ -8733,7 +9129,7 @@
       <c r="A158" s="26">
         <v>11</v>
       </c>
-      <c r="B158" s="79"/>
+      <c r="B158" s="93"/>
       <c r="C158" s="68" t="s">
         <v>151</v>
       </c>
@@ -8757,7 +9153,7 @@
       <c r="A159" s="26">
         <v>12</v>
       </c>
-      <c r="B159" s="79"/>
+      <c r="B159" s="93"/>
       <c r="C159" s="28" t="s">
         <v>153</v>
       </c>
@@ -8779,7 +9175,7 @@
       <c r="A160" s="26">
         <v>13</v>
       </c>
-      <c r="B160" s="80"/>
+      <c r="B160" s="87"/>
       <c r="C160" s="28" t="s">
         <v>56</v>
       </c>
@@ -8803,7 +9199,7 @@
       <c r="A161" s="26">
         <v>14</v>
       </c>
-      <c r="B161" s="73" t="s">
+      <c r="B161" s="83" t="s">
         <v>4</v>
       </c>
       <c r="C161" s="28" t="s">
@@ -8829,7 +9225,7 @@
       <c r="A162" s="26">
         <v>15</v>
       </c>
-      <c r="B162" s="74"/>
+      <c r="B162" s="82"/>
       <c r="C162" s="28" t="s">
         <v>161</v>
       </c>
@@ -8853,7 +9249,7 @@
       <c r="A163" s="26">
         <v>16</v>
       </c>
-      <c r="B163" s="78" t="s">
+      <c r="B163" s="92" t="s">
         <v>5</v>
       </c>
       <c r="C163" s="28" t="s">
@@ -8877,7 +9273,7 @@
       <c r="A164" s="26">
         <v>17</v>
       </c>
-      <c r="B164" s="81"/>
+      <c r="B164" s="110"/>
       <c r="C164" s="27" t="s">
         <v>165</v>
       </c>
@@ -8899,7 +9295,7 @@
       <c r="A165" s="26">
         <v>18</v>
       </c>
-      <c r="B165" s="80"/>
+      <c r="B165" s="87"/>
       <c r="C165" s="27" t="s">
         <v>167</v>
       </c>
@@ -8919,7 +9315,7 @@
       <c r="A166" s="26">
         <v>19</v>
       </c>
-      <c r="B166" s="73" t="s">
+      <c r="B166" s="83" t="s">
         <v>6</v>
       </c>
       <c r="C166" s="28" t="s">
@@ -8943,7 +9339,7 @@
       <c r="A167" s="26">
         <v>20</v>
       </c>
-      <c r="B167" s="74"/>
+      <c r="B167" s="82"/>
       <c r="C167" s="28" t="s">
         <v>172</v>
       </c>
@@ -8963,7 +9359,7 @@
       <c r="A168" s="26">
         <v>21</v>
       </c>
-      <c r="B168" s="74"/>
+      <c r="B168" s="82"/>
       <c r="C168" s="28" t="s">
         <v>173</v>
       </c>
@@ -8983,7 +9379,7 @@
       <c r="A169" s="26">
         <v>22</v>
       </c>
-      <c r="B169" s="74"/>
+      <c r="B169" s="82"/>
       <c r="C169" s="28" t="s">
         <v>174</v>
       </c>
@@ -9003,7 +9399,7 @@
       <c r="A170" s="26">
         <v>23</v>
       </c>
-      <c r="B170" s="74"/>
+      <c r="B170" s="82"/>
       <c r="C170" s="28" t="s">
         <v>175</v>
       </c>
@@ -9023,7 +9419,7 @@
       <c r="A171" s="26">
         <v>24</v>
       </c>
-      <c r="B171" s="74"/>
+      <c r="B171" s="82"/>
       <c r="C171" s="28" t="s">
         <v>176</v>
       </c>
@@ -9043,7 +9439,7 @@
       <c r="A172" s="26">
         <v>25</v>
       </c>
-      <c r="B172" s="74"/>
+      <c r="B172" s="82"/>
       <c r="C172" s="28" t="s">
         <v>177</v>
       </c>
@@ -9063,7 +9459,7 @@
       <c r="A173" s="26">
         <v>26</v>
       </c>
-      <c r="B173" s="74"/>
+      <c r="B173" s="82"/>
       <c r="C173" s="28" t="s">
         <v>41</v>
       </c>
@@ -9083,7 +9479,7 @@
       <c r="A174" s="26">
         <v>27</v>
       </c>
-      <c r="B174" s="73" t="s">
+      <c r="B174" s="83" t="s">
         <v>7</v>
       </c>
       <c r="C174" s="28" t="s">
@@ -9107,7 +9503,7 @@
       <c r="A175" s="26">
         <v>28</v>
       </c>
-      <c r="B175" s="74"/>
+      <c r="B175" s="82"/>
       <c r="C175" s="27" t="s">
         <v>181</v>
       </c>
@@ -9129,7 +9525,7 @@
       <c r="A176" s="26">
         <v>29</v>
       </c>
-      <c r="B176" s="74"/>
+      <c r="B176" s="82"/>
       <c r="C176" s="28" t="s">
         <v>184</v>
       </c>
@@ -9151,7 +9547,7 @@
       <c r="A177" s="26">
         <v>30</v>
       </c>
-      <c r="B177" s="78" t="s">
+      <c r="B177" s="92" t="s">
         <v>8</v>
       </c>
       <c r="C177" s="28" t="s">
@@ -9177,7 +9573,7 @@
       <c r="A178" s="31">
         <v>31</v>
       </c>
-      <c r="B178" s="79"/>
+      <c r="B178" s="93"/>
       <c r="C178" s="32" t="s">
         <v>189</v>
       </c>
@@ -9201,7 +9597,7 @@
       <c r="A179" s="23">
         <v>32</v>
       </c>
-      <c r="B179" s="82" t="s">
+      <c r="B179" s="94" t="s">
         <v>191</v>
       </c>
       <c r="C179" s="33" t="s">
@@ -9225,7 +9621,7 @@
       <c r="A180" s="26">
         <v>33</v>
       </c>
-      <c r="B180" s="83"/>
+      <c r="B180" s="95"/>
       <c r="C180" s="27" t="s">
         <v>195</v>
       </c>
@@ -9247,7 +9643,7 @@
       <c r="A181" s="26">
         <v>34</v>
       </c>
-      <c r="B181" s="84"/>
+      <c r="B181" s="96"/>
       <c r="C181" s="34" t="s">
         <v>198</v>
       </c>
@@ -9269,7 +9665,7 @@
       <c r="A182" s="31">
         <v>35</v>
       </c>
-      <c r="B182" s="84"/>
+      <c r="B182" s="96"/>
       <c r="C182" s="34" t="s">
         <v>199</v>
       </c>
@@ -9291,7 +9687,7 @@
       <c r="A183" s="31">
         <v>36</v>
       </c>
-      <c r="B183" s="84"/>
+      <c r="B183" s="96"/>
       <c r="C183" s="34" t="s">
         <v>202</v>
       </c>
@@ -9311,7 +9707,7 @@
       <c r="A184" s="31">
         <v>37</v>
       </c>
-      <c r="B184" s="84"/>
+      <c r="B184" s="96"/>
       <c r="C184" s="34" t="s">
         <v>254</v>
       </c>
@@ -9333,7 +9729,7 @@
       <c r="A185" s="35">
         <v>38</v>
       </c>
-      <c r="B185" s="85"/>
+      <c r="B185" s="91"/>
       <c r="C185" s="36" t="s">
         <v>258</v>
       </c>
@@ -9384,11 +9780,11 @@
       <c r="B199" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="C199" s="86" t="s">
+      <c r="C199" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="D199" s="86"/>
-      <c r="E199" s="86"/>
+      <c r="D199" s="97"/>
+      <c r="E199" s="97"/>
       <c r="F199" s="39" t="s">
         <v>43</v>
       </c>
@@ -9397,17 +9793,17 @@
       </c>
     </row>
     <row r="200" spans="1:7">
-      <c r="A200" s="87" t="s">
+      <c r="A200" s="80" t="s">
         <v>212</v>
       </c>
-      <c r="B200" s="74" t="s">
+      <c r="B200" s="82" t="s">
         <v>213</v>
       </c>
-      <c r="C200" s="89" t="s">
+      <c r="C200" s="99" t="s">
         <v>57</v>
       </c>
-      <c r="D200" s="90"/>
-      <c r="E200" s="90"/>
+      <c r="D200" s="100"/>
+      <c r="E200" s="100"/>
       <c r="F200" s="28" t="s">
         <v>214</v>
       </c>
@@ -9416,13 +9812,13 @@
       </c>
     </row>
     <row r="201" spans="1:7">
-      <c r="A201" s="87"/>
-      <c r="B201" s="88"/>
-      <c r="C201" s="91" t="s">
+      <c r="A201" s="80"/>
+      <c r="B201" s="98"/>
+      <c r="C201" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="D201" s="92"/>
-      <c r="E201" s="92"/>
+      <c r="D201" s="102"/>
+      <c r="E201" s="102"/>
       <c r="F201" s="32" t="s">
         <v>215</v>
       </c>
@@ -9431,15 +9827,15 @@
       </c>
     </row>
     <row r="202" spans="1:7">
-      <c r="A202" s="87"/>
-      <c r="B202" s="74" t="s">
+      <c r="A202" s="80"/>
+      <c r="B202" s="82" t="s">
         <v>216</v>
       </c>
-      <c r="C202" s="93" t="s">
+      <c r="C202" s="103" t="s">
         <v>217</v>
       </c>
-      <c r="D202" s="93"/>
-      <c r="E202" s="93"/>
+      <c r="D202" s="103"/>
+      <c r="E202" s="103"/>
       <c r="F202" s="28" t="s">
         <v>214</v>
       </c>
@@ -9448,13 +9844,13 @@
       </c>
     </row>
     <row r="203" spans="1:7">
-      <c r="A203" s="87"/>
-      <c r="B203" s="74"/>
-      <c r="C203" s="91" t="s">
+      <c r="A203" s="80"/>
+      <c r="B203" s="82"/>
+      <c r="C203" s="101" t="s">
         <v>217</v>
       </c>
-      <c r="D203" s="91"/>
-      <c r="E203" s="91"/>
+      <c r="D203" s="101"/>
+      <c r="E203" s="101"/>
       <c r="F203" s="28" t="s">
         <v>215</v>
       </c>
@@ -9463,15 +9859,15 @@
       </c>
     </row>
     <row r="204" spans="1:7">
-      <c r="A204" s="87"/>
-      <c r="B204" s="88" t="s">
+      <c r="A204" s="80"/>
+      <c r="B204" s="98" t="s">
         <v>218</v>
       </c>
-      <c r="C204" s="94" t="s">
+      <c r="C204" s="104" t="s">
         <v>57</v>
       </c>
-      <c r="D204" s="95"/>
-      <c r="E204" s="96"/>
+      <c r="D204" s="105"/>
+      <c r="E204" s="106"/>
       <c r="F204" s="28" t="s">
         <v>214</v>
       </c>
@@ -9480,13 +9876,13 @@
       </c>
     </row>
     <row r="205" spans="1:7">
-      <c r="A205" s="87"/>
-      <c r="B205" s="80"/>
-      <c r="C205" s="94" t="s">
+      <c r="A205" s="80"/>
+      <c r="B205" s="87"/>
+      <c r="C205" s="104" t="s">
         <v>57</v>
       </c>
-      <c r="D205" s="95"/>
-      <c r="E205" s="96"/>
+      <c r="D205" s="105"/>
+      <c r="E205" s="106"/>
       <c r="F205" s="28" t="s">
         <v>215</v>
       </c>
@@ -9495,15 +9891,15 @@
       </c>
     </row>
     <row r="206" spans="1:7">
-      <c r="A206" s="87"/>
-      <c r="B206" s="74" t="s">
+      <c r="A206" s="80"/>
+      <c r="B206" s="82" t="s">
         <v>219</v>
       </c>
-      <c r="C206" s="93" t="s">
+      <c r="C206" s="103" t="s">
         <v>220</v>
       </c>
-      <c r="D206" s="93"/>
-      <c r="E206" s="93"/>
+      <c r="D206" s="103"/>
+      <c r="E206" s="103"/>
       <c r="F206" s="28" t="s">
         <v>214</v>
       </c>
@@ -9512,13 +9908,13 @@
       </c>
     </row>
     <row r="207" spans="1:7">
-      <c r="A207" s="87"/>
-      <c r="B207" s="74"/>
-      <c r="C207" s="93" t="s">
+      <c r="A207" s="80"/>
+      <c r="B207" s="82"/>
+      <c r="C207" s="103" t="s">
         <v>220</v>
       </c>
-      <c r="D207" s="93"/>
-      <c r="E207" s="93"/>
+      <c r="D207" s="103"/>
+      <c r="E207" s="103"/>
       <c r="F207" s="28" t="s">
         <v>215</v>
       </c>
@@ -9527,17 +9923,17 @@
       </c>
     </row>
     <row r="208" spans="1:7">
-      <c r="A208" s="87" t="s">
+      <c r="A208" s="80" t="s">
         <v>221</v>
       </c>
-      <c r="B208" s="74" t="s">
+      <c r="B208" s="82" t="s">
         <v>222</v>
       </c>
-      <c r="C208" s="73" t="s">
+      <c r="C208" s="83" t="s">
         <v>45</v>
       </c>
-      <c r="D208" s="74"/>
-      <c r="E208" s="74"/>
+      <c r="D208" s="82"/>
+      <c r="E208" s="82"/>
       <c r="F208" s="28" t="s">
         <v>214</v>
       </c>
@@ -9546,13 +9942,13 @@
       </c>
     </row>
     <row r="209" spans="1:7">
-      <c r="A209" s="87"/>
-      <c r="B209" s="74"/>
-      <c r="C209" s="74" t="s">
+      <c r="A209" s="80"/>
+      <c r="B209" s="82"/>
+      <c r="C209" s="82" t="s">
         <v>46</v>
       </c>
-      <c r="D209" s="74"/>
-      <c r="E209" s="74"/>
+      <c r="D209" s="82"/>
+      <c r="E209" s="82"/>
       <c r="F209" s="28" t="s">
         <v>215</v>
       </c>
@@ -9561,15 +9957,15 @@
       </c>
     </row>
     <row r="210" spans="1:7">
-      <c r="A210" s="87"/>
-      <c r="B210" s="74" t="s">
+      <c r="A210" s="80"/>
+      <c r="B210" s="82" t="s">
         <v>224</v>
       </c>
-      <c r="C210" s="73" t="s">
+      <c r="C210" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="D210" s="74"/>
-      <c r="E210" s="74"/>
+      <c r="D210" s="82"/>
+      <c r="E210" s="82"/>
       <c r="F210" s="28" t="s">
         <v>214</v>
       </c>
@@ -9578,13 +9974,13 @@
       </c>
     </row>
     <row r="211" spans="1:7">
-      <c r="A211" s="87"/>
-      <c r="B211" s="74"/>
-      <c r="C211" s="74" t="s">
+      <c r="A211" s="80"/>
+      <c r="B211" s="82"/>
+      <c r="C211" s="82" t="s">
         <v>48</v>
       </c>
-      <c r="D211" s="74"/>
-      <c r="E211" s="74"/>
+      <c r="D211" s="82"/>
+      <c r="E211" s="82"/>
       <c r="F211" s="28" t="s">
         <v>215</v>
       </c>
@@ -9593,17 +9989,17 @@
       </c>
     </row>
     <row r="212" spans="1:7">
-      <c r="A212" s="87" t="s">
+      <c r="A212" s="80" t="s">
         <v>225</v>
       </c>
-      <c r="B212" s="74" t="s">
+      <c r="B212" s="82" t="s">
         <v>226</v>
       </c>
-      <c r="C212" s="73" t="s">
+      <c r="C212" s="83" t="s">
         <v>49</v>
       </c>
-      <c r="D212" s="74"/>
-      <c r="E212" s="74"/>
+      <c r="D212" s="82"/>
+      <c r="E212" s="82"/>
       <c r="F212" s="28" t="s">
         <v>214</v>
       </c>
@@ -9612,13 +10008,13 @@
       </c>
     </row>
     <row r="213" spans="1:7">
-      <c r="A213" s="87"/>
-      <c r="B213" s="74"/>
-      <c r="C213" s="74" t="s">
+      <c r="A213" s="80"/>
+      <c r="B213" s="82"/>
+      <c r="C213" s="82" t="s">
         <v>50</v>
       </c>
-      <c r="D213" s="74"/>
-      <c r="E213" s="74"/>
+      <c r="D213" s="82"/>
+      <c r="E213" s="82"/>
       <c r="F213" s="28" t="s">
         <v>215</v>
       </c>
@@ -9627,15 +10023,15 @@
       </c>
     </row>
     <row r="214" spans="1:7">
-      <c r="A214" s="87"/>
-      <c r="B214" s="74" t="s">
+      <c r="A214" s="80"/>
+      <c r="B214" s="82" t="s">
         <v>227</v>
       </c>
-      <c r="C214" s="73" t="s">
+      <c r="C214" s="83" t="s">
         <v>228</v>
       </c>
-      <c r="D214" s="74"/>
-      <c r="E214" s="74"/>
+      <c r="D214" s="82"/>
+      <c r="E214" s="82"/>
       <c r="F214" s="28" t="s">
         <v>214</v>
       </c>
@@ -9644,13 +10040,13 @@
       </c>
     </row>
     <row r="215" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A215" s="98"/>
-      <c r="B215" s="99"/>
-      <c r="C215" s="99" t="s">
+      <c r="A215" s="81"/>
+      <c r="B215" s="84"/>
+      <c r="C215" s="84" t="s">
         <v>229</v>
       </c>
-      <c r="D215" s="99"/>
-      <c r="E215" s="99"/>
+      <c r="D215" s="84"/>
+      <c r="E215" s="84"/>
       <c r="F215" s="36" t="s">
         <v>215</v>
       </c>
@@ -9689,12 +10085,12 @@
       <c r="A220" s="45" t="s">
         <v>232</v>
       </c>
-      <c r="B220" s="100" t="s">
+      <c r="B220" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="C220" s="100"/>
-      <c r="D220" s="100"/>
-      <c r="E220" s="100"/>
+      <c r="C220" s="85"/>
+      <c r="D220" s="85"/>
+      <c r="E220" s="85"/>
       <c r="F220" s="46" t="s">
         <v>233</v>
       </c>
@@ -9706,12 +10102,12 @@
       <c r="A221" s="48" t="s">
         <v>235</v>
       </c>
-      <c r="B221" s="101" t="s">
+      <c r="B221" s="86" t="s">
         <v>236</v>
       </c>
-      <c r="C221" s="80"/>
-      <c r="D221" s="80"/>
-      <c r="E221" s="80"/>
+      <c r="C221" s="87"/>
+      <c r="D221" s="87"/>
+      <c r="E221" s="87"/>
       <c r="F221" s="49" t="s">
         <v>111</v>
       </c>
@@ -9723,12 +10119,12 @@
       <c r="A222" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="B222" s="102" t="s">
+      <c r="B222" s="88" t="s">
         <v>238</v>
       </c>
-      <c r="C222" s="103"/>
-      <c r="D222" s="103"/>
-      <c r="E222" s="104"/>
+      <c r="C222" s="89"/>
+      <c r="D222" s="89"/>
+      <c r="E222" s="90"/>
       <c r="F222" s="15" t="s">
         <v>63</v>
       </c>
@@ -9740,12 +10136,12 @@
       <c r="A223" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B223" s="102" t="s">
+      <c r="B223" s="88" t="s">
         <v>239</v>
       </c>
-      <c r="C223" s="103"/>
-      <c r="D223" s="103"/>
-      <c r="E223" s="104"/>
+      <c r="C223" s="89"/>
+      <c r="D223" s="89"/>
+      <c r="E223" s="90"/>
       <c r="F223" s="18" t="s">
         <v>63</v>
       </c>
@@ -9757,12 +10153,12 @@
       <c r="A224" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="B224" s="85" t="s">
+      <c r="B224" s="91" t="s">
         <v>241</v>
       </c>
-      <c r="C224" s="99"/>
-      <c r="D224" s="99"/>
-      <c r="E224" s="99"/>
+      <c r="C224" s="84"/>
+      <c r="D224" s="84"/>
+      <c r="E224" s="84"/>
       <c r="F224" s="21" t="s">
         <v>63</v>
       </c>
@@ -9807,11 +10203,11 @@
       <c r="C229" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D229" s="97" t="s">
+      <c r="D229" s="79" t="s">
         <v>54</v>
       </c>
-      <c r="E229" s="97"/>
-      <c r="F229" s="97"/>
+      <c r="E229" s="79"/>
+      <c r="F229" s="79"/>
       <c r="G229" s="57"/>
     </row>
     <row r="230" spans="1:7">
@@ -9824,11 +10220,11 @@
       <c r="C230" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D230" s="109" t="s">
+      <c r="D230" s="78" t="s">
         <v>55</v>
       </c>
-      <c r="E230" s="109"/>
-      <c r="F230" s="109"/>
+      <c r="E230" s="78"/>
+      <c r="F230" s="78"/>
       <c r="G230" s="41"/>
     </row>
     <row r="231" spans="1:7">
@@ -9841,11 +10237,11 @@
       <c r="C231" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D231" s="109" t="s">
+      <c r="D231" s="78" t="s">
         <v>245</v>
       </c>
-      <c r="E231" s="109"/>
-      <c r="F231" s="109"/>
+      <c r="E231" s="78"/>
+      <c r="F231" s="78"/>
       <c r="G231" s="41"/>
     </row>
     <row r="232" spans="1:7">
@@ -9858,11 +10254,11 @@
       <c r="C232" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D232" s="109" t="s">
+      <c r="D232" s="78" t="s">
         <v>246</v>
       </c>
-      <c r="E232" s="109"/>
-      <c r="F232" s="109"/>
+      <c r="E232" s="78"/>
+      <c r="F232" s="78"/>
       <c r="G232" s="41"/>
     </row>
     <row r="233" spans="1:7">
@@ -9875,11 +10271,11 @@
       <c r="C233" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D233" s="109" t="s">
+      <c r="D233" s="78" t="s">
         <v>247</v>
       </c>
-      <c r="E233" s="109"/>
-      <c r="F233" s="109"/>
+      <c r="E233" s="78"/>
+      <c r="F233" s="78"/>
       <c r="G233" s="41"/>
     </row>
     <row r="234" spans="1:7">
@@ -9892,11 +10288,11 @@
       <c r="C234" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D234" s="109" t="s">
+      <c r="D234" s="78" t="s">
         <v>248</v>
       </c>
-      <c r="E234" s="109"/>
-      <c r="F234" s="109"/>
+      <c r="E234" s="78"/>
+      <c r="F234" s="78"/>
       <c r="G234" s="41"/>
     </row>
     <row r="235" spans="1:7">
@@ -9909,11 +10305,11 @@
       <c r="C235" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D235" s="105" t="s">
+      <c r="D235" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="E235" s="106"/>
-      <c r="F235" s="107"/>
+      <c r="E235" s="75"/>
+      <c r="F235" s="76"/>
       <c r="G235" s="43"/>
     </row>
     <row r="236" spans="1:7">
@@ -9926,11 +10322,11 @@
       <c r="C236" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D236" s="105" t="s">
+      <c r="D236" s="74" t="s">
         <v>65</v>
       </c>
-      <c r="E236" s="106"/>
-      <c r="F236" s="107"/>
+      <c r="E236" s="75"/>
+      <c r="F236" s="76"/>
       <c r="G236" s="43"/>
     </row>
     <row r="237" spans="1:7">
@@ -9943,11 +10339,11 @@
       <c r="C237" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D237" s="105" t="s">
+      <c r="D237" s="74" t="s">
         <v>69</v>
       </c>
-      <c r="E237" s="106"/>
-      <c r="F237" s="107"/>
+      <c r="E237" s="75"/>
+      <c r="F237" s="76"/>
       <c r="G237" s="43"/>
     </row>
     <row r="238" spans="1:7">
@@ -10045,56 +10441,33 @@
       <c r="C243" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="D243" s="108" t="s">
+      <c r="D243" s="77" t="s">
         <v>264</v>
       </c>
-      <c r="E243" s="108"/>
-      <c r="F243" s="108"/>
+      <c r="E243" s="77"/>
+      <c r="F243" s="77"/>
       <c r="G243" s="44"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
+    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" scale="115">
       <selection activeCell="C4" sqref="C4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" scale="115">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
       <selection activeCell="C4" sqref="C4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="51">
-    <mergeCell ref="D236:F236"/>
-    <mergeCell ref="D237:F237"/>
-    <mergeCell ref="D243:F243"/>
-    <mergeCell ref="D230:F230"/>
-    <mergeCell ref="D231:F231"/>
-    <mergeCell ref="D232:F232"/>
-    <mergeCell ref="D233:F233"/>
-    <mergeCell ref="D234:F234"/>
-    <mergeCell ref="D235:F235"/>
-    <mergeCell ref="D229:F229"/>
-    <mergeCell ref="A212:A215"/>
-    <mergeCell ref="B212:B213"/>
-    <mergeCell ref="C212:E212"/>
-    <mergeCell ref="C213:E213"/>
-    <mergeCell ref="B214:B215"/>
-    <mergeCell ref="C214:E214"/>
-    <mergeCell ref="C215:E215"/>
-    <mergeCell ref="B220:E220"/>
-    <mergeCell ref="B221:E221"/>
-    <mergeCell ref="B222:E222"/>
-    <mergeCell ref="B223:E223"/>
-    <mergeCell ref="B224:E224"/>
-    <mergeCell ref="A208:A211"/>
-    <mergeCell ref="B208:B209"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C209:E209"/>
-    <mergeCell ref="B210:B211"/>
-    <mergeCell ref="C210:E210"/>
-    <mergeCell ref="C211:E211"/>
+    <mergeCell ref="B174:B176"/>
+    <mergeCell ref="F111:N111"/>
+    <mergeCell ref="B148:B160"/>
+    <mergeCell ref="B161:B162"/>
+    <mergeCell ref="B163:B165"/>
+    <mergeCell ref="B166:B173"/>
     <mergeCell ref="B177:B178"/>
     <mergeCell ref="B179:B185"/>
     <mergeCell ref="C199:E199"/>
@@ -10111,12 +10484,35 @@
     <mergeCell ref="B206:B207"/>
     <mergeCell ref="C206:E206"/>
     <mergeCell ref="C207:E207"/>
-    <mergeCell ref="B174:B176"/>
-    <mergeCell ref="F111:N111"/>
-    <mergeCell ref="B148:B160"/>
-    <mergeCell ref="B161:B162"/>
-    <mergeCell ref="B163:B165"/>
-    <mergeCell ref="B166:B173"/>
+    <mergeCell ref="A208:A211"/>
+    <mergeCell ref="B208:B209"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C209:E209"/>
+    <mergeCell ref="B210:B211"/>
+    <mergeCell ref="C210:E210"/>
+    <mergeCell ref="C211:E211"/>
+    <mergeCell ref="D229:F229"/>
+    <mergeCell ref="A212:A215"/>
+    <mergeCell ref="B212:B213"/>
+    <mergeCell ref="C212:E212"/>
+    <mergeCell ref="C213:E213"/>
+    <mergeCell ref="B214:B215"/>
+    <mergeCell ref="C214:E214"/>
+    <mergeCell ref="C215:E215"/>
+    <mergeCell ref="B220:E220"/>
+    <mergeCell ref="B221:E221"/>
+    <mergeCell ref="B222:E222"/>
+    <mergeCell ref="B223:E223"/>
+    <mergeCell ref="B224:E224"/>
+    <mergeCell ref="D236:F236"/>
+    <mergeCell ref="D237:F237"/>
+    <mergeCell ref="D243:F243"/>
+    <mergeCell ref="D230:F230"/>
+    <mergeCell ref="D231:F231"/>
+    <mergeCell ref="D232:F232"/>
+    <mergeCell ref="D233:F233"/>
+    <mergeCell ref="D234:F234"/>
+    <mergeCell ref="D235:F235"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -10139,18 +10535,18 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="E26" sqref="E26"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
i365--Apollo eit2 suite added
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/radiant/silicon_07_apollo.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/radiant/silicon_07_apollo.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="pSvbrBtM5D7J1tTbaFvNMFAx+gsFF1+zjWgivCK1irAkzVtGcdIaviGYDMewqTuAFCctlIpswoSn4Z8ezPPc6w==" workbookSaltValue="fuR2EkRIGc7n0eTkIKsWWA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="6300" windowWidth="28830" windowHeight="6240" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="suite" sheetId="1" r:id="rId1"/>
@@ -19,24 +19,24 @@
     <sheet name="comments" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">case!$A$2:$AE$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">case!$A$2:$AE$2</definedName>
     <definedName name="Z_16B2C8B3_13FA_43FB_96C1_3763C72619A6_.wvu.FilterData" localSheetId="1" hidden="1">case!$A$2:$AE$2</definedName>
     <definedName name="Z_179F0E1F_F6F7_410E_B883_54B8A90BA550_.wvu.FilterData" localSheetId="1" hidden="1">case!$A$2:$AE$2</definedName>
-    <definedName name="Z_3E5CE8AE_B586_4A12_8744_B7D8B6DA7A89_.wvu.FilterData" localSheetId="1" hidden="1">case!$A$2:$AE$8</definedName>
+    <definedName name="Z_3E5CE8AE_B586_4A12_8744_B7D8B6DA7A89_.wvu.FilterData" localSheetId="1" hidden="1">case!$A$2:$AE$2</definedName>
     <definedName name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" localSheetId="1" hidden="1">case!$A$2:$AE$2</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
+    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
     <customWorkbookView name="Jeffrey Ye - Personal View" guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="3"/>
-    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
-    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
-    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="576">
   <si>
     <t>[suite_info]</t>
   </si>
@@ -1341,81 +1341,6 @@
     <t>ITR1/07_SoftIP/307_Mult_Add_Sub/301_MAS_A_9_9_SS_11_1_L</t>
   </si>
   <si>
-    <t>ITR2/EIT2/DSP/101_MULT8_REG_REG_REG</t>
-  </si>
-  <si>
-    <t>ITR2/EIT2/DSP/201_MULT9A_REG_REG_REG</t>
-  </si>
-  <si>
-    <t>ITR2/EIT2/DSP/301_MULT18X18A_rega_regb_rego</t>
-  </si>
-  <si>
-    <t>ITR2/EIT2/DSP/400_MULTADDSUB18X18A_default</t>
-  </si>
-  <si>
-    <t>ITR2/EIT2/DSP/501_DOT9_INREG_REG1</t>
-  </si>
-  <si>
-    <t>ITR2/EIT2/DSP/601_DOT9A_INREG_REG1</t>
-  </si>
-  <si>
-    <t>ITR2/EIT2/EBR/105_SP16KA_1Kx18</t>
-  </si>
-  <si>
-    <t>ITR2/EIT2/EBR/201_SP32K_32Kx1</t>
-  </si>
-  <si>
-    <t>ITR2/EIT2/EBR/301_DP32K_1K_X36</t>
-  </si>
-  <si>
-    <t>ITR2/EIT2/EBR/401_pdp32k_1x32k</t>
-  </si>
-  <si>
-    <t>ITR2/EIT2/EBR/501_pdpsc32k_1x32k</t>
-  </si>
-  <si>
-    <t>ITR2/EIT2/EBR/602_FIFO32K_16KX2</t>
-  </si>
-  <si>
-    <t>Primitive MULT8              sim and flow check</t>
-  </si>
-  <si>
-    <t>Primitive MULT9A             sim and flow check</t>
-  </si>
-  <si>
-    <t>Primitive MULT18X18A         sim and flow check</t>
-  </si>
-  <si>
-    <t>Primitive MULTADDSUB18X18A   sim and flow check</t>
-  </si>
-  <si>
-    <t>Primitive DOT9               sim and flow check</t>
-  </si>
-  <si>
-    <t>Primitive DOT9A              sim and flow check</t>
-  </si>
-  <si>
-    <t>Primitive SP16KA             sim and flow check</t>
-  </si>
-  <si>
-    <t>Primitive SP32K              sim and flow check</t>
-  </si>
-  <si>
-    <t>Primitive DP32K              sim and flow check</t>
-  </si>
-  <si>
-    <t>Primitive pdp32k             sim and flow check</t>
-  </si>
-  <si>
-    <t>Primitive pdpsc32k           sim and flow check</t>
-  </si>
-  <si>
-    <t>Primitive FIFO32K            sim and flow check</t>
-  </si>
-  <si>
-    <t>sim;impl</t>
-  </si>
-  <si>
     <t>53</t>
   </si>
   <si>
@@ -1452,13 +1377,424 @@
     <t>64</t>
   </si>
   <si>
-    <t>silicon_07_apollo_v1.02</t>
+    <t>IOLOGIC</t>
+  </si>
+  <si>
+    <t>ITR2/13_IOLogic/03_sim/301_IFD1P3BX_ASYNC_PRESET</t>
+  </si>
+  <si>
+    <t>IFD1P3BX</t>
+  </si>
+  <si>
+    <t>Input FF with Asynchronous Preset</t>
+  </si>
+  <si>
+    <t>ITR2/13_IOLogic/03_sim/302_IFD1P3DX_ASYNC_CLR</t>
+  </si>
+  <si>
+    <t>IFD1P3DX</t>
+  </si>
+  <si>
+    <t>Input FF with Asynchronous Clear</t>
+  </si>
+  <si>
+    <t>ITR2/13_IOLogic/03_sim/303_IFD1P3IX_SYNC_CLR</t>
+  </si>
+  <si>
+    <t>IFD1P3IX</t>
+  </si>
+  <si>
+    <t>Input FF with Synchronous Clear</t>
+  </si>
+  <si>
+    <t>ITR2/13_IOLogic/03_sim/304_IFD1P3JX_SYNC_PRESET</t>
+  </si>
+  <si>
+    <t>IFD1P3JX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input FF with Synchronous Preset </t>
+  </si>
+  <si>
+    <t>ITR2/13_IOLogic/03_sim/305_OFD1P3BX_ASYNC_PRESET</t>
+  </si>
+  <si>
+    <t>OFD1P3BX</t>
+  </si>
+  <si>
+    <t>Output FF with Asynchronous Preset</t>
+  </si>
+  <si>
+    <t>ITR2/13_IOLogic/03_sim/306_OFD1P3DX_ASYNC_CLR</t>
+  </si>
+  <si>
+    <t>OFD1P3DX</t>
+  </si>
+  <si>
+    <t>Output FF with Asynchronous Clear</t>
+  </si>
+  <si>
+    <t>ITR2/13_IOLogic/03_sim/307_OFD1P3IX_SYNC_CLR</t>
+  </si>
+  <si>
+    <t>OFD1P3IX</t>
+  </si>
+  <si>
+    <t>Output FF with Synchronous Clear</t>
+  </si>
+  <si>
+    <t>ITR2/13_IOLogic/03_sim/308_OFD1P3JX_SYNC_PRESET</t>
+  </si>
+  <si>
+    <t>OFD1P3JX</t>
+  </si>
+  <si>
+    <t>Output FF with Synchronous Preset</t>
+  </si>
+  <si>
+    <t>ITR2/13_IOLogic/01_impl/301_IFD1P3BX_ASYNC_PRESET</t>
+  </si>
+  <si>
+    <t>ITR2/13_IOLogic/01_impl/302_IFD1P3DX_ASYNC_CLR</t>
+  </si>
+  <si>
+    <t>ITR2/13_IOLogic/01_impl/303_IFD1P3IX_SYNC_CLR</t>
+  </si>
+  <si>
+    <t>Input FF with Synchronous Clear (Clear Overrides Enable)</t>
+  </si>
+  <si>
+    <t>ITR2/13_IOLogic/01_impl/304_IFD1P3JX_SYNC_PRESET</t>
+  </si>
+  <si>
+    <t>Input FF with Synchronous Preset (Preset Overrides Enable)</t>
+  </si>
+  <si>
+    <t>ITR2/13_IOLogic/01_impl/305_OFD1P3BX_ASYNC_PRESET</t>
+  </si>
+  <si>
+    <t>ITR2/13_IOLogic/01_impl/306_OFD1P3DX_ASYNC_CLR</t>
+  </si>
+  <si>
+    <t>ITR2/13_IOLogic/01_impl/307_OFD1P3IX_SYNC_CLR</t>
+  </si>
+  <si>
+    <t>Output FF with Synchronous Clear (Clear Overrides Enable)</t>
+  </si>
+  <si>
+    <t>ITR2/13_IOLogic/01_impl/308_OFD1P3JX_SYNC_PRESET</t>
+  </si>
+  <si>
+    <t>Output FF with Synchronous Preset (Preset Overrides Enable)</t>
+  </si>
+  <si>
+    <t>ITR2/12_DSP/03_sim/01_MULT8X8/101_MULT8_REG_REG_REG</t>
+  </si>
+  <si>
+    <t>REG test,all REG="REGISTERED "</t>
+  </si>
+  <si>
+    <t>ITR2/12_DSP/03_sim/02_MULT9X9A/203_MULT9A_REG_BYP_REG</t>
+  </si>
+  <si>
+    <t>REG test,REGINPUTA="REGISTERED ",REGINPUTB="BYPASSED ",REGOUTPUT="REGISTERED "</t>
+  </si>
+  <si>
+    <t>ITR2/12_DSP/03_sim/03_MULT18X18A/301_MULT18X18A_rega_regb_rego</t>
+  </si>
+  <si>
+    <t>MULT18X18A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGINPUTA = "REGISTERED", REGINPUTB = "REGISTERED", REGOUTPUT = "REGISTERED", </t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>ITR2/12_DSP/03_sim/04_MULTADDSUB18X18A/400_MULTADDSUB18X18A_default</t>
+  </si>
+  <si>
+    <t>MULTADDSUB18X18A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default </t>
+  </si>
+  <si>
+    <t>ITR2/12_DSP/03_sim/05_DOTPRODADDSUB9X9/501_DOT9_INREG_REG1</t>
+  </si>
+  <si>
+    <t>REGINPUT test, all REGINPUT="REGISTERED_ONCE"</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>ITR2/12_DSP/03_sim/06_DOTPRODADDSUB9X9A/602_DOT9A_INREG_REG2</t>
+  </si>
+  <si>
+    <t>REGINPUT test, all REGINPUT="REGISTERED_TWICE"</t>
+  </si>
+  <si>
+    <t>ITR2/12_DSP/01_impl/01_MULT8X8/101_MULT8_impl</t>
+  </si>
+  <si>
+    <t>impl test</t>
+  </si>
+  <si>
+    <t>ITR2/12_DSP/01_impl/02_MULT9X9A/201_MULT9A_impl</t>
+  </si>
+  <si>
+    <t>ITR2/12_DSP/01_impl/05_DOTPRODADDSUB9X9/501_DOT9_impl</t>
+  </si>
+  <si>
+    <t>ITR2/12_DSP/01_impl/06_DOTPRODADDSUB9X9A/601_DOT9A_impl</t>
+  </si>
+  <si>
+    <t>ITR2/11_EBR/03_sim/04_PDP32K/401_pdp32k_1x32k</t>
+  </si>
+  <si>
+    <t>DATA_WIDTH_W/R ="X1" Addr_Width = 15 CSDECODE_W = "000" CSDECODE_R = "000"</t>
+  </si>
+  <si>
+    <t>ITR2/11_EBR/03_sim/05_PDPSC32K/501_pdpsc32k_1x32k</t>
+  </si>
+  <si>
+    <t>ITR2/11_EBR/01_impl/04_PDP32K/401_pdp32k_X1_impl</t>
+  </si>
+  <si>
+    <t>X1 impl</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>ITR2/11_EBR/01_impl/05_PDPSC32K/501_pdpsc32k_X1_impl</t>
+  </si>
+  <si>
+    <t>ITR2/11_EBR/03_sim/01_SP16KA/105_SP16KA_1Kx18</t>
+  </si>
+  <si>
+    <t>ITR2/11_EBR/03_sim/02_SP32K/201_SP32K_32Kx1</t>
+  </si>
+  <si>
+    <t>ITR2/11_EBR/03_sim/03_DP32K/301_DP32K_1K_X36</t>
+  </si>
+  <si>
+    <t>ITR2/07_SoftIP/311_1D_Filter/301_1DF_AS_2_P_S_S18_S18_B</t>
+  </si>
+  <si>
+    <t>1D_Filter,1D Asymmetry Serial,Taps=2,Positive,Sync,A_sign=Signed,A_width=18,B_sign=Signed,B_width=18,Big Endian,default</t>
+  </si>
+  <si>
+    <t>ITR2/07_SoftIP/312_Adder_Tree/302_AT_2_2_A_101</t>
+  </si>
+  <si>
+    <t>Adder_Tree,width=2,number=2,async,pipelined_mode=1,reg_input=0,reg_output=1</t>
+  </si>
+  <si>
+    <t>ITR2/07_SoftIP/313_DSP_Mult_Accumulate/302_DMA_2_2_UU_S_1111</t>
+  </si>
+  <si>
+    <t>DSP_Mult_Accumulate,A_width=2,B_width=2,A=unsigned,B=unsigned,sync,reg_inputA=1,reg_inputB=1,pipeline=1</t>
+  </si>
+  <si>
+    <t>ITR2/07_SoftIP/314_DSP_Mult_Add_Sub/301_DMAS_9_9_UU_S_1111</t>
+  </si>
+  <si>
+    <t>DSP_Mult_Add_Sub,A_width=9,B_width=9,A=unsigned,B=unsigned,sync,reg_AB0=1,,reg_AB1=1,pipeline=1,reg_output=1,default</t>
+  </si>
+  <si>
+    <t>ITR2/07_SoftIP/315_DSP_Mult_Add_Sub_Sum/301_DMASS_9_9_UU_S_1111</t>
+  </si>
+  <si>
+    <t>DSP_Mult_Add_Sub_Sum,A_width=9,B_width=9,A=unsigned,B=unsigned,sync,reg_A=1,,reg_B=1,pipeline=1,reg_output=1,default</t>
+  </si>
+  <si>
+    <t>ITR2/07_SoftIP/316_DSP_Mult_Mult_Accumulate/302_DMMA_2_2_SS_A_1111</t>
+  </si>
+  <si>
+    <t>DSP_Mult_Mult_Accumulate,A_width=2,B_width=2,A=signed,B=signed,async,reg_AB0=1,,reg_AB1=1,pipeline=1</t>
+  </si>
+  <si>
+    <t>ITR2/07_SoftIP/317_DSP_Multiplier/301_DM_9_9_S_SS_000</t>
+  </si>
+  <si>
+    <t>DSP_Multiplier,A_width=9,B_width=9,sync,A=signed,B=signed,reg_A=0,,reg_B=0,reg_output=0,default</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>79</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>91</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>93</t>
+  </si>
+  <si>
+    <t>94</t>
+  </si>
+  <si>
+    <t>ITR2/11_EBR/03_sim/06_FIFO32K/101_FIFO32K_32KX1</t>
+  </si>
+  <si>
+    <t>ITR2/11_EBR/01_impl/06_FIFO32K/602_FIFO32K_16KX2_impl</t>
+  </si>
+  <si>
+    <t>ITR2/07_SoftIP/401_RAM_DP/401_RAM_DP_default_512x36_Oreg_sync</t>
+  </si>
+  <si>
+    <t>ITR2/07_SoftIP/402_RAM_DP_Ture/411_RAM_DP_True_default_512x18_Oreg_RSTAseertion_sync</t>
+  </si>
+  <si>
+    <t>ITR2/07_SoftIP/403_RAM_DQ/421_RAM_DQ_default_512x36_Oreg_sync</t>
+  </si>
+  <si>
+    <t>ITR2/07_SoftIP/404_ROM/430_ROM_default_512x36_Oreg_sync_MemoryFile_hex</t>
+  </si>
+  <si>
+    <t>ITR2/07_SoftIP/405_FIFO/101_FIFO_default</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>97</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>ITR2/11_EBR/01_impl/01_SP16KA/101_SP16KA_16Kx1</t>
+  </si>
+  <si>
+    <t>ITR2/11_EBR/01_impl/02_SP32K/201_SP32K_32Kx1</t>
+  </si>
+  <si>
+    <t>ITR2/11_EBR/01_impl/03_DP32K/301_DP32K_1K_X36</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t>ITR2/07_SoftIP/406_FIFO_DC/101_FIFO_DC_default</t>
+  </si>
+  <si>
+    <t>106</t>
+  </si>
+  <si>
+    <t>ITR2/07_SoftIP/407_Shift_Register/101_Shift_Register_default</t>
+  </si>
+  <si>
+    <t>ITR2/12_DSP/01_impl/03_MULT18X18A/301_MULT18X18A_impl</t>
+  </si>
+  <si>
+    <t>MULT18X18A cell model</t>
+  </si>
+  <si>
+    <t>ITR2/12_DSP/01_impl/04_MULTADDSUB18X18A/401_MULTADDSUB18X18A_impl</t>
+  </si>
+  <si>
+    <t>MULTADDSBU18X18A cell model</t>
+  </si>
+  <si>
+    <t>suite_path = 07_Apollo</t>
   </si>
   <si>
     <t>repository = http://lsh-tmp/radiant/trunk/silicon</t>
   </si>
   <si>
-    <t>suite_path = 07_Apollo</t>
+    <t>silicon_07_apollo_v1.03</t>
   </si>
 </sst>
 </file>
@@ -1469,7 +1805,7 @@
     <numFmt numFmtId="164" formatCode="0.00_ "/>
     <numFmt numFmtId="165" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1654,6 +1990,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2549,7 +2891,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="12" fillId="7" borderId="7" xfId="13" applyNumberFormat="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -2755,9 +3097,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="12" fillId="7" borderId="27" xfId="13" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2770,76 +3109,49 @@
     <xf numFmtId="49" fontId="12" fillId="7" borderId="7" xfId="13" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
@@ -2859,17 +3171,44 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="48" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -2954,7 +3293,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -5121,7 +5466,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -5176,7 +5527,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="Add Test Case - TestRail - Mozilla Firefox"/>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Add Test Case - TestRail - Mozilla Firefox">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -5221,7 +5578,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -5340,7 +5703,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="6" name="Straight Arrow Connector 5"/>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -5387,7 +5756,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="Straight Arrow Connector 6"/>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -5711,8 +6086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -5743,7 +6118,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>461</v>
+        <v>575</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -5751,12 +6126,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>462</v>
+        <v>574</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="B5" s="2" t="s">
-        <v>463</v>
+        <v>573</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -6027,23 +6402,23 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
-    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" topLeftCell="A2">
-      <selection activeCell="C52" sqref="C52"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
+      <selection activeCell="B35" sqref="B35"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
       <selection activeCell="B4" sqref="B4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-    </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
-      <selection activeCell="B35" sqref="B35"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="G15" sqref="G15"/>
+    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" topLeftCell="A2">
+      <selection activeCell="C52" sqref="C52"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
@@ -6056,14 +6431,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE66"/>
+  <dimension ref="A1:AE108"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D62" sqref="D62:D66"/>
+      <selection pane="bottomRight" activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -6096,41 +6471,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="71"/>
-      <c r="O1" s="71"/>
-      <c r="P1" s="71"/>
-      <c r="Q1" s="71"/>
-      <c r="R1" s="71"/>
-      <c r="S1" s="71"/>
-      <c r="T1" s="71"/>
-      <c r="U1" s="71"/>
-      <c r="V1" s="71"/>
-      <c r="W1" s="72"/>
-      <c r="X1" s="73" t="s">
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
+      <c r="O1" s="70"/>
+      <c r="P1" s="70"/>
+      <c r="Q1" s="70"/>
+      <c r="R1" s="70"/>
+      <c r="S1" s="70"/>
+      <c r="T1" s="70"/>
+      <c r="U1" s="70"/>
+      <c r="V1" s="70"/>
+      <c r="W1" s="71"/>
+      <c r="X1" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="Y1" s="73"/>
-      <c r="Z1" s="73"/>
-      <c r="AA1" s="73"/>
-      <c r="AB1" s="73"/>
-      <c r="AC1" s="73"/>
-      <c r="AD1" s="73"/>
-      <c r="AE1" s="73"/>
+      <c r="Y1" s="72"/>
+      <c r="Z1" s="72"/>
+      <c r="AA1" s="72"/>
+      <c r="AB1" s="72"/>
+      <c r="AC1" s="72"/>
+      <c r="AD1" s="72"/>
+      <c r="AE1" s="72"/>
     </row>
     <row r="2" spans="1:31" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -7584,62 +7959,71 @@
     </row>
     <row r="55" spans="1:31">
       <c r="A55" s="2" t="s">
-        <v>449</v>
+        <v>424</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>117</v>
+        <v>436</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="H55" s="69" t="s">
-        <v>436</v>
+        <v>437</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>439</v>
       </c>
       <c r="S55" s="2" t="s">
         <v>303</v>
       </c>
       <c r="T55" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="AE55" s="69" t="s">
-        <v>448</v>
+        <v>300</v>
+      </c>
+      <c r="AE55" s="2" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="56" spans="1:31">
       <c r="A56" s="2" t="s">
-        <v>450</v>
+        <v>425</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>117</v>
+        <v>436</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>425</v>
-      </c>
-      <c r="H56" s="69" t="s">
-        <v>437</v>
+        <v>440</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>442</v>
       </c>
       <c r="S56" s="2" t="s">
         <v>303</v>
       </c>
       <c r="T56" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="AE56" s="69" t="s">
-        <v>448</v>
+        <v>300</v>
+      </c>
+      <c r="AE56" s="2" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="57" spans="1:31">
       <c r="A57" s="2" t="s">
-        <v>451</v>
+        <v>426</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>117</v>
+        <v>436</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>426</v>
-      </c>
-      <c r="H57" s="69" t="s">
-        <v>438</v>
+        <v>443</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>445</v>
       </c>
       <c r="S57" s="2" t="s">
         <v>303</v>
@@ -7647,22 +8031,25 @@
       <c r="T57" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="AE57" s="69" t="s">
-        <v>448</v>
+      <c r="AE57" s="2" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="58" spans="1:31">
       <c r="A58" s="2" t="s">
-        <v>452</v>
+        <v>427</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>117</v>
+        <v>436</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="H58" s="69" t="s">
-        <v>439</v>
+        <v>446</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>448</v>
       </c>
       <c r="S58" s="2" t="s">
         <v>303</v>
@@ -7670,201 +8057,1171 @@
       <c r="T58" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="AE58" s="69" t="s">
-        <v>448</v>
+      <c r="AE58" s="2" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="59" spans="1:31">
       <c r="A59" s="2" t="s">
-        <v>453</v>
+        <v>428</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>117</v>
+        <v>436</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="H59" s="69" t="s">
-        <v>440</v>
+        <v>449</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>451</v>
       </c>
       <c r="S59" s="2" t="s">
         <v>303</v>
       </c>
       <c r="T59" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="AE59" s="69" t="s">
-        <v>448</v>
+        <v>300</v>
+      </c>
+      <c r="AE59" s="2" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="60" spans="1:31">
       <c r="A60" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="H60" s="2" t="s">
         <v>454</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="H60" s="69" t="s">
-        <v>441</v>
       </c>
       <c r="S60" s="2" t="s">
         <v>303</v>
       </c>
       <c r="T60" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="AE60" s="69" t="s">
-        <v>448</v>
+        <v>300</v>
+      </c>
+      <c r="AE60" s="2" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="61" spans="1:31">
       <c r="A61" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="E61" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="H61" s="69" t="s">
-        <v>442</v>
+      <c r="G61" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>457</v>
       </c>
       <c r="S61" s="2" t="s">
         <v>303</v>
       </c>
       <c r="T61" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="AE61" s="69" t="s">
-        <v>448</v>
+        <v>300</v>
+      </c>
+      <c r="AE61" s="2" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="62" spans="1:31">
       <c r="A62" s="2" t="s">
-        <v>456</v>
+        <v>431</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>118</v>
+        <v>436</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="H62" s="69" t="s">
-        <v>443</v>
+        <v>458</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>460</v>
       </c>
       <c r="S62" s="2" t="s">
         <v>303</v>
       </c>
       <c r="T62" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="AE62" s="69" t="s">
-        <v>448</v>
+        <v>300</v>
+      </c>
+      <c r="AE62" s="2" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="63" spans="1:31">
       <c r="A63" s="2" t="s">
-        <v>457</v>
+        <v>432</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>118</v>
+        <v>436</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>432</v>
-      </c>
-      <c r="H63" s="69" t="s">
-        <v>444</v>
+        <v>461</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>439</v>
       </c>
       <c r="S63" s="2" t="s">
         <v>303</v>
       </c>
       <c r="T63" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="AE63" s="69" t="s">
-        <v>448</v>
+        <v>300</v>
+      </c>
+      <c r="AE63" s="2" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="64" spans="1:31">
       <c r="A64" s="2" t="s">
-        <v>458</v>
+        <v>433</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>118</v>
+        <v>436</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="H64" s="69" t="s">
-        <v>445</v>
+        <v>462</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>442</v>
       </c>
       <c r="S64" s="2" t="s">
         <v>303</v>
       </c>
       <c r="T64" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="AE64" s="69" t="s">
-        <v>448</v>
+        <v>300</v>
+      </c>
+      <c r="AE64" s="2" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="65" spans="1:31">
       <c r="A65" s="2" t="s">
-        <v>459</v>
+        <v>434</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>118</v>
+        <v>436</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="H65" s="69" t="s">
-        <v>446</v>
+        <v>463</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>464</v>
       </c>
       <c r="S65" s="2" t="s">
         <v>303</v>
       </c>
       <c r="T65" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="AE65" s="69" t="s">
-        <v>448</v>
+        <v>300</v>
+      </c>
+      <c r="AE65" s="2" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="66" spans="1:31">
       <c r="A66" s="2" t="s">
-        <v>460</v>
+        <v>435</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>118</v>
+        <v>436</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="H66" s="69" t="s">
+        <v>465</v>
+      </c>
+      <c r="G66" s="2" t="s">
         <v>447</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>466</v>
       </c>
       <c r="S66" s="2" t="s">
         <v>303</v>
       </c>
       <c r="T66" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="AE66" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="67" spans="1:31">
+      <c r="A67" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="S67" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T67" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="AE67" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="68" spans="1:31">
+      <c r="A68" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="S68" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T68" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="AE68" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="69" spans="1:31">
+      <c r="A69" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="S69" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T69" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="AE69" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="70" spans="1:31">
+      <c r="A70" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="S70" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T70" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="AE70" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="71" spans="1:31">
+      <c r="A71" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="S71" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T71" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="AE71" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="72" spans="1:31">
+      <c r="A72" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="S72" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T72" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="AE72" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="73" spans="1:31">
+      <c r="A73" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="S73" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T73" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="AE73" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="74" spans="1:31">
+      <c r="A74" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="S74" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T74" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="AE74" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="75" spans="1:31">
+      <c r="A75" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="S75" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T75" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="AE75" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="76" spans="1:31">
+      <c r="A76" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="S76" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T76" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="AE76" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="77" spans="1:31">
+      <c r="A77" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="S77" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T77" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="AE77" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="78" spans="1:31">
+      <c r="A78" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="S78" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T78" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="AE78" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="79" spans="1:31">
+      <c r="A79" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="S79" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T79" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="AE79" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="80" spans="1:31">
+      <c r="A80" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="S80" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T80" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="AE80" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="81" spans="1:31">
+      <c r="A81" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="S81" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T81" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="AE81" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="82" spans="1:31">
+      <c r="A82" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="S82" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T82" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="AE82" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="83" spans="1:31">
+      <c r="A83" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="S83" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T83" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="AE83" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="84" spans="1:31">
+      <c r="A84" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="S84" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T84" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="AE84" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="85" spans="1:31">
+      <c r="A85" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="S85" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T85" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="AE85" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="86" spans="1:31">
+      <c r="A86" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="S86" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T86" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="AE86" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="87" spans="1:31">
+      <c r="A87" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="S87" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T87" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="AE87" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="88" spans="1:31">
+      <c r="A88" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="S88" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T88" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="AE66" s="69" t="s">
-        <v>448</v>
+      <c r="AE88" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="89" spans="1:31">
+      <c r="A89" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="S89" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T89" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="AE89" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="90" spans="1:31">
+      <c r="A90" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="S90" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T90" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="AE90" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="91" spans="1:31">
+      <c r="A91" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="S91" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T91" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="AE91" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="92" spans="1:31">
+      <c r="A92" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="H92" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="S92" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T92" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="AE92" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="93" spans="1:31">
+      <c r="A93" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="H93" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="S93" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T93" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="AE93" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="94" spans="1:31">
+      <c r="A94" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="S94" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T94" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="AE94" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="95" spans="1:31">
+      <c r="A95" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="H95" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="S95" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="T95" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="AE95" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="96" spans="1:31">
+      <c r="A96" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="H96" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="S96" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="T96" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="AE96" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="97" spans="1:31">
+      <c r="A97" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="H97" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="S97" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="T97" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="AE97" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="98" spans="1:31">
+      <c r="A98" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="H98" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="S98" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="T98" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="AE98" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="99" spans="1:31">
+      <c r="A99" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="H99" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="S99" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="T99" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="AE99" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="100" spans="1:31">
+      <c r="A100" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="H100" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="S100" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="T100" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="AE100" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="101" spans="1:31">
+      <c r="A101" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="H101" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="S101" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="T101" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="AE101" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="102" spans="1:31">
+      <c r="A102" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="S102" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="T102" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="AE102" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="103" spans="1:31">
+      <c r="A103" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="S103" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="T103" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="AE103" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="104" spans="1:31">
+      <c r="A104" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="S104" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="T104" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="AE104" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="105" spans="1:31">
+      <c r="A105" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="S105" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="T105" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="AE105" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="106" spans="1:31">
+      <c r="A106" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="S106" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="T106" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="AE106" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="107" spans="1:31">
+      <c r="A107" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="S107" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="T107" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="AE107" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="108" spans="1:31">
+      <c r="A108" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="S108" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="T108" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="AE108" s="2" t="s">
+        <v>309</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="oSh3vRnxVqjddGqXIe7WCBtY0UIhfw+5hx9hFmwK+zOVJn30i2qdL6F35lxIbLPoaaesJXtjEAYmG4HcQFEykg==" saltValue="88e6IcLciP+0JP9xgq1/0Q==" spinCount="100000" sheet="1" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <autoFilter ref="A2:AE36"/>
+  <autoFilter ref="A2:AE2"/>
   <mergeCells count="2">
     <mergeCell ref="A1:W1"/>
     <mergeCell ref="X1:AE1"/>
   </mergeCells>
+  <phoneticPr fontId="23" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE1 M1:AB1 G1:H1 C1:E1 A1">
       <formula1>#REF!</formula1>
@@ -7995,17 +9352,17 @@
       <c r="E111" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F111" s="107" t="s">
+      <c r="F111" s="75" t="s">
         <v>87</v>
       </c>
-      <c r="G111" s="108"/>
-      <c r="H111" s="108"/>
-      <c r="I111" s="108"/>
-      <c r="J111" s="108"/>
-      <c r="K111" s="108"/>
-      <c r="L111" s="108"/>
-      <c r="M111" s="108"/>
-      <c r="N111" s="109"/>
+      <c r="G111" s="76"/>
+      <c r="H111" s="76"/>
+      <c r="I111" s="76"/>
+      <c r="J111" s="76"/>
+      <c r="K111" s="76"/>
+      <c r="L111" s="76"/>
+      <c r="M111" s="76"/>
+      <c r="N111" s="77"/>
     </row>
     <row r="112" spans="1:14">
       <c r="A112" s="11" t="s">
@@ -8895,7 +10252,7 @@
       <c r="A148" s="26">
         <v>1</v>
       </c>
-      <c r="B148" s="92" t="s">
+      <c r="B148" s="78" t="s">
         <v>3</v>
       </c>
       <c r="C148" s="27" t="s">
@@ -8921,7 +10278,7 @@
       <c r="A149" s="26">
         <v>2</v>
       </c>
-      <c r="B149" s="93"/>
+      <c r="B149" s="79"/>
       <c r="C149" s="28" t="s">
         <v>136</v>
       </c>
@@ -8943,7 +10300,7 @@
       <c r="A150" s="26">
         <v>3</v>
       </c>
-      <c r="B150" s="93"/>
+      <c r="B150" s="79"/>
       <c r="C150" s="28" t="s">
         <v>9</v>
       </c>
@@ -8963,7 +10320,7 @@
       <c r="A151" s="26">
         <v>4</v>
       </c>
-      <c r="B151" s="93"/>
+      <c r="B151" s="79"/>
       <c r="C151" s="28" t="s">
         <v>138</v>
       </c>
@@ -8987,7 +10344,7 @@
       <c r="A152" s="26">
         <v>5</v>
       </c>
-      <c r="B152" s="93"/>
+      <c r="B152" s="79"/>
       <c r="C152" s="27" t="s">
         <v>140</v>
       </c>
@@ -9011,7 +10368,7 @@
       <c r="A153" s="26">
         <v>6</v>
       </c>
-      <c r="B153" s="93"/>
+      <c r="B153" s="79"/>
       <c r="C153" s="27" t="s">
         <v>144</v>
       </c>
@@ -9035,7 +10392,7 @@
       <c r="A154" s="26">
         <v>7</v>
       </c>
-      <c r="B154" s="93"/>
+      <c r="B154" s="79"/>
       <c r="C154" s="28" t="s">
         <v>147</v>
       </c>
@@ -9057,7 +10414,7 @@
       <c r="A155" s="26">
         <v>8</v>
       </c>
-      <c r="B155" s="93"/>
+      <c r="B155" s="79"/>
       <c r="C155" s="27" t="s">
         <v>148</v>
       </c>
@@ -9081,7 +10438,7 @@
       <c r="A156" s="26">
         <v>9</v>
       </c>
-      <c r="B156" s="93"/>
+      <c r="B156" s="79"/>
       <c r="C156" s="27" t="s">
         <v>149</v>
       </c>
@@ -9105,7 +10462,7 @@
       <c r="A157" s="26">
         <v>10</v>
       </c>
-      <c r="B157" s="93"/>
+      <c r="B157" s="79"/>
       <c r="C157" s="28" t="s">
         <v>150</v>
       </c>
@@ -9129,7 +10486,7 @@
       <c r="A158" s="26">
         <v>11</v>
       </c>
-      <c r="B158" s="93"/>
+      <c r="B158" s="79"/>
       <c r="C158" s="68" t="s">
         <v>151</v>
       </c>
@@ -9153,7 +10510,7 @@
       <c r="A159" s="26">
         <v>12</v>
       </c>
-      <c r="B159" s="93"/>
+      <c r="B159" s="79"/>
       <c r="C159" s="28" t="s">
         <v>153</v>
       </c>
@@ -9175,7 +10532,7 @@
       <c r="A160" s="26">
         <v>13</v>
       </c>
-      <c r="B160" s="87"/>
+      <c r="B160" s="80"/>
       <c r="C160" s="28" t="s">
         <v>56</v>
       </c>
@@ -9199,7 +10556,7 @@
       <c r="A161" s="26">
         <v>14</v>
       </c>
-      <c r="B161" s="83" t="s">
+      <c r="B161" s="73" t="s">
         <v>4</v>
       </c>
       <c r="C161" s="28" t="s">
@@ -9225,7 +10582,7 @@
       <c r="A162" s="26">
         <v>15</v>
       </c>
-      <c r="B162" s="82"/>
+      <c r="B162" s="74"/>
       <c r="C162" s="28" t="s">
         <v>161</v>
       </c>
@@ -9249,7 +10606,7 @@
       <c r="A163" s="26">
         <v>16</v>
       </c>
-      <c r="B163" s="92" t="s">
+      <c r="B163" s="78" t="s">
         <v>5</v>
       </c>
       <c r="C163" s="28" t="s">
@@ -9273,7 +10630,7 @@
       <c r="A164" s="26">
         <v>17</v>
       </c>
-      <c r="B164" s="110"/>
+      <c r="B164" s="81"/>
       <c r="C164" s="27" t="s">
         <v>165</v>
       </c>
@@ -9295,7 +10652,7 @@
       <c r="A165" s="26">
         <v>18</v>
       </c>
-      <c r="B165" s="87"/>
+      <c r="B165" s="80"/>
       <c r="C165" s="27" t="s">
         <v>167</v>
       </c>
@@ -9315,7 +10672,7 @@
       <c r="A166" s="26">
         <v>19</v>
       </c>
-      <c r="B166" s="83" t="s">
+      <c r="B166" s="73" t="s">
         <v>6</v>
       </c>
       <c r="C166" s="28" t="s">
@@ -9339,7 +10696,7 @@
       <c r="A167" s="26">
         <v>20</v>
       </c>
-      <c r="B167" s="82"/>
+      <c r="B167" s="74"/>
       <c r="C167" s="28" t="s">
         <v>172</v>
       </c>
@@ -9359,7 +10716,7 @@
       <c r="A168" s="26">
         <v>21</v>
       </c>
-      <c r="B168" s="82"/>
+      <c r="B168" s="74"/>
       <c r="C168" s="28" t="s">
         <v>173</v>
       </c>
@@ -9379,7 +10736,7 @@
       <c r="A169" s="26">
         <v>22</v>
       </c>
-      <c r="B169" s="82"/>
+      <c r="B169" s="74"/>
       <c r="C169" s="28" t="s">
         <v>174</v>
       </c>
@@ -9399,7 +10756,7 @@
       <c r="A170" s="26">
         <v>23</v>
       </c>
-      <c r="B170" s="82"/>
+      <c r="B170" s="74"/>
       <c r="C170" s="28" t="s">
         <v>175</v>
       </c>
@@ -9419,7 +10776,7 @@
       <c r="A171" s="26">
         <v>24</v>
       </c>
-      <c r="B171" s="82"/>
+      <c r="B171" s="74"/>
       <c r="C171" s="28" t="s">
         <v>176</v>
       </c>
@@ -9439,7 +10796,7 @@
       <c r="A172" s="26">
         <v>25</v>
       </c>
-      <c r="B172" s="82"/>
+      <c r="B172" s="74"/>
       <c r="C172" s="28" t="s">
         <v>177</v>
       </c>
@@ -9459,7 +10816,7 @@
       <c r="A173" s="26">
         <v>26</v>
       </c>
-      <c r="B173" s="82"/>
+      <c r="B173" s="74"/>
       <c r="C173" s="28" t="s">
         <v>41</v>
       </c>
@@ -9479,7 +10836,7 @@
       <c r="A174" s="26">
         <v>27</v>
       </c>
-      <c r="B174" s="83" t="s">
+      <c r="B174" s="73" t="s">
         <v>7</v>
       </c>
       <c r="C174" s="28" t="s">
@@ -9503,7 +10860,7 @@
       <c r="A175" s="26">
         <v>28</v>
       </c>
-      <c r="B175" s="82"/>
+      <c r="B175" s="74"/>
       <c r="C175" s="27" t="s">
         <v>181</v>
       </c>
@@ -9525,7 +10882,7 @@
       <c r="A176" s="26">
         <v>29</v>
       </c>
-      <c r="B176" s="82"/>
+      <c r="B176" s="74"/>
       <c r="C176" s="28" t="s">
         <v>184</v>
       </c>
@@ -9547,7 +10904,7 @@
       <c r="A177" s="26">
         <v>30</v>
       </c>
-      <c r="B177" s="92" t="s">
+      <c r="B177" s="78" t="s">
         <v>8</v>
       </c>
       <c r="C177" s="28" t="s">
@@ -9573,7 +10930,7 @@
       <c r="A178" s="31">
         <v>31</v>
       </c>
-      <c r="B178" s="93"/>
+      <c r="B178" s="79"/>
       <c r="C178" s="32" t="s">
         <v>189</v>
       </c>
@@ -9597,7 +10954,7 @@
       <c r="A179" s="23">
         <v>32</v>
       </c>
-      <c r="B179" s="94" t="s">
+      <c r="B179" s="82" t="s">
         <v>191</v>
       </c>
       <c r="C179" s="33" t="s">
@@ -9621,7 +10978,7 @@
       <c r="A180" s="26">
         <v>33</v>
       </c>
-      <c r="B180" s="95"/>
+      <c r="B180" s="83"/>
       <c r="C180" s="27" t="s">
         <v>195</v>
       </c>
@@ -9643,7 +11000,7 @@
       <c r="A181" s="26">
         <v>34</v>
       </c>
-      <c r="B181" s="96"/>
+      <c r="B181" s="84"/>
       <c r="C181" s="34" t="s">
         <v>198</v>
       </c>
@@ -9665,7 +11022,7 @@
       <c r="A182" s="31">
         <v>35</v>
       </c>
-      <c r="B182" s="96"/>
+      <c r="B182" s="84"/>
       <c r="C182" s="34" t="s">
         <v>199</v>
       </c>
@@ -9687,7 +11044,7 @@
       <c r="A183" s="31">
         <v>36</v>
       </c>
-      <c r="B183" s="96"/>
+      <c r="B183" s="84"/>
       <c r="C183" s="34" t="s">
         <v>202</v>
       </c>
@@ -9707,7 +11064,7 @@
       <c r="A184" s="31">
         <v>37</v>
       </c>
-      <c r="B184" s="96"/>
+      <c r="B184" s="84"/>
       <c r="C184" s="34" t="s">
         <v>254</v>
       </c>
@@ -9729,7 +11086,7 @@
       <c r="A185" s="35">
         <v>38</v>
       </c>
-      <c r="B185" s="91"/>
+      <c r="B185" s="85"/>
       <c r="C185" s="36" t="s">
         <v>258</v>
       </c>
@@ -9780,11 +11137,11 @@
       <c r="B199" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="C199" s="97" t="s">
+      <c r="C199" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="D199" s="97"/>
-      <c r="E199" s="97"/>
+      <c r="D199" s="86"/>
+      <c r="E199" s="86"/>
       <c r="F199" s="39" t="s">
         <v>43</v>
       </c>
@@ -9793,17 +11150,17 @@
       </c>
     </row>
     <row r="200" spans="1:7">
-      <c r="A200" s="80" t="s">
+      <c r="A200" s="87" t="s">
         <v>212</v>
       </c>
-      <c r="B200" s="82" t="s">
+      <c r="B200" s="74" t="s">
         <v>213</v>
       </c>
-      <c r="C200" s="99" t="s">
+      <c r="C200" s="89" t="s">
         <v>57</v>
       </c>
-      <c r="D200" s="100"/>
-      <c r="E200" s="100"/>
+      <c r="D200" s="90"/>
+      <c r="E200" s="90"/>
       <c r="F200" s="28" t="s">
         <v>214</v>
       </c>
@@ -9812,13 +11169,13 @@
       </c>
     </row>
     <row r="201" spans="1:7">
-      <c r="A201" s="80"/>
-      <c r="B201" s="98"/>
-      <c r="C201" s="101" t="s">
+      <c r="A201" s="87"/>
+      <c r="B201" s="88"/>
+      <c r="C201" s="91" t="s">
         <v>57</v>
       </c>
-      <c r="D201" s="102"/>
-      <c r="E201" s="102"/>
+      <c r="D201" s="92"/>
+      <c r="E201" s="92"/>
       <c r="F201" s="32" t="s">
         <v>215</v>
       </c>
@@ -9827,15 +11184,15 @@
       </c>
     </row>
     <row r="202" spans="1:7">
-      <c r="A202" s="80"/>
-      <c r="B202" s="82" t="s">
+      <c r="A202" s="87"/>
+      <c r="B202" s="74" t="s">
         <v>216</v>
       </c>
-      <c r="C202" s="103" t="s">
+      <c r="C202" s="93" t="s">
         <v>217</v>
       </c>
-      <c r="D202" s="103"/>
-      <c r="E202" s="103"/>
+      <c r="D202" s="93"/>
+      <c r="E202" s="93"/>
       <c r="F202" s="28" t="s">
         <v>214</v>
       </c>
@@ -9844,13 +11201,13 @@
       </c>
     </row>
     <row r="203" spans="1:7">
-      <c r="A203" s="80"/>
-      <c r="B203" s="82"/>
-      <c r="C203" s="101" t="s">
+      <c r="A203" s="87"/>
+      <c r="B203" s="74"/>
+      <c r="C203" s="91" t="s">
         <v>217</v>
       </c>
-      <c r="D203" s="101"/>
-      <c r="E203" s="101"/>
+      <c r="D203" s="91"/>
+      <c r="E203" s="91"/>
       <c r="F203" s="28" t="s">
         <v>215</v>
       </c>
@@ -9859,15 +11216,15 @@
       </c>
     </row>
     <row r="204" spans="1:7">
-      <c r="A204" s="80"/>
-      <c r="B204" s="98" t="s">
+      <c r="A204" s="87"/>
+      <c r="B204" s="88" t="s">
         <v>218</v>
       </c>
-      <c r="C204" s="104" t="s">
+      <c r="C204" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="D204" s="105"/>
-      <c r="E204" s="106"/>
+      <c r="D204" s="95"/>
+      <c r="E204" s="96"/>
       <c r="F204" s="28" t="s">
         <v>214</v>
       </c>
@@ -9876,13 +11233,13 @@
       </c>
     </row>
     <row r="205" spans="1:7">
-      <c r="A205" s="80"/>
-      <c r="B205" s="87"/>
-      <c r="C205" s="104" t="s">
+      <c r="A205" s="87"/>
+      <c r="B205" s="80"/>
+      <c r="C205" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="D205" s="105"/>
-      <c r="E205" s="106"/>
+      <c r="D205" s="95"/>
+      <c r="E205" s="96"/>
       <c r="F205" s="28" t="s">
         <v>215</v>
       </c>
@@ -9891,15 +11248,15 @@
       </c>
     </row>
     <row r="206" spans="1:7">
-      <c r="A206" s="80"/>
-      <c r="B206" s="82" t="s">
+      <c r="A206" s="87"/>
+      <c r="B206" s="74" t="s">
         <v>219</v>
       </c>
-      <c r="C206" s="103" t="s">
+      <c r="C206" s="93" t="s">
         <v>220</v>
       </c>
-      <c r="D206" s="103"/>
-      <c r="E206" s="103"/>
+      <c r="D206" s="93"/>
+      <c r="E206" s="93"/>
       <c r="F206" s="28" t="s">
         <v>214</v>
       </c>
@@ -9908,13 +11265,13 @@
       </c>
     </row>
     <row r="207" spans="1:7">
-      <c r="A207" s="80"/>
-      <c r="B207" s="82"/>
-      <c r="C207" s="103" t="s">
+      <c r="A207" s="87"/>
+      <c r="B207" s="74"/>
+      <c r="C207" s="93" t="s">
         <v>220</v>
       </c>
-      <c r="D207" s="103"/>
-      <c r="E207" s="103"/>
+      <c r="D207" s="93"/>
+      <c r="E207" s="93"/>
       <c r="F207" s="28" t="s">
         <v>215</v>
       </c>
@@ -9923,17 +11280,17 @@
       </c>
     </row>
     <row r="208" spans="1:7">
-      <c r="A208" s="80" t="s">
+      <c r="A208" s="87" t="s">
         <v>221</v>
       </c>
-      <c r="B208" s="82" t="s">
+      <c r="B208" s="74" t="s">
         <v>222</v>
       </c>
-      <c r="C208" s="83" t="s">
+      <c r="C208" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="D208" s="82"/>
-      <c r="E208" s="82"/>
+      <c r="D208" s="74"/>
+      <c r="E208" s="74"/>
       <c r="F208" s="28" t="s">
         <v>214</v>
       </c>
@@ -9942,13 +11299,13 @@
       </c>
     </row>
     <row r="209" spans="1:7">
-      <c r="A209" s="80"/>
-      <c r="B209" s="82"/>
-      <c r="C209" s="82" t="s">
+      <c r="A209" s="87"/>
+      <c r="B209" s="74"/>
+      <c r="C209" s="74" t="s">
         <v>46</v>
       </c>
-      <c r="D209" s="82"/>
-      <c r="E209" s="82"/>
+      <c r="D209" s="74"/>
+      <c r="E209" s="74"/>
       <c r="F209" s="28" t="s">
         <v>215</v>
       </c>
@@ -9957,15 +11314,15 @@
       </c>
     </row>
     <row r="210" spans="1:7">
-      <c r="A210" s="80"/>
-      <c r="B210" s="82" t="s">
+      <c r="A210" s="87"/>
+      <c r="B210" s="74" t="s">
         <v>224</v>
       </c>
-      <c r="C210" s="83" t="s">
+      <c r="C210" s="73" t="s">
         <v>47</v>
       </c>
-      <c r="D210" s="82"/>
-      <c r="E210" s="82"/>
+      <c r="D210" s="74"/>
+      <c r="E210" s="74"/>
       <c r="F210" s="28" t="s">
         <v>214</v>
       </c>
@@ -9974,13 +11331,13 @@
       </c>
     </row>
     <row r="211" spans="1:7">
-      <c r="A211" s="80"/>
-      <c r="B211" s="82"/>
-      <c r="C211" s="82" t="s">
+      <c r="A211" s="87"/>
+      <c r="B211" s="74"/>
+      <c r="C211" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="D211" s="82"/>
-      <c r="E211" s="82"/>
+      <c r="D211" s="74"/>
+      <c r="E211" s="74"/>
       <c r="F211" s="28" t="s">
         <v>215</v>
       </c>
@@ -9989,17 +11346,17 @@
       </c>
     </row>
     <row r="212" spans="1:7">
-      <c r="A212" s="80" t="s">
+      <c r="A212" s="87" t="s">
         <v>225</v>
       </c>
-      <c r="B212" s="82" t="s">
+      <c r="B212" s="74" t="s">
         <v>226</v>
       </c>
-      <c r="C212" s="83" t="s">
+      <c r="C212" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="D212" s="82"/>
-      <c r="E212" s="82"/>
+      <c r="D212" s="74"/>
+      <c r="E212" s="74"/>
       <c r="F212" s="28" t="s">
         <v>214</v>
       </c>
@@ -10008,13 +11365,13 @@
       </c>
     </row>
     <row r="213" spans="1:7">
-      <c r="A213" s="80"/>
-      <c r="B213" s="82"/>
-      <c r="C213" s="82" t="s">
+      <c r="A213" s="87"/>
+      <c r="B213" s="74"/>
+      <c r="C213" s="74" t="s">
         <v>50</v>
       </c>
-      <c r="D213" s="82"/>
-      <c r="E213" s="82"/>
+      <c r="D213" s="74"/>
+      <c r="E213" s="74"/>
       <c r="F213" s="28" t="s">
         <v>215</v>
       </c>
@@ -10023,15 +11380,15 @@
       </c>
     </row>
     <row r="214" spans="1:7">
-      <c r="A214" s="80"/>
-      <c r="B214" s="82" t="s">
+      <c r="A214" s="87"/>
+      <c r="B214" s="74" t="s">
         <v>227</v>
       </c>
-      <c r="C214" s="83" t="s">
+      <c r="C214" s="73" t="s">
         <v>228</v>
       </c>
-      <c r="D214" s="82"/>
-      <c r="E214" s="82"/>
+      <c r="D214" s="74"/>
+      <c r="E214" s="74"/>
       <c r="F214" s="28" t="s">
         <v>214</v>
       </c>
@@ -10040,13 +11397,13 @@
       </c>
     </row>
     <row r="215" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A215" s="81"/>
-      <c r="B215" s="84"/>
-      <c r="C215" s="84" t="s">
+      <c r="A215" s="98"/>
+      <c r="B215" s="99"/>
+      <c r="C215" s="99" t="s">
         <v>229</v>
       </c>
-      <c r="D215" s="84"/>
-      <c r="E215" s="84"/>
+      <c r="D215" s="99"/>
+      <c r="E215" s="99"/>
       <c r="F215" s="36" t="s">
         <v>215</v>
       </c>
@@ -10085,12 +11442,12 @@
       <c r="A220" s="45" t="s">
         <v>232</v>
       </c>
-      <c r="B220" s="85" t="s">
+      <c r="B220" s="100" t="s">
         <v>52</v>
       </c>
-      <c r="C220" s="85"/>
-      <c r="D220" s="85"/>
-      <c r="E220" s="85"/>
+      <c r="C220" s="100"/>
+      <c r="D220" s="100"/>
+      <c r="E220" s="100"/>
       <c r="F220" s="46" t="s">
         <v>233</v>
       </c>
@@ -10102,12 +11459,12 @@
       <c r="A221" s="48" t="s">
         <v>235</v>
       </c>
-      <c r="B221" s="86" t="s">
+      <c r="B221" s="101" t="s">
         <v>236</v>
       </c>
-      <c r="C221" s="87"/>
-      <c r="D221" s="87"/>
-      <c r="E221" s="87"/>
+      <c r="C221" s="80"/>
+      <c r="D221" s="80"/>
+      <c r="E221" s="80"/>
       <c r="F221" s="49" t="s">
         <v>111</v>
       </c>
@@ -10119,12 +11476,12 @@
       <c r="A222" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="B222" s="88" t="s">
+      <c r="B222" s="102" t="s">
         <v>238</v>
       </c>
-      <c r="C222" s="89"/>
-      <c r="D222" s="89"/>
-      <c r="E222" s="90"/>
+      <c r="C222" s="103"/>
+      <c r="D222" s="103"/>
+      <c r="E222" s="104"/>
       <c r="F222" s="15" t="s">
         <v>63</v>
       </c>
@@ -10136,12 +11493,12 @@
       <c r="A223" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B223" s="88" t="s">
+      <c r="B223" s="102" t="s">
         <v>239</v>
       </c>
-      <c r="C223" s="89"/>
-      <c r="D223" s="89"/>
-      <c r="E223" s="90"/>
+      <c r="C223" s="103"/>
+      <c r="D223" s="103"/>
+      <c r="E223" s="104"/>
       <c r="F223" s="18" t="s">
         <v>63</v>
       </c>
@@ -10153,12 +11510,12 @@
       <c r="A224" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="B224" s="91" t="s">
+      <c r="B224" s="85" t="s">
         <v>241</v>
       </c>
-      <c r="C224" s="84"/>
-      <c r="D224" s="84"/>
-      <c r="E224" s="84"/>
+      <c r="C224" s="99"/>
+      <c r="D224" s="99"/>
+      <c r="E224" s="99"/>
       <c r="F224" s="21" t="s">
         <v>63</v>
       </c>
@@ -10203,11 +11560,11 @@
       <c r="C229" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D229" s="79" t="s">
+      <c r="D229" s="97" t="s">
         <v>54</v>
       </c>
-      <c r="E229" s="79"/>
-      <c r="F229" s="79"/>
+      <c r="E229" s="97"/>
+      <c r="F229" s="97"/>
       <c r="G229" s="57"/>
     </row>
     <row r="230" spans="1:7">
@@ -10220,11 +11577,11 @@
       <c r="C230" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D230" s="78" t="s">
+      <c r="D230" s="109" t="s">
         <v>55</v>
       </c>
-      <c r="E230" s="78"/>
-      <c r="F230" s="78"/>
+      <c r="E230" s="109"/>
+      <c r="F230" s="109"/>
       <c r="G230" s="41"/>
     </row>
     <row r="231" spans="1:7">
@@ -10237,11 +11594,11 @@
       <c r="C231" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D231" s="78" t="s">
+      <c r="D231" s="109" t="s">
         <v>245</v>
       </c>
-      <c r="E231" s="78"/>
-      <c r="F231" s="78"/>
+      <c r="E231" s="109"/>
+      <c r="F231" s="109"/>
       <c r="G231" s="41"/>
     </row>
     <row r="232" spans="1:7">
@@ -10254,11 +11611,11 @@
       <c r="C232" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D232" s="78" t="s">
+      <c r="D232" s="109" t="s">
         <v>246</v>
       </c>
-      <c r="E232" s="78"/>
-      <c r="F232" s="78"/>
+      <c r="E232" s="109"/>
+      <c r="F232" s="109"/>
       <c r="G232" s="41"/>
     </row>
     <row r="233" spans="1:7">
@@ -10271,11 +11628,11 @@
       <c r="C233" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D233" s="78" t="s">
+      <c r="D233" s="109" t="s">
         <v>247</v>
       </c>
-      <c r="E233" s="78"/>
-      <c r="F233" s="78"/>
+      <c r="E233" s="109"/>
+      <c r="F233" s="109"/>
       <c r="G233" s="41"/>
     </row>
     <row r="234" spans="1:7">
@@ -10288,11 +11645,11 @@
       <c r="C234" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D234" s="78" t="s">
+      <c r="D234" s="109" t="s">
         <v>248</v>
       </c>
-      <c r="E234" s="78"/>
-      <c r="F234" s="78"/>
+      <c r="E234" s="109"/>
+      <c r="F234" s="109"/>
       <c r="G234" s="41"/>
     </row>
     <row r="235" spans="1:7">
@@ -10305,11 +11662,11 @@
       <c r="C235" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D235" s="74" t="s">
+      <c r="D235" s="105" t="s">
         <v>64</v>
       </c>
-      <c r="E235" s="75"/>
-      <c r="F235" s="76"/>
+      <c r="E235" s="106"/>
+      <c r="F235" s="107"/>
       <c r="G235" s="43"/>
     </row>
     <row r="236" spans="1:7">
@@ -10322,11 +11679,11 @@
       <c r="C236" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D236" s="74" t="s">
+      <c r="D236" s="105" t="s">
         <v>65</v>
       </c>
-      <c r="E236" s="75"/>
-      <c r="F236" s="76"/>
+      <c r="E236" s="106"/>
+      <c r="F236" s="107"/>
       <c r="G236" s="43"/>
     </row>
     <row r="237" spans="1:7">
@@ -10339,11 +11696,11 @@
       <c r="C237" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D237" s="74" t="s">
+      <c r="D237" s="105" t="s">
         <v>69</v>
       </c>
-      <c r="E237" s="75"/>
-      <c r="F237" s="76"/>
+      <c r="E237" s="106"/>
+      <c r="F237" s="107"/>
       <c r="G237" s="43"/>
     </row>
     <row r="238" spans="1:7">
@@ -10441,33 +11798,56 @@
       <c r="C243" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="D243" s="77" t="s">
+      <c r="D243" s="108" t="s">
         <v>264</v>
       </c>
-      <c r="E243" s="77"/>
-      <c r="F243" s="77"/>
+      <c r="E243" s="108"/>
+      <c r="F243" s="108"/>
       <c r="G243" s="44"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" scale="115">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
       <selection activeCell="C4" sqref="C4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
+    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" scale="115">
       <selection activeCell="C4" sqref="C4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="51">
-    <mergeCell ref="B174:B176"/>
-    <mergeCell ref="F111:N111"/>
-    <mergeCell ref="B148:B160"/>
-    <mergeCell ref="B161:B162"/>
-    <mergeCell ref="B163:B165"/>
-    <mergeCell ref="B166:B173"/>
+    <mergeCell ref="D236:F236"/>
+    <mergeCell ref="D237:F237"/>
+    <mergeCell ref="D243:F243"/>
+    <mergeCell ref="D230:F230"/>
+    <mergeCell ref="D231:F231"/>
+    <mergeCell ref="D232:F232"/>
+    <mergeCell ref="D233:F233"/>
+    <mergeCell ref="D234:F234"/>
+    <mergeCell ref="D235:F235"/>
+    <mergeCell ref="D229:F229"/>
+    <mergeCell ref="A212:A215"/>
+    <mergeCell ref="B212:B213"/>
+    <mergeCell ref="C212:E212"/>
+    <mergeCell ref="C213:E213"/>
+    <mergeCell ref="B214:B215"/>
+    <mergeCell ref="C214:E214"/>
+    <mergeCell ref="C215:E215"/>
+    <mergeCell ref="B220:E220"/>
+    <mergeCell ref="B221:E221"/>
+    <mergeCell ref="B222:E222"/>
+    <mergeCell ref="B223:E223"/>
+    <mergeCell ref="B224:E224"/>
+    <mergeCell ref="A208:A211"/>
+    <mergeCell ref="B208:B209"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C209:E209"/>
+    <mergeCell ref="B210:B211"/>
+    <mergeCell ref="C210:E210"/>
+    <mergeCell ref="C211:E211"/>
     <mergeCell ref="B177:B178"/>
     <mergeCell ref="B179:B185"/>
     <mergeCell ref="C199:E199"/>
@@ -10484,35 +11864,12 @@
     <mergeCell ref="B206:B207"/>
     <mergeCell ref="C206:E206"/>
     <mergeCell ref="C207:E207"/>
-    <mergeCell ref="A208:A211"/>
-    <mergeCell ref="B208:B209"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C209:E209"/>
-    <mergeCell ref="B210:B211"/>
-    <mergeCell ref="C210:E210"/>
-    <mergeCell ref="C211:E211"/>
-    <mergeCell ref="D229:F229"/>
-    <mergeCell ref="A212:A215"/>
-    <mergeCell ref="B212:B213"/>
-    <mergeCell ref="C212:E212"/>
-    <mergeCell ref="C213:E213"/>
-    <mergeCell ref="B214:B215"/>
-    <mergeCell ref="C214:E214"/>
-    <mergeCell ref="C215:E215"/>
-    <mergeCell ref="B220:E220"/>
-    <mergeCell ref="B221:E221"/>
-    <mergeCell ref="B222:E222"/>
-    <mergeCell ref="B223:E223"/>
-    <mergeCell ref="B224:E224"/>
-    <mergeCell ref="D236:F236"/>
-    <mergeCell ref="D237:F237"/>
-    <mergeCell ref="D243:F243"/>
-    <mergeCell ref="D230:F230"/>
-    <mergeCell ref="D231:F231"/>
-    <mergeCell ref="D232:F232"/>
-    <mergeCell ref="D233:F233"/>
-    <mergeCell ref="D234:F234"/>
-    <mergeCell ref="D235:F235"/>
+    <mergeCell ref="B174:B176"/>
+    <mergeCell ref="F111:N111"/>
+    <mergeCell ref="B148:B160"/>
+    <mergeCell ref="B161:B162"/>
+    <mergeCell ref="B163:B165"/>
+    <mergeCell ref="B166:B173"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -10535,18 +11892,18 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
+      <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
-      <selection activeCell="E26" sqref="E26"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
i368--Apollo eit2 suite added
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/radiant/silicon_07_apollo.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/radiant/silicon_07_apollo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\update\07_Apollo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\repository\tmp_client\doc\TMP_EIT_suites\radiant\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="pSvbrBtM5D7J1tTbaFvNMFAx+gsFF1+zjWgivCK1irAkzVtGcdIaviGYDMewqTuAFCctlIpswoSn4Z8ezPPc6w==" workbookSaltValue="fuR2EkRIGc7n0eTkIKsWWA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="suite" sheetId="1" r:id="rId1"/>
@@ -27,10 +27,10 @@
   </definedNames>
   <calcPr calcId="122211"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jeffrey Ye - Personal View" guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="3"/>
+    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
+    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
     <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
-    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
-    <customWorkbookView name="Jeffrey Ye - Personal View" guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="3"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -1713,9 +1713,6 @@
     <t>ITR2/07_SoftIP/401_RAM_DP/401_RAM_DP_default_512x36_Oreg_sync</t>
   </si>
   <si>
-    <t>ITR2/07_SoftIP/402_RAM_DP_Ture/411_RAM_DP_True_default_512x18_Oreg_RSTAseertion_sync</t>
-  </si>
-  <si>
     <t>ITR2/07_SoftIP/403_RAM_DQ/421_RAM_DQ_default_512x36_Oreg_sync</t>
   </si>
   <si>
@@ -1795,6 +1792,9 @@
   </si>
   <si>
     <t>silicon_07_apollo_v1.03</t>
+  </si>
+  <si>
+    <t>ITR2/07_SoftIP/402_RAM_DP_True/411_RAM_DP_True_default_512x18_Oreg_RSTAseertion_sync</t>
   </si>
 </sst>
 </file>
@@ -3109,20 +3109,59 @@
     <xf numFmtId="49" fontId="12" fillId="7" borderId="7" xfId="13" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3130,12 +3169,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3145,13 +3178,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
@@ -3171,44 +3198,17 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="48" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -6086,7 +6086,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
@@ -6118,7 +6118,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -6126,12 +6126,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="B5" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -6402,23 +6402,23 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="G15" sqref="G15"/>
+    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" topLeftCell="A2">
+      <selection activeCell="C52" sqref="C52"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="B4" sqref="B4"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="B35" sqref="B35"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-    </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="B4" sqref="B4"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" topLeftCell="A2">
-      <selection activeCell="C52" sqref="C52"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
@@ -6433,12 +6433,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE108"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B87" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E52" sqref="E52"/>
+      <selection pane="bottomRight" activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -8571,13 +8571,13 @@
         <v>117</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>478</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="S79" s="2" t="s">
         <v>303</v>
@@ -8597,13 +8597,13 @@
         <v>117</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>482</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="S80" s="2" t="s">
         <v>303</v>
@@ -8795,7 +8795,7 @@
         <v>118</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="S89" s="2" t="s">
         <v>303</v>
@@ -8815,7 +8815,7 @@
         <v>118</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="S90" s="2" t="s">
         <v>303</v>
@@ -8835,7 +8835,7 @@
         <v>118</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="S91" s="2" t="s">
         <v>303</v>
@@ -8961,7 +8961,7 @@
     </row>
     <row r="97" spans="1:31">
       <c r="A97" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>346</v>
@@ -8984,7 +8984,7 @@
     </row>
     <row r="98" spans="1:31">
       <c r="A98" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>346</v>
@@ -9007,7 +9007,7 @@
     </row>
     <row r="99" spans="1:31">
       <c r="A99" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>346</v>
@@ -9030,7 +9030,7 @@
     </row>
     <row r="100" spans="1:31">
       <c r="A100" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>346</v>
@@ -9053,7 +9053,7 @@
     </row>
     <row r="101" spans="1:31">
       <c r="A101" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>346</v>
@@ -9076,7 +9076,7 @@
     </row>
     <row r="102" spans="1:31">
       <c r="A102" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>346</v>
@@ -9096,13 +9096,13 @@
     </row>
     <row r="103" spans="1:31">
       <c r="A103" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>346</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>548</v>
+        <v>575</v>
       </c>
       <c r="S103" s="2" t="s">
         <v>346</v>
@@ -9116,13 +9116,13 @@
     </row>
     <row r="104" spans="1:31">
       <c r="A104" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>346</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="S104" s="2" t="s">
         <v>346</v>
@@ -9136,13 +9136,13 @@
     </row>
     <row r="105" spans="1:31">
       <c r="A105" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>346</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="S105" s="2" t="s">
         <v>346</v>
@@ -9156,13 +9156,13 @@
     </row>
     <row r="106" spans="1:31">
       <c r="A106" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>346</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="S106" s="2" t="s">
         <v>346</v>
@@ -9176,13 +9176,13 @@
     </row>
     <row r="107" spans="1:31">
       <c r="A107" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>346</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="S107" s="2" t="s">
         <v>346</v>
@@ -9196,13 +9196,13 @@
     </row>
     <row r="108" spans="1:31">
       <c r="A108" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>346</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="S108" s="2" t="s">
         <v>346</v>
@@ -9352,17 +9352,17 @@
       <c r="E111" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F111" s="75" t="s">
+      <c r="F111" s="106" t="s">
         <v>87</v>
       </c>
-      <c r="G111" s="76"/>
-      <c r="H111" s="76"/>
-      <c r="I111" s="76"/>
-      <c r="J111" s="76"/>
-      <c r="K111" s="76"/>
-      <c r="L111" s="76"/>
-      <c r="M111" s="76"/>
-      <c r="N111" s="77"/>
+      <c r="G111" s="107"/>
+      <c r="H111" s="107"/>
+      <c r="I111" s="107"/>
+      <c r="J111" s="107"/>
+      <c r="K111" s="107"/>
+      <c r="L111" s="107"/>
+      <c r="M111" s="107"/>
+      <c r="N111" s="108"/>
     </row>
     <row r="112" spans="1:14">
       <c r="A112" s="11" t="s">
@@ -10252,7 +10252,7 @@
       <c r="A148" s="26">
         <v>1</v>
       </c>
-      <c r="B148" s="78" t="s">
+      <c r="B148" s="91" t="s">
         <v>3</v>
       </c>
       <c r="C148" s="27" t="s">
@@ -10278,7 +10278,7 @@
       <c r="A149" s="26">
         <v>2</v>
       </c>
-      <c r="B149" s="79"/>
+      <c r="B149" s="92"/>
       <c r="C149" s="28" t="s">
         <v>136</v>
       </c>
@@ -10300,7 +10300,7 @@
       <c r="A150" s="26">
         <v>3</v>
       </c>
-      <c r="B150" s="79"/>
+      <c r="B150" s="92"/>
       <c r="C150" s="28" t="s">
         <v>9</v>
       </c>
@@ -10320,7 +10320,7 @@
       <c r="A151" s="26">
         <v>4</v>
       </c>
-      <c r="B151" s="79"/>
+      <c r="B151" s="92"/>
       <c r="C151" s="28" t="s">
         <v>138</v>
       </c>
@@ -10344,7 +10344,7 @@
       <c r="A152" s="26">
         <v>5</v>
       </c>
-      <c r="B152" s="79"/>
+      <c r="B152" s="92"/>
       <c r="C152" s="27" t="s">
         <v>140</v>
       </c>
@@ -10368,7 +10368,7 @@
       <c r="A153" s="26">
         <v>6</v>
       </c>
-      <c r="B153" s="79"/>
+      <c r="B153" s="92"/>
       <c r="C153" s="27" t="s">
         <v>144</v>
       </c>
@@ -10392,7 +10392,7 @@
       <c r="A154" s="26">
         <v>7</v>
       </c>
-      <c r="B154" s="79"/>
+      <c r="B154" s="92"/>
       <c r="C154" s="28" t="s">
         <v>147</v>
       </c>
@@ -10414,7 +10414,7 @@
       <c r="A155" s="26">
         <v>8</v>
       </c>
-      <c r="B155" s="79"/>
+      <c r="B155" s="92"/>
       <c r="C155" s="27" t="s">
         <v>148</v>
       </c>
@@ -10438,7 +10438,7 @@
       <c r="A156" s="26">
         <v>9</v>
       </c>
-      <c r="B156" s="79"/>
+      <c r="B156" s="92"/>
       <c r="C156" s="27" t="s">
         <v>149</v>
       </c>
@@ -10462,7 +10462,7 @@
       <c r="A157" s="26">
         <v>10</v>
       </c>
-      <c r="B157" s="79"/>
+      <c r="B157" s="92"/>
       <c r="C157" s="28" t="s">
         <v>150</v>
       </c>
@@ -10486,7 +10486,7 @@
       <c r="A158" s="26">
         <v>11</v>
       </c>
-      <c r="B158" s="79"/>
+      <c r="B158" s="92"/>
       <c r="C158" s="68" t="s">
         <v>151</v>
       </c>
@@ -10510,7 +10510,7 @@
       <c r="A159" s="26">
         <v>12</v>
       </c>
-      <c r="B159" s="79"/>
+      <c r="B159" s="92"/>
       <c r="C159" s="28" t="s">
         <v>153</v>
       </c>
@@ -10532,7 +10532,7 @@
       <c r="A160" s="26">
         <v>13</v>
       </c>
-      <c r="B160" s="80"/>
+      <c r="B160" s="86"/>
       <c r="C160" s="28" t="s">
         <v>56</v>
       </c>
@@ -10556,7 +10556,7 @@
       <c r="A161" s="26">
         <v>14</v>
       </c>
-      <c r="B161" s="73" t="s">
+      <c r="B161" s="82" t="s">
         <v>4</v>
       </c>
       <c r="C161" s="28" t="s">
@@ -10582,7 +10582,7 @@
       <c r="A162" s="26">
         <v>15</v>
       </c>
-      <c r="B162" s="74"/>
+      <c r="B162" s="81"/>
       <c r="C162" s="28" t="s">
         <v>161</v>
       </c>
@@ -10606,7 +10606,7 @@
       <c r="A163" s="26">
         <v>16</v>
       </c>
-      <c r="B163" s="78" t="s">
+      <c r="B163" s="91" t="s">
         <v>5</v>
       </c>
       <c r="C163" s="28" t="s">
@@ -10630,7 +10630,7 @@
       <c r="A164" s="26">
         <v>17</v>
       </c>
-      <c r="B164" s="81"/>
+      <c r="B164" s="109"/>
       <c r="C164" s="27" t="s">
         <v>165</v>
       </c>
@@ -10652,7 +10652,7 @@
       <c r="A165" s="26">
         <v>18</v>
       </c>
-      <c r="B165" s="80"/>
+      <c r="B165" s="86"/>
       <c r="C165" s="27" t="s">
         <v>167</v>
       </c>
@@ -10672,7 +10672,7 @@
       <c r="A166" s="26">
         <v>19</v>
       </c>
-      <c r="B166" s="73" t="s">
+      <c r="B166" s="82" t="s">
         <v>6</v>
       </c>
       <c r="C166" s="28" t="s">
@@ -10696,7 +10696,7 @@
       <c r="A167" s="26">
         <v>20</v>
       </c>
-      <c r="B167" s="74"/>
+      <c r="B167" s="81"/>
       <c r="C167" s="28" t="s">
         <v>172</v>
       </c>
@@ -10716,7 +10716,7 @@
       <c r="A168" s="26">
         <v>21</v>
       </c>
-      <c r="B168" s="74"/>
+      <c r="B168" s="81"/>
       <c r="C168" s="28" t="s">
         <v>173</v>
       </c>
@@ -10736,7 +10736,7 @@
       <c r="A169" s="26">
         <v>22</v>
       </c>
-      <c r="B169" s="74"/>
+      <c r="B169" s="81"/>
       <c r="C169" s="28" t="s">
         <v>174</v>
       </c>
@@ -10756,7 +10756,7 @@
       <c r="A170" s="26">
         <v>23</v>
       </c>
-      <c r="B170" s="74"/>
+      <c r="B170" s="81"/>
       <c r="C170" s="28" t="s">
         <v>175</v>
       </c>
@@ -10776,7 +10776,7 @@
       <c r="A171" s="26">
         <v>24</v>
       </c>
-      <c r="B171" s="74"/>
+      <c r="B171" s="81"/>
       <c r="C171" s="28" t="s">
         <v>176</v>
       </c>
@@ -10796,7 +10796,7 @@
       <c r="A172" s="26">
         <v>25</v>
       </c>
-      <c r="B172" s="74"/>
+      <c r="B172" s="81"/>
       <c r="C172" s="28" t="s">
         <v>177</v>
       </c>
@@ -10816,7 +10816,7 @@
       <c r="A173" s="26">
         <v>26</v>
       </c>
-      <c r="B173" s="74"/>
+      <c r="B173" s="81"/>
       <c r="C173" s="28" t="s">
         <v>41</v>
       </c>
@@ -10836,7 +10836,7 @@
       <c r="A174" s="26">
         <v>27</v>
       </c>
-      <c r="B174" s="73" t="s">
+      <c r="B174" s="82" t="s">
         <v>7</v>
       </c>
       <c r="C174" s="28" t="s">
@@ -10860,7 +10860,7 @@
       <c r="A175" s="26">
         <v>28</v>
       </c>
-      <c r="B175" s="74"/>
+      <c r="B175" s="81"/>
       <c r="C175" s="27" t="s">
         <v>181</v>
       </c>
@@ -10882,7 +10882,7 @@
       <c r="A176" s="26">
         <v>29</v>
       </c>
-      <c r="B176" s="74"/>
+      <c r="B176" s="81"/>
       <c r="C176" s="28" t="s">
         <v>184</v>
       </c>
@@ -10904,7 +10904,7 @@
       <c r="A177" s="26">
         <v>30</v>
       </c>
-      <c r="B177" s="78" t="s">
+      <c r="B177" s="91" t="s">
         <v>8</v>
       </c>
       <c r="C177" s="28" t="s">
@@ -10930,7 +10930,7 @@
       <c r="A178" s="31">
         <v>31</v>
       </c>
-      <c r="B178" s="79"/>
+      <c r="B178" s="92"/>
       <c r="C178" s="32" t="s">
         <v>189</v>
       </c>
@@ -10954,7 +10954,7 @@
       <c r="A179" s="23">
         <v>32</v>
       </c>
-      <c r="B179" s="82" t="s">
+      <c r="B179" s="93" t="s">
         <v>191</v>
       </c>
       <c r="C179" s="33" t="s">
@@ -10978,7 +10978,7 @@
       <c r="A180" s="26">
         <v>33</v>
       </c>
-      <c r="B180" s="83"/>
+      <c r="B180" s="94"/>
       <c r="C180" s="27" t="s">
         <v>195</v>
       </c>
@@ -11000,7 +11000,7 @@
       <c r="A181" s="26">
         <v>34</v>
       </c>
-      <c r="B181" s="84"/>
+      <c r="B181" s="95"/>
       <c r="C181" s="34" t="s">
         <v>198</v>
       </c>
@@ -11022,7 +11022,7 @@
       <c r="A182" s="31">
         <v>35</v>
       </c>
-      <c r="B182" s="84"/>
+      <c r="B182" s="95"/>
       <c r="C182" s="34" t="s">
         <v>199</v>
       </c>
@@ -11044,7 +11044,7 @@
       <c r="A183" s="31">
         <v>36</v>
       </c>
-      <c r="B183" s="84"/>
+      <c r="B183" s="95"/>
       <c r="C183" s="34" t="s">
         <v>202</v>
       </c>
@@ -11064,7 +11064,7 @@
       <c r="A184" s="31">
         <v>37</v>
       </c>
-      <c r="B184" s="84"/>
+      <c r="B184" s="95"/>
       <c r="C184" s="34" t="s">
         <v>254</v>
       </c>
@@ -11086,7 +11086,7 @@
       <c r="A185" s="35">
         <v>38</v>
       </c>
-      <c r="B185" s="85"/>
+      <c r="B185" s="90"/>
       <c r="C185" s="36" t="s">
         <v>258</v>
       </c>
@@ -11137,11 +11137,11 @@
       <c r="B199" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="C199" s="86" t="s">
+      <c r="C199" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="D199" s="86"/>
-      <c r="E199" s="86"/>
+      <c r="D199" s="96"/>
+      <c r="E199" s="96"/>
       <c r="F199" s="39" t="s">
         <v>43</v>
       </c>
@@ -11150,17 +11150,17 @@
       </c>
     </row>
     <row r="200" spans="1:7">
-      <c r="A200" s="87" t="s">
+      <c r="A200" s="79" t="s">
         <v>212</v>
       </c>
-      <c r="B200" s="74" t="s">
+      <c r="B200" s="81" t="s">
         <v>213</v>
       </c>
-      <c r="C200" s="89" t="s">
+      <c r="C200" s="98" t="s">
         <v>57</v>
       </c>
-      <c r="D200" s="90"/>
-      <c r="E200" s="90"/>
+      <c r="D200" s="99"/>
+      <c r="E200" s="99"/>
       <c r="F200" s="28" t="s">
         <v>214</v>
       </c>
@@ -11169,13 +11169,13 @@
       </c>
     </row>
     <row r="201" spans="1:7">
-      <c r="A201" s="87"/>
-      <c r="B201" s="88"/>
-      <c r="C201" s="91" t="s">
+      <c r="A201" s="79"/>
+      <c r="B201" s="97"/>
+      <c r="C201" s="100" t="s">
         <v>57</v>
       </c>
-      <c r="D201" s="92"/>
-      <c r="E201" s="92"/>
+      <c r="D201" s="101"/>
+      <c r="E201" s="101"/>
       <c r="F201" s="32" t="s">
         <v>215</v>
       </c>
@@ -11184,15 +11184,15 @@
       </c>
     </row>
     <row r="202" spans="1:7">
-      <c r="A202" s="87"/>
-      <c r="B202" s="74" t="s">
+      <c r="A202" s="79"/>
+      <c r="B202" s="81" t="s">
         <v>216</v>
       </c>
-      <c r="C202" s="93" t="s">
+      <c r="C202" s="102" t="s">
         <v>217</v>
       </c>
-      <c r="D202" s="93"/>
-      <c r="E202" s="93"/>
+      <c r="D202" s="102"/>
+      <c r="E202" s="102"/>
       <c r="F202" s="28" t="s">
         <v>214</v>
       </c>
@@ -11201,13 +11201,13 @@
       </c>
     </row>
     <row r="203" spans="1:7">
-      <c r="A203" s="87"/>
-      <c r="B203" s="74"/>
-      <c r="C203" s="91" t="s">
+      <c r="A203" s="79"/>
+      <c r="B203" s="81"/>
+      <c r="C203" s="100" t="s">
         <v>217</v>
       </c>
-      <c r="D203" s="91"/>
-      <c r="E203" s="91"/>
+      <c r="D203" s="100"/>
+      <c r="E203" s="100"/>
       <c r="F203" s="28" t="s">
         <v>215</v>
       </c>
@@ -11216,15 +11216,15 @@
       </c>
     </row>
     <row r="204" spans="1:7">
-      <c r="A204" s="87"/>
-      <c r="B204" s="88" t="s">
+      <c r="A204" s="79"/>
+      <c r="B204" s="97" t="s">
         <v>218</v>
       </c>
-      <c r="C204" s="94" t="s">
+      <c r="C204" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="D204" s="95"/>
-      <c r="E204" s="96"/>
+      <c r="D204" s="104"/>
+      <c r="E204" s="105"/>
       <c r="F204" s="28" t="s">
         <v>214</v>
       </c>
@@ -11233,13 +11233,13 @@
       </c>
     </row>
     <row r="205" spans="1:7">
-      <c r="A205" s="87"/>
-      <c r="B205" s="80"/>
-      <c r="C205" s="94" t="s">
+      <c r="A205" s="79"/>
+      <c r="B205" s="86"/>
+      <c r="C205" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="D205" s="95"/>
-      <c r="E205" s="96"/>
+      <c r="D205" s="104"/>
+      <c r="E205" s="105"/>
       <c r="F205" s="28" t="s">
         <v>215</v>
       </c>
@@ -11248,15 +11248,15 @@
       </c>
     </row>
     <row r="206" spans="1:7">
-      <c r="A206" s="87"/>
-      <c r="B206" s="74" t="s">
+      <c r="A206" s="79"/>
+      <c r="B206" s="81" t="s">
         <v>219</v>
       </c>
-      <c r="C206" s="93" t="s">
+      <c r="C206" s="102" t="s">
         <v>220</v>
       </c>
-      <c r="D206" s="93"/>
-      <c r="E206" s="93"/>
+      <c r="D206" s="102"/>
+      <c r="E206" s="102"/>
       <c r="F206" s="28" t="s">
         <v>214</v>
       </c>
@@ -11265,13 +11265,13 @@
       </c>
     </row>
     <row r="207" spans="1:7">
-      <c r="A207" s="87"/>
-      <c r="B207" s="74"/>
-      <c r="C207" s="93" t="s">
+      <c r="A207" s="79"/>
+      <c r="B207" s="81"/>
+      <c r="C207" s="102" t="s">
         <v>220</v>
       </c>
-      <c r="D207" s="93"/>
-      <c r="E207" s="93"/>
+      <c r="D207" s="102"/>
+      <c r="E207" s="102"/>
       <c r="F207" s="28" t="s">
         <v>215</v>
       </c>
@@ -11280,17 +11280,17 @@
       </c>
     </row>
     <row r="208" spans="1:7">
-      <c r="A208" s="87" t="s">
+      <c r="A208" s="79" t="s">
         <v>221</v>
       </c>
-      <c r="B208" s="74" t="s">
+      <c r="B208" s="81" t="s">
         <v>222</v>
       </c>
-      <c r="C208" s="73" t="s">
+      <c r="C208" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="D208" s="74"/>
-      <c r="E208" s="74"/>
+      <c r="D208" s="81"/>
+      <c r="E208" s="81"/>
       <c r="F208" s="28" t="s">
         <v>214</v>
       </c>
@@ -11299,13 +11299,13 @@
       </c>
     </row>
     <row r="209" spans="1:7">
-      <c r="A209" s="87"/>
-      <c r="B209" s="74"/>
-      <c r="C209" s="74" t="s">
+      <c r="A209" s="79"/>
+      <c r="B209" s="81"/>
+      <c r="C209" s="81" t="s">
         <v>46</v>
       </c>
-      <c r="D209" s="74"/>
-      <c r="E209" s="74"/>
+      <c r="D209" s="81"/>
+      <c r="E209" s="81"/>
       <c r="F209" s="28" t="s">
         <v>215</v>
       </c>
@@ -11314,15 +11314,15 @@
       </c>
     </row>
     <row r="210" spans="1:7">
-      <c r="A210" s="87"/>
-      <c r="B210" s="74" t="s">
+      <c r="A210" s="79"/>
+      <c r="B210" s="81" t="s">
         <v>224</v>
       </c>
-      <c r="C210" s="73" t="s">
+      <c r="C210" s="82" t="s">
         <v>47</v>
       </c>
-      <c r="D210" s="74"/>
-      <c r="E210" s="74"/>
+      <c r="D210" s="81"/>
+      <c r="E210" s="81"/>
       <c r="F210" s="28" t="s">
         <v>214</v>
       </c>
@@ -11331,13 +11331,13 @@
       </c>
     </row>
     <row r="211" spans="1:7">
-      <c r="A211" s="87"/>
-      <c r="B211" s="74"/>
-      <c r="C211" s="74" t="s">
+      <c r="A211" s="79"/>
+      <c r="B211" s="81"/>
+      <c r="C211" s="81" t="s">
         <v>48</v>
       </c>
-      <c r="D211" s="74"/>
-      <c r="E211" s="74"/>
+      <c r="D211" s="81"/>
+      <c r="E211" s="81"/>
       <c r="F211" s="28" t="s">
         <v>215</v>
       </c>
@@ -11346,17 +11346,17 @@
       </c>
     </row>
     <row r="212" spans="1:7">
-      <c r="A212" s="87" t="s">
+      <c r="A212" s="79" t="s">
         <v>225</v>
       </c>
-      <c r="B212" s="74" t="s">
+      <c r="B212" s="81" t="s">
         <v>226</v>
       </c>
-      <c r="C212" s="73" t="s">
+      <c r="C212" s="82" t="s">
         <v>49</v>
       </c>
-      <c r="D212" s="74"/>
-      <c r="E212" s="74"/>
+      <c r="D212" s="81"/>
+      <c r="E212" s="81"/>
       <c r="F212" s="28" t="s">
         <v>214</v>
       </c>
@@ -11365,13 +11365,13 @@
       </c>
     </row>
     <row r="213" spans="1:7">
-      <c r="A213" s="87"/>
-      <c r="B213" s="74"/>
-      <c r="C213" s="74" t="s">
+      <c r="A213" s="79"/>
+      <c r="B213" s="81"/>
+      <c r="C213" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="D213" s="74"/>
-      <c r="E213" s="74"/>
+      <c r="D213" s="81"/>
+      <c r="E213" s="81"/>
       <c r="F213" s="28" t="s">
         <v>215</v>
       </c>
@@ -11380,15 +11380,15 @@
       </c>
     </row>
     <row r="214" spans="1:7">
-      <c r="A214" s="87"/>
-      <c r="B214" s="74" t="s">
+      <c r="A214" s="79"/>
+      <c r="B214" s="81" t="s">
         <v>227</v>
       </c>
-      <c r="C214" s="73" t="s">
+      <c r="C214" s="82" t="s">
         <v>228</v>
       </c>
-      <c r="D214" s="74"/>
-      <c r="E214" s="74"/>
+      <c r="D214" s="81"/>
+      <c r="E214" s="81"/>
       <c r="F214" s="28" t="s">
         <v>214</v>
       </c>
@@ -11397,13 +11397,13 @@
       </c>
     </row>
     <row r="215" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A215" s="98"/>
-      <c r="B215" s="99"/>
-      <c r="C215" s="99" t="s">
+      <c r="A215" s="80"/>
+      <c r="B215" s="83"/>
+      <c r="C215" s="83" t="s">
         <v>229</v>
       </c>
-      <c r="D215" s="99"/>
-      <c r="E215" s="99"/>
+      <c r="D215" s="83"/>
+      <c r="E215" s="83"/>
       <c r="F215" s="36" t="s">
         <v>215</v>
       </c>
@@ -11442,12 +11442,12 @@
       <c r="A220" s="45" t="s">
         <v>232</v>
       </c>
-      <c r="B220" s="100" t="s">
+      <c r="B220" s="84" t="s">
         <v>52</v>
       </c>
-      <c r="C220" s="100"/>
-      <c r="D220" s="100"/>
-      <c r="E220" s="100"/>
+      <c r="C220" s="84"/>
+      <c r="D220" s="84"/>
+      <c r="E220" s="84"/>
       <c r="F220" s="46" t="s">
         <v>233</v>
       </c>
@@ -11459,12 +11459,12 @@
       <c r="A221" s="48" t="s">
         <v>235</v>
       </c>
-      <c r="B221" s="101" t="s">
+      <c r="B221" s="85" t="s">
         <v>236</v>
       </c>
-      <c r="C221" s="80"/>
-      <c r="D221" s="80"/>
-      <c r="E221" s="80"/>
+      <c r="C221" s="86"/>
+      <c r="D221" s="86"/>
+      <c r="E221" s="86"/>
       <c r="F221" s="49" t="s">
         <v>111</v>
       </c>
@@ -11476,12 +11476,12 @@
       <c r="A222" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="B222" s="102" t="s">
+      <c r="B222" s="87" t="s">
         <v>238</v>
       </c>
-      <c r="C222" s="103"/>
-      <c r="D222" s="103"/>
-      <c r="E222" s="104"/>
+      <c r="C222" s="88"/>
+      <c r="D222" s="88"/>
+      <c r="E222" s="89"/>
       <c r="F222" s="15" t="s">
         <v>63</v>
       </c>
@@ -11493,12 +11493,12 @@
       <c r="A223" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B223" s="102" t="s">
+      <c r="B223" s="87" t="s">
         <v>239</v>
       </c>
-      <c r="C223" s="103"/>
-      <c r="D223" s="103"/>
-      <c r="E223" s="104"/>
+      <c r="C223" s="88"/>
+      <c r="D223" s="88"/>
+      <c r="E223" s="89"/>
       <c r="F223" s="18" t="s">
         <v>63</v>
       </c>
@@ -11510,12 +11510,12 @@
       <c r="A224" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="B224" s="85" t="s">
+      <c r="B224" s="90" t="s">
         <v>241</v>
       </c>
-      <c r="C224" s="99"/>
-      <c r="D224" s="99"/>
-      <c r="E224" s="99"/>
+      <c r="C224" s="83"/>
+      <c r="D224" s="83"/>
+      <c r="E224" s="83"/>
       <c r="F224" s="21" t="s">
         <v>63</v>
       </c>
@@ -11560,11 +11560,11 @@
       <c r="C229" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D229" s="97" t="s">
+      <c r="D229" s="78" t="s">
         <v>54</v>
       </c>
-      <c r="E229" s="97"/>
-      <c r="F229" s="97"/>
+      <c r="E229" s="78"/>
+      <c r="F229" s="78"/>
       <c r="G229" s="57"/>
     </row>
     <row r="230" spans="1:7">
@@ -11577,11 +11577,11 @@
       <c r="C230" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D230" s="109" t="s">
+      <c r="D230" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="E230" s="109"/>
-      <c r="F230" s="109"/>
+      <c r="E230" s="77"/>
+      <c r="F230" s="77"/>
       <c r="G230" s="41"/>
     </row>
     <row r="231" spans="1:7">
@@ -11594,11 +11594,11 @@
       <c r="C231" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D231" s="109" t="s">
+      <c r="D231" s="77" t="s">
         <v>245</v>
       </c>
-      <c r="E231" s="109"/>
-      <c r="F231" s="109"/>
+      <c r="E231" s="77"/>
+      <c r="F231" s="77"/>
       <c r="G231" s="41"/>
     </row>
     <row r="232" spans="1:7">
@@ -11611,11 +11611,11 @@
       <c r="C232" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D232" s="109" t="s">
+      <c r="D232" s="77" t="s">
         <v>246</v>
       </c>
-      <c r="E232" s="109"/>
-      <c r="F232" s="109"/>
+      <c r="E232" s="77"/>
+      <c r="F232" s="77"/>
       <c r="G232" s="41"/>
     </row>
     <row r="233" spans="1:7">
@@ -11628,11 +11628,11 @@
       <c r="C233" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D233" s="109" t="s">
+      <c r="D233" s="77" t="s">
         <v>247</v>
       </c>
-      <c r="E233" s="109"/>
-      <c r="F233" s="109"/>
+      <c r="E233" s="77"/>
+      <c r="F233" s="77"/>
       <c r="G233" s="41"/>
     </row>
     <row r="234" spans="1:7">
@@ -11645,11 +11645,11 @@
       <c r="C234" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D234" s="109" t="s">
+      <c r="D234" s="77" t="s">
         <v>248</v>
       </c>
-      <c r="E234" s="109"/>
-      <c r="F234" s="109"/>
+      <c r="E234" s="77"/>
+      <c r="F234" s="77"/>
       <c r="G234" s="41"/>
     </row>
     <row r="235" spans="1:7">
@@ -11662,11 +11662,11 @@
       <c r="C235" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D235" s="105" t="s">
+      <c r="D235" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="E235" s="106"/>
-      <c r="F235" s="107"/>
+      <c r="E235" s="74"/>
+      <c r="F235" s="75"/>
       <c r="G235" s="43"/>
     </row>
     <row r="236" spans="1:7">
@@ -11679,11 +11679,11 @@
       <c r="C236" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D236" s="105" t="s">
+      <c r="D236" s="73" t="s">
         <v>65</v>
       </c>
-      <c r="E236" s="106"/>
-      <c r="F236" s="107"/>
+      <c r="E236" s="74"/>
+      <c r="F236" s="75"/>
       <c r="G236" s="43"/>
     </row>
     <row r="237" spans="1:7">
@@ -11696,11 +11696,11 @@
       <c r="C237" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D237" s="105" t="s">
+      <c r="D237" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="E237" s="106"/>
-      <c r="F237" s="107"/>
+      <c r="E237" s="74"/>
+      <c r="F237" s="75"/>
       <c r="G237" s="43"/>
     </row>
     <row r="238" spans="1:7">
@@ -11798,56 +11798,33 @@
       <c r="C243" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="D243" s="108" t="s">
+      <c r="D243" s="76" t="s">
         <v>264</v>
       </c>
-      <c r="E243" s="108"/>
-      <c r="F243" s="108"/>
+      <c r="E243" s="76"/>
+      <c r="F243" s="76"/>
       <c r="G243" s="44"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
+    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" scale="115">
       <selection activeCell="C4" sqref="C4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" scale="115">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
       <selection activeCell="C4" sqref="C4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="51">
-    <mergeCell ref="D236:F236"/>
-    <mergeCell ref="D237:F237"/>
-    <mergeCell ref="D243:F243"/>
-    <mergeCell ref="D230:F230"/>
-    <mergeCell ref="D231:F231"/>
-    <mergeCell ref="D232:F232"/>
-    <mergeCell ref="D233:F233"/>
-    <mergeCell ref="D234:F234"/>
-    <mergeCell ref="D235:F235"/>
-    <mergeCell ref="D229:F229"/>
-    <mergeCell ref="A212:A215"/>
-    <mergeCell ref="B212:B213"/>
-    <mergeCell ref="C212:E212"/>
-    <mergeCell ref="C213:E213"/>
-    <mergeCell ref="B214:B215"/>
-    <mergeCell ref="C214:E214"/>
-    <mergeCell ref="C215:E215"/>
-    <mergeCell ref="B220:E220"/>
-    <mergeCell ref="B221:E221"/>
-    <mergeCell ref="B222:E222"/>
-    <mergeCell ref="B223:E223"/>
-    <mergeCell ref="B224:E224"/>
-    <mergeCell ref="A208:A211"/>
-    <mergeCell ref="B208:B209"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C209:E209"/>
-    <mergeCell ref="B210:B211"/>
-    <mergeCell ref="C210:E210"/>
-    <mergeCell ref="C211:E211"/>
+    <mergeCell ref="B174:B176"/>
+    <mergeCell ref="F111:N111"/>
+    <mergeCell ref="B148:B160"/>
+    <mergeCell ref="B161:B162"/>
+    <mergeCell ref="B163:B165"/>
+    <mergeCell ref="B166:B173"/>
     <mergeCell ref="B177:B178"/>
     <mergeCell ref="B179:B185"/>
     <mergeCell ref="C199:E199"/>
@@ -11864,12 +11841,35 @@
     <mergeCell ref="B206:B207"/>
     <mergeCell ref="C206:E206"/>
     <mergeCell ref="C207:E207"/>
-    <mergeCell ref="B174:B176"/>
-    <mergeCell ref="F111:N111"/>
-    <mergeCell ref="B148:B160"/>
-    <mergeCell ref="B161:B162"/>
-    <mergeCell ref="B163:B165"/>
-    <mergeCell ref="B166:B173"/>
+    <mergeCell ref="A208:A211"/>
+    <mergeCell ref="B208:B209"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C209:E209"/>
+    <mergeCell ref="B210:B211"/>
+    <mergeCell ref="C210:E210"/>
+    <mergeCell ref="C211:E211"/>
+    <mergeCell ref="D229:F229"/>
+    <mergeCell ref="A212:A215"/>
+    <mergeCell ref="B212:B213"/>
+    <mergeCell ref="C212:E212"/>
+    <mergeCell ref="C213:E213"/>
+    <mergeCell ref="B214:B215"/>
+    <mergeCell ref="C214:E214"/>
+    <mergeCell ref="C215:E215"/>
+    <mergeCell ref="B220:E220"/>
+    <mergeCell ref="B221:E221"/>
+    <mergeCell ref="B222:E222"/>
+    <mergeCell ref="B223:E223"/>
+    <mergeCell ref="B224:E224"/>
+    <mergeCell ref="D236:F236"/>
+    <mergeCell ref="D237:F237"/>
+    <mergeCell ref="D243:F243"/>
+    <mergeCell ref="D230:F230"/>
+    <mergeCell ref="D231:F231"/>
+    <mergeCell ref="D232:F232"/>
+    <mergeCell ref="D233:F233"/>
+    <mergeCell ref="D234:F234"/>
+    <mergeCell ref="D235:F235"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -11892,18 +11892,18 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="E26" sqref="E26"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
i402--Apollo EIT2 suite update
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/radiant/silicon_07_apollo.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/radiant/silicon_07_apollo.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="pSvbrBtM5D7J1tTbaFvNMFAx+gsFF1+zjWgivCK1irAkzVtGcdIaviGYDMewqTuAFCctlIpswoSn4Z8ezPPc6w==" workbookSaltValue="fuR2EkRIGc7n0eTkIKsWWA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="suite" sheetId="1" r:id="rId1"/>
@@ -27,10 +27,10 @@
   </definedNames>
   <calcPr calcId="122211"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
+    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
     <customWorkbookView name="Jeffrey Ye - Personal View" guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="3"/>
-    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
-    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
-    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -1785,16 +1785,16 @@
     <t>MULTADDSBU18X18A cell model</t>
   </si>
   <si>
-    <t>suite_path = 07_Apollo</t>
-  </si>
-  <si>
     <t>repository = http://lsh-tmp/radiant/trunk/silicon</t>
   </si>
   <si>
-    <t>silicon_07_apollo_v1.03</t>
-  </si>
-  <si>
     <t>ITR2/07_SoftIP/402_RAM_DP_True/411_RAM_DP_True_default_512x18_Oreg_RSTAseertion_sync</t>
+  </si>
+  <si>
+    <t>silicon_07_apollo_v1.04</t>
+  </si>
+  <si>
+    <t>suite_path = 07_Apollo;timeout=7200;est_mem = 8</t>
   </si>
 </sst>
 </file>
@@ -3109,76 +3109,49 @@
     <xf numFmtId="49" fontId="12" fillId="7" borderId="7" xfId="13" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
@@ -3198,17 +3171,44 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="48" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -6086,9 +6086,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -6126,12 +6124,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="B5" s="2" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -6402,23 +6400,23 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
-    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" topLeftCell="A2">
-      <selection activeCell="C52" sqref="C52"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
+      <selection activeCell="B35" sqref="B35"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
       <selection activeCell="B4" sqref="B4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-    </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
-      <selection activeCell="B35" sqref="B35"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="G15" sqref="G15"/>
+    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" topLeftCell="A2">
+      <selection activeCell="C52" sqref="C52"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
@@ -6433,8 +6431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE108"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B87" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -9102,7 +9100,7 @@
         <v>346</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="S103" s="2" t="s">
         <v>346</v>
@@ -9352,17 +9350,17 @@
       <c r="E111" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F111" s="106" t="s">
+      <c r="F111" s="75" t="s">
         <v>87</v>
       </c>
-      <c r="G111" s="107"/>
-      <c r="H111" s="107"/>
-      <c r="I111" s="107"/>
-      <c r="J111" s="107"/>
-      <c r="K111" s="107"/>
-      <c r="L111" s="107"/>
-      <c r="M111" s="107"/>
-      <c r="N111" s="108"/>
+      <c r="G111" s="76"/>
+      <c r="H111" s="76"/>
+      <c r="I111" s="76"/>
+      <c r="J111" s="76"/>
+      <c r="K111" s="76"/>
+      <c r="L111" s="76"/>
+      <c r="M111" s="76"/>
+      <c r="N111" s="77"/>
     </row>
     <row r="112" spans="1:14">
       <c r="A112" s="11" t="s">
@@ -10252,7 +10250,7 @@
       <c r="A148" s="26">
         <v>1</v>
       </c>
-      <c r="B148" s="91" t="s">
+      <c r="B148" s="78" t="s">
         <v>3</v>
       </c>
       <c r="C148" s="27" t="s">
@@ -10278,7 +10276,7 @@
       <c r="A149" s="26">
         <v>2</v>
       </c>
-      <c r="B149" s="92"/>
+      <c r="B149" s="79"/>
       <c r="C149" s="28" t="s">
         <v>136</v>
       </c>
@@ -10300,7 +10298,7 @@
       <c r="A150" s="26">
         <v>3</v>
       </c>
-      <c r="B150" s="92"/>
+      <c r="B150" s="79"/>
       <c r="C150" s="28" t="s">
         <v>9</v>
       </c>
@@ -10320,7 +10318,7 @@
       <c r="A151" s="26">
         <v>4</v>
       </c>
-      <c r="B151" s="92"/>
+      <c r="B151" s="79"/>
       <c r="C151" s="28" t="s">
         <v>138</v>
       </c>
@@ -10344,7 +10342,7 @@
       <c r="A152" s="26">
         <v>5</v>
       </c>
-      <c r="B152" s="92"/>
+      <c r="B152" s="79"/>
       <c r="C152" s="27" t="s">
         <v>140</v>
       </c>
@@ -10368,7 +10366,7 @@
       <c r="A153" s="26">
         <v>6</v>
       </c>
-      <c r="B153" s="92"/>
+      <c r="B153" s="79"/>
       <c r="C153" s="27" t="s">
         <v>144</v>
       </c>
@@ -10392,7 +10390,7 @@
       <c r="A154" s="26">
         <v>7</v>
       </c>
-      <c r="B154" s="92"/>
+      <c r="B154" s="79"/>
       <c r="C154" s="28" t="s">
         <v>147</v>
       </c>
@@ -10414,7 +10412,7 @@
       <c r="A155" s="26">
         <v>8</v>
       </c>
-      <c r="B155" s="92"/>
+      <c r="B155" s="79"/>
       <c r="C155" s="27" t="s">
         <v>148</v>
       </c>
@@ -10438,7 +10436,7 @@
       <c r="A156" s="26">
         <v>9</v>
       </c>
-      <c r="B156" s="92"/>
+      <c r="B156" s="79"/>
       <c r="C156" s="27" t="s">
         <v>149</v>
       </c>
@@ -10462,7 +10460,7 @@
       <c r="A157" s="26">
         <v>10</v>
       </c>
-      <c r="B157" s="92"/>
+      <c r="B157" s="79"/>
       <c r="C157" s="28" t="s">
         <v>150</v>
       </c>
@@ -10486,7 +10484,7 @@
       <c r="A158" s="26">
         <v>11</v>
       </c>
-      <c r="B158" s="92"/>
+      <c r="B158" s="79"/>
       <c r="C158" s="68" t="s">
         <v>151</v>
       </c>
@@ -10510,7 +10508,7 @@
       <c r="A159" s="26">
         <v>12</v>
       </c>
-      <c r="B159" s="92"/>
+      <c r="B159" s="79"/>
       <c r="C159" s="28" t="s">
         <v>153</v>
       </c>
@@ -10532,7 +10530,7 @@
       <c r="A160" s="26">
         <v>13</v>
       </c>
-      <c r="B160" s="86"/>
+      <c r="B160" s="80"/>
       <c r="C160" s="28" t="s">
         <v>56</v>
       </c>
@@ -10556,7 +10554,7 @@
       <c r="A161" s="26">
         <v>14</v>
       </c>
-      <c r="B161" s="82" t="s">
+      <c r="B161" s="73" t="s">
         <v>4</v>
       </c>
       <c r="C161" s="28" t="s">
@@ -10582,7 +10580,7 @@
       <c r="A162" s="26">
         <v>15</v>
       </c>
-      <c r="B162" s="81"/>
+      <c r="B162" s="74"/>
       <c r="C162" s="28" t="s">
         <v>161</v>
       </c>
@@ -10606,7 +10604,7 @@
       <c r="A163" s="26">
         <v>16</v>
       </c>
-      <c r="B163" s="91" t="s">
+      <c r="B163" s="78" t="s">
         <v>5</v>
       </c>
       <c r="C163" s="28" t="s">
@@ -10630,7 +10628,7 @@
       <c r="A164" s="26">
         <v>17</v>
       </c>
-      <c r="B164" s="109"/>
+      <c r="B164" s="81"/>
       <c r="C164" s="27" t="s">
         <v>165</v>
       </c>
@@ -10652,7 +10650,7 @@
       <c r="A165" s="26">
         <v>18</v>
       </c>
-      <c r="B165" s="86"/>
+      <c r="B165" s="80"/>
       <c r="C165" s="27" t="s">
         <v>167</v>
       </c>
@@ -10672,7 +10670,7 @@
       <c r="A166" s="26">
         <v>19</v>
       </c>
-      <c r="B166" s="82" t="s">
+      <c r="B166" s="73" t="s">
         <v>6</v>
       </c>
       <c r="C166" s="28" t="s">
@@ -10696,7 +10694,7 @@
       <c r="A167" s="26">
         <v>20</v>
       </c>
-      <c r="B167" s="81"/>
+      <c r="B167" s="74"/>
       <c r="C167" s="28" t="s">
         <v>172</v>
       </c>
@@ -10716,7 +10714,7 @@
       <c r="A168" s="26">
         <v>21</v>
       </c>
-      <c r="B168" s="81"/>
+      <c r="B168" s="74"/>
       <c r="C168" s="28" t="s">
         <v>173</v>
       </c>
@@ -10736,7 +10734,7 @@
       <c r="A169" s="26">
         <v>22</v>
       </c>
-      <c r="B169" s="81"/>
+      <c r="B169" s="74"/>
       <c r="C169" s="28" t="s">
         <v>174</v>
       </c>
@@ -10756,7 +10754,7 @@
       <c r="A170" s="26">
         <v>23</v>
       </c>
-      <c r="B170" s="81"/>
+      <c r="B170" s="74"/>
       <c r="C170" s="28" t="s">
         <v>175</v>
       </c>
@@ -10776,7 +10774,7 @@
       <c r="A171" s="26">
         <v>24</v>
       </c>
-      <c r="B171" s="81"/>
+      <c r="B171" s="74"/>
       <c r="C171" s="28" t="s">
         <v>176</v>
       </c>
@@ -10796,7 +10794,7 @@
       <c r="A172" s="26">
         <v>25</v>
       </c>
-      <c r="B172" s="81"/>
+      <c r="B172" s="74"/>
       <c r="C172" s="28" t="s">
         <v>177</v>
       </c>
@@ -10816,7 +10814,7 @@
       <c r="A173" s="26">
         <v>26</v>
       </c>
-      <c r="B173" s="81"/>
+      <c r="B173" s="74"/>
       <c r="C173" s="28" t="s">
         <v>41</v>
       </c>
@@ -10836,7 +10834,7 @@
       <c r="A174" s="26">
         <v>27</v>
       </c>
-      <c r="B174" s="82" t="s">
+      <c r="B174" s="73" t="s">
         <v>7</v>
       </c>
       <c r="C174" s="28" t="s">
@@ -10860,7 +10858,7 @@
       <c r="A175" s="26">
         <v>28</v>
       </c>
-      <c r="B175" s="81"/>
+      <c r="B175" s="74"/>
       <c r="C175" s="27" t="s">
         <v>181</v>
       </c>
@@ -10882,7 +10880,7 @@
       <c r="A176" s="26">
         <v>29</v>
       </c>
-      <c r="B176" s="81"/>
+      <c r="B176" s="74"/>
       <c r="C176" s="28" t="s">
         <v>184</v>
       </c>
@@ -10904,7 +10902,7 @@
       <c r="A177" s="26">
         <v>30</v>
       </c>
-      <c r="B177" s="91" t="s">
+      <c r="B177" s="78" t="s">
         <v>8</v>
       </c>
       <c r="C177" s="28" t="s">
@@ -10930,7 +10928,7 @@
       <c r="A178" s="31">
         <v>31</v>
       </c>
-      <c r="B178" s="92"/>
+      <c r="B178" s="79"/>
       <c r="C178" s="32" t="s">
         <v>189</v>
       </c>
@@ -10954,7 +10952,7 @@
       <c r="A179" s="23">
         <v>32</v>
       </c>
-      <c r="B179" s="93" t="s">
+      <c r="B179" s="82" t="s">
         <v>191</v>
       </c>
       <c r="C179" s="33" t="s">
@@ -10978,7 +10976,7 @@
       <c r="A180" s="26">
         <v>33</v>
       </c>
-      <c r="B180" s="94"/>
+      <c r="B180" s="83"/>
       <c r="C180" s="27" t="s">
         <v>195</v>
       </c>
@@ -11000,7 +10998,7 @@
       <c r="A181" s="26">
         <v>34</v>
       </c>
-      <c r="B181" s="95"/>
+      <c r="B181" s="84"/>
       <c r="C181" s="34" t="s">
         <v>198</v>
       </c>
@@ -11022,7 +11020,7 @@
       <c r="A182" s="31">
         <v>35</v>
       </c>
-      <c r="B182" s="95"/>
+      <c r="B182" s="84"/>
       <c r="C182" s="34" t="s">
         <v>199</v>
       </c>
@@ -11044,7 +11042,7 @@
       <c r="A183" s="31">
         <v>36</v>
       </c>
-      <c r="B183" s="95"/>
+      <c r="B183" s="84"/>
       <c r="C183" s="34" t="s">
         <v>202</v>
       </c>
@@ -11064,7 +11062,7 @@
       <c r="A184" s="31">
         <v>37</v>
       </c>
-      <c r="B184" s="95"/>
+      <c r="B184" s="84"/>
       <c r="C184" s="34" t="s">
         <v>254</v>
       </c>
@@ -11086,7 +11084,7 @@
       <c r="A185" s="35">
         <v>38</v>
       </c>
-      <c r="B185" s="90"/>
+      <c r="B185" s="85"/>
       <c r="C185" s="36" t="s">
         <v>258</v>
       </c>
@@ -11137,11 +11135,11 @@
       <c r="B199" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="C199" s="96" t="s">
+      <c r="C199" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="D199" s="96"/>
-      <c r="E199" s="96"/>
+      <c r="D199" s="86"/>
+      <c r="E199" s="86"/>
       <c r="F199" s="39" t="s">
         <v>43</v>
       </c>
@@ -11150,17 +11148,17 @@
       </c>
     </row>
     <row r="200" spans="1:7">
-      <c r="A200" s="79" t="s">
+      <c r="A200" s="87" t="s">
         <v>212</v>
       </c>
-      <c r="B200" s="81" t="s">
+      <c r="B200" s="74" t="s">
         <v>213</v>
       </c>
-      <c r="C200" s="98" t="s">
+      <c r="C200" s="89" t="s">
         <v>57</v>
       </c>
-      <c r="D200" s="99"/>
-      <c r="E200" s="99"/>
+      <c r="D200" s="90"/>
+      <c r="E200" s="90"/>
       <c r="F200" s="28" t="s">
         <v>214</v>
       </c>
@@ -11169,13 +11167,13 @@
       </c>
     </row>
     <row r="201" spans="1:7">
-      <c r="A201" s="79"/>
-      <c r="B201" s="97"/>
-      <c r="C201" s="100" t="s">
+      <c r="A201" s="87"/>
+      <c r="B201" s="88"/>
+      <c r="C201" s="91" t="s">
         <v>57</v>
       </c>
-      <c r="D201" s="101"/>
-      <c r="E201" s="101"/>
+      <c r="D201" s="92"/>
+      <c r="E201" s="92"/>
       <c r="F201" s="32" t="s">
         <v>215</v>
       </c>
@@ -11184,15 +11182,15 @@
       </c>
     </row>
     <row r="202" spans="1:7">
-      <c r="A202" s="79"/>
-      <c r="B202" s="81" t="s">
+      <c r="A202" s="87"/>
+      <c r="B202" s="74" t="s">
         <v>216</v>
       </c>
-      <c r="C202" s="102" t="s">
+      <c r="C202" s="93" t="s">
         <v>217</v>
       </c>
-      <c r="D202" s="102"/>
-      <c r="E202" s="102"/>
+      <c r="D202" s="93"/>
+      <c r="E202" s="93"/>
       <c r="F202" s="28" t="s">
         <v>214</v>
       </c>
@@ -11201,13 +11199,13 @@
       </c>
     </row>
     <row r="203" spans="1:7">
-      <c r="A203" s="79"/>
-      <c r="B203" s="81"/>
-      <c r="C203" s="100" t="s">
+      <c r="A203" s="87"/>
+      <c r="B203" s="74"/>
+      <c r="C203" s="91" t="s">
         <v>217</v>
       </c>
-      <c r="D203" s="100"/>
-      <c r="E203" s="100"/>
+      <c r="D203" s="91"/>
+      <c r="E203" s="91"/>
       <c r="F203" s="28" t="s">
         <v>215</v>
       </c>
@@ -11216,15 +11214,15 @@
       </c>
     </row>
     <row r="204" spans="1:7">
-      <c r="A204" s="79"/>
-      <c r="B204" s="97" t="s">
+      <c r="A204" s="87"/>
+      <c r="B204" s="88" t="s">
         <v>218</v>
       </c>
-      <c r="C204" s="103" t="s">
+      <c r="C204" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="D204" s="104"/>
-      <c r="E204" s="105"/>
+      <c r="D204" s="95"/>
+      <c r="E204" s="96"/>
       <c r="F204" s="28" t="s">
         <v>214</v>
       </c>
@@ -11233,13 +11231,13 @@
       </c>
     </row>
     <row r="205" spans="1:7">
-      <c r="A205" s="79"/>
-      <c r="B205" s="86"/>
-      <c r="C205" s="103" t="s">
+      <c r="A205" s="87"/>
+      <c r="B205" s="80"/>
+      <c r="C205" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="D205" s="104"/>
-      <c r="E205" s="105"/>
+      <c r="D205" s="95"/>
+      <c r="E205" s="96"/>
       <c r="F205" s="28" t="s">
         <v>215</v>
       </c>
@@ -11248,15 +11246,15 @@
       </c>
     </row>
     <row r="206" spans="1:7">
-      <c r="A206" s="79"/>
-      <c r="B206" s="81" t="s">
+      <c r="A206" s="87"/>
+      <c r="B206" s="74" t="s">
         <v>219</v>
       </c>
-      <c r="C206" s="102" t="s">
+      <c r="C206" s="93" t="s">
         <v>220</v>
       </c>
-      <c r="D206" s="102"/>
-      <c r="E206" s="102"/>
+      <c r="D206" s="93"/>
+      <c r="E206" s="93"/>
       <c r="F206" s="28" t="s">
         <v>214</v>
       </c>
@@ -11265,13 +11263,13 @@
       </c>
     </row>
     <row r="207" spans="1:7">
-      <c r="A207" s="79"/>
-      <c r="B207" s="81"/>
-      <c r="C207" s="102" t="s">
+      <c r="A207" s="87"/>
+      <c r="B207" s="74"/>
+      <c r="C207" s="93" t="s">
         <v>220</v>
       </c>
-      <c r="D207" s="102"/>
-      <c r="E207" s="102"/>
+      <c r="D207" s="93"/>
+      <c r="E207" s="93"/>
       <c r="F207" s="28" t="s">
         <v>215</v>
       </c>
@@ -11280,17 +11278,17 @@
       </c>
     </row>
     <row r="208" spans="1:7">
-      <c r="A208" s="79" t="s">
+      <c r="A208" s="87" t="s">
         <v>221</v>
       </c>
-      <c r="B208" s="81" t="s">
+      <c r="B208" s="74" t="s">
         <v>222</v>
       </c>
-      <c r="C208" s="82" t="s">
+      <c r="C208" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="D208" s="81"/>
-      <c r="E208" s="81"/>
+      <c r="D208" s="74"/>
+      <c r="E208" s="74"/>
       <c r="F208" s="28" t="s">
         <v>214</v>
       </c>
@@ -11299,13 +11297,13 @@
       </c>
     </row>
     <row r="209" spans="1:7">
-      <c r="A209" s="79"/>
-      <c r="B209" s="81"/>
-      <c r="C209" s="81" t="s">
+      <c r="A209" s="87"/>
+      <c r="B209" s="74"/>
+      <c r="C209" s="74" t="s">
         <v>46</v>
       </c>
-      <c r="D209" s="81"/>
-      <c r="E209" s="81"/>
+      <c r="D209" s="74"/>
+      <c r="E209" s="74"/>
       <c r="F209" s="28" t="s">
         <v>215</v>
       </c>
@@ -11314,15 +11312,15 @@
       </c>
     </row>
     <row r="210" spans="1:7">
-      <c r="A210" s="79"/>
-      <c r="B210" s="81" t="s">
+      <c r="A210" s="87"/>
+      <c r="B210" s="74" t="s">
         <v>224</v>
       </c>
-      <c r="C210" s="82" t="s">
+      <c r="C210" s="73" t="s">
         <v>47</v>
       </c>
-      <c r="D210" s="81"/>
-      <c r="E210" s="81"/>
+      <c r="D210" s="74"/>
+      <c r="E210" s="74"/>
       <c r="F210" s="28" t="s">
         <v>214</v>
       </c>
@@ -11331,13 +11329,13 @@
       </c>
     </row>
     <row r="211" spans="1:7">
-      <c r="A211" s="79"/>
-      <c r="B211" s="81"/>
-      <c r="C211" s="81" t="s">
+      <c r="A211" s="87"/>
+      <c r="B211" s="74"/>
+      <c r="C211" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="D211" s="81"/>
-      <c r="E211" s="81"/>
+      <c r="D211" s="74"/>
+      <c r="E211" s="74"/>
       <c r="F211" s="28" t="s">
         <v>215</v>
       </c>
@@ -11346,17 +11344,17 @@
       </c>
     </row>
     <row r="212" spans="1:7">
-      <c r="A212" s="79" t="s">
+      <c r="A212" s="87" t="s">
         <v>225</v>
       </c>
-      <c r="B212" s="81" t="s">
+      <c r="B212" s="74" t="s">
         <v>226</v>
       </c>
-      <c r="C212" s="82" t="s">
+      <c r="C212" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="D212" s="81"/>
-      <c r="E212" s="81"/>
+      <c r="D212" s="74"/>
+      <c r="E212" s="74"/>
       <c r="F212" s="28" t="s">
         <v>214</v>
       </c>
@@ -11365,13 +11363,13 @@
       </c>
     </row>
     <row r="213" spans="1:7">
-      <c r="A213" s="79"/>
-      <c r="B213" s="81"/>
-      <c r="C213" s="81" t="s">
+      <c r="A213" s="87"/>
+      <c r="B213" s="74"/>
+      <c r="C213" s="74" t="s">
         <v>50</v>
       </c>
-      <c r="D213" s="81"/>
-      <c r="E213" s="81"/>
+      <c r="D213" s="74"/>
+      <c r="E213" s="74"/>
       <c r="F213" s="28" t="s">
         <v>215</v>
       </c>
@@ -11380,15 +11378,15 @@
       </c>
     </row>
     <row r="214" spans="1:7">
-      <c r="A214" s="79"/>
-      <c r="B214" s="81" t="s">
+      <c r="A214" s="87"/>
+      <c r="B214" s="74" t="s">
         <v>227</v>
       </c>
-      <c r="C214" s="82" t="s">
+      <c r="C214" s="73" t="s">
         <v>228</v>
       </c>
-      <c r="D214" s="81"/>
-      <c r="E214" s="81"/>
+      <c r="D214" s="74"/>
+      <c r="E214" s="74"/>
       <c r="F214" s="28" t="s">
         <v>214</v>
       </c>
@@ -11397,13 +11395,13 @@
       </c>
     </row>
     <row r="215" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A215" s="80"/>
-      <c r="B215" s="83"/>
-      <c r="C215" s="83" t="s">
+      <c r="A215" s="98"/>
+      <c r="B215" s="99"/>
+      <c r="C215" s="99" t="s">
         <v>229</v>
       </c>
-      <c r="D215" s="83"/>
-      <c r="E215" s="83"/>
+      <c r="D215" s="99"/>
+      <c r="E215" s="99"/>
       <c r="F215" s="36" t="s">
         <v>215</v>
       </c>
@@ -11442,12 +11440,12 @@
       <c r="A220" s="45" t="s">
         <v>232</v>
       </c>
-      <c r="B220" s="84" t="s">
+      <c r="B220" s="100" t="s">
         <v>52</v>
       </c>
-      <c r="C220" s="84"/>
-      <c r="D220" s="84"/>
-      <c r="E220" s="84"/>
+      <c r="C220" s="100"/>
+      <c r="D220" s="100"/>
+      <c r="E220" s="100"/>
       <c r="F220" s="46" t="s">
         <v>233</v>
       </c>
@@ -11459,12 +11457,12 @@
       <c r="A221" s="48" t="s">
         <v>235</v>
       </c>
-      <c r="B221" s="85" t="s">
+      <c r="B221" s="101" t="s">
         <v>236</v>
       </c>
-      <c r="C221" s="86"/>
-      <c r="D221" s="86"/>
-      <c r="E221" s="86"/>
+      <c r="C221" s="80"/>
+      <c r="D221" s="80"/>
+      <c r="E221" s="80"/>
       <c r="F221" s="49" t="s">
         <v>111</v>
       </c>
@@ -11476,12 +11474,12 @@
       <c r="A222" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="B222" s="87" t="s">
+      <c r="B222" s="102" t="s">
         <v>238</v>
       </c>
-      <c r="C222" s="88"/>
-      <c r="D222" s="88"/>
-      <c r="E222" s="89"/>
+      <c r="C222" s="103"/>
+      <c r="D222" s="103"/>
+      <c r="E222" s="104"/>
       <c r="F222" s="15" t="s">
         <v>63</v>
       </c>
@@ -11493,12 +11491,12 @@
       <c r="A223" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B223" s="87" t="s">
+      <c r="B223" s="102" t="s">
         <v>239</v>
       </c>
-      <c r="C223" s="88"/>
-      <c r="D223" s="88"/>
-      <c r="E223" s="89"/>
+      <c r="C223" s="103"/>
+      <c r="D223" s="103"/>
+      <c r="E223" s="104"/>
       <c r="F223" s="18" t="s">
         <v>63</v>
       </c>
@@ -11510,12 +11508,12 @@
       <c r="A224" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="B224" s="90" t="s">
+      <c r="B224" s="85" t="s">
         <v>241</v>
       </c>
-      <c r="C224" s="83"/>
-      <c r="D224" s="83"/>
-      <c r="E224" s="83"/>
+      <c r="C224" s="99"/>
+      <c r="D224" s="99"/>
+      <c r="E224" s="99"/>
       <c r="F224" s="21" t="s">
         <v>63</v>
       </c>
@@ -11560,11 +11558,11 @@
       <c r="C229" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D229" s="78" t="s">
+      <c r="D229" s="97" t="s">
         <v>54</v>
       </c>
-      <c r="E229" s="78"/>
-      <c r="F229" s="78"/>
+      <c r="E229" s="97"/>
+      <c r="F229" s="97"/>
       <c r="G229" s="57"/>
     </row>
     <row r="230" spans="1:7">
@@ -11577,11 +11575,11 @@
       <c r="C230" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D230" s="77" t="s">
+      <c r="D230" s="109" t="s">
         <v>55</v>
       </c>
-      <c r="E230" s="77"/>
-      <c r="F230" s="77"/>
+      <c r="E230" s="109"/>
+      <c r="F230" s="109"/>
       <c r="G230" s="41"/>
     </row>
     <row r="231" spans="1:7">
@@ -11594,11 +11592,11 @@
       <c r="C231" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D231" s="77" t="s">
+      <c r="D231" s="109" t="s">
         <v>245</v>
       </c>
-      <c r="E231" s="77"/>
-      <c r="F231" s="77"/>
+      <c r="E231" s="109"/>
+      <c r="F231" s="109"/>
       <c r="G231" s="41"/>
     </row>
     <row r="232" spans="1:7">
@@ -11611,11 +11609,11 @@
       <c r="C232" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D232" s="77" t="s">
+      <c r="D232" s="109" t="s">
         <v>246</v>
       </c>
-      <c r="E232" s="77"/>
-      <c r="F232" s="77"/>
+      <c r="E232" s="109"/>
+      <c r="F232" s="109"/>
       <c r="G232" s="41"/>
     </row>
     <row r="233" spans="1:7">
@@ -11628,11 +11626,11 @@
       <c r="C233" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D233" s="77" t="s">
+      <c r="D233" s="109" t="s">
         <v>247</v>
       </c>
-      <c r="E233" s="77"/>
-      <c r="F233" s="77"/>
+      <c r="E233" s="109"/>
+      <c r="F233" s="109"/>
       <c r="G233" s="41"/>
     </row>
     <row r="234" spans="1:7">
@@ -11645,11 +11643,11 @@
       <c r="C234" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D234" s="77" t="s">
+      <c r="D234" s="109" t="s">
         <v>248</v>
       </c>
-      <c r="E234" s="77"/>
-      <c r="F234" s="77"/>
+      <c r="E234" s="109"/>
+      <c r="F234" s="109"/>
       <c r="G234" s="41"/>
     </row>
     <row r="235" spans="1:7">
@@ -11662,11 +11660,11 @@
       <c r="C235" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D235" s="73" t="s">
+      <c r="D235" s="105" t="s">
         <v>64</v>
       </c>
-      <c r="E235" s="74"/>
-      <c r="F235" s="75"/>
+      <c r="E235" s="106"/>
+      <c r="F235" s="107"/>
       <c r="G235" s="43"/>
     </row>
     <row r="236" spans="1:7">
@@ -11679,11 +11677,11 @@
       <c r="C236" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D236" s="73" t="s">
+      <c r="D236" s="105" t="s">
         <v>65</v>
       </c>
-      <c r="E236" s="74"/>
-      <c r="F236" s="75"/>
+      <c r="E236" s="106"/>
+      <c r="F236" s="107"/>
       <c r="G236" s="43"/>
     </row>
     <row r="237" spans="1:7">
@@ -11696,11 +11694,11 @@
       <c r="C237" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D237" s="73" t="s">
+      <c r="D237" s="105" t="s">
         <v>69</v>
       </c>
-      <c r="E237" s="74"/>
-      <c r="F237" s="75"/>
+      <c r="E237" s="106"/>
+      <c r="F237" s="107"/>
       <c r="G237" s="43"/>
     </row>
     <row r="238" spans="1:7">
@@ -11798,33 +11796,56 @@
       <c r="C243" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="D243" s="76" t="s">
+      <c r="D243" s="108" t="s">
         <v>264</v>
       </c>
-      <c r="E243" s="76"/>
-      <c r="F243" s="76"/>
+      <c r="E243" s="108"/>
+      <c r="F243" s="108"/>
       <c r="G243" s="44"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" scale="115">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
       <selection activeCell="C4" sqref="C4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
+    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" scale="115">
       <selection activeCell="C4" sqref="C4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="51">
-    <mergeCell ref="B174:B176"/>
-    <mergeCell ref="F111:N111"/>
-    <mergeCell ref="B148:B160"/>
-    <mergeCell ref="B161:B162"/>
-    <mergeCell ref="B163:B165"/>
-    <mergeCell ref="B166:B173"/>
+    <mergeCell ref="D236:F236"/>
+    <mergeCell ref="D237:F237"/>
+    <mergeCell ref="D243:F243"/>
+    <mergeCell ref="D230:F230"/>
+    <mergeCell ref="D231:F231"/>
+    <mergeCell ref="D232:F232"/>
+    <mergeCell ref="D233:F233"/>
+    <mergeCell ref="D234:F234"/>
+    <mergeCell ref="D235:F235"/>
+    <mergeCell ref="D229:F229"/>
+    <mergeCell ref="A212:A215"/>
+    <mergeCell ref="B212:B213"/>
+    <mergeCell ref="C212:E212"/>
+    <mergeCell ref="C213:E213"/>
+    <mergeCell ref="B214:B215"/>
+    <mergeCell ref="C214:E214"/>
+    <mergeCell ref="C215:E215"/>
+    <mergeCell ref="B220:E220"/>
+    <mergeCell ref="B221:E221"/>
+    <mergeCell ref="B222:E222"/>
+    <mergeCell ref="B223:E223"/>
+    <mergeCell ref="B224:E224"/>
+    <mergeCell ref="A208:A211"/>
+    <mergeCell ref="B208:B209"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C209:E209"/>
+    <mergeCell ref="B210:B211"/>
+    <mergeCell ref="C210:E210"/>
+    <mergeCell ref="C211:E211"/>
     <mergeCell ref="B177:B178"/>
     <mergeCell ref="B179:B185"/>
     <mergeCell ref="C199:E199"/>
@@ -11841,35 +11862,12 @@
     <mergeCell ref="B206:B207"/>
     <mergeCell ref="C206:E206"/>
     <mergeCell ref="C207:E207"/>
-    <mergeCell ref="A208:A211"/>
-    <mergeCell ref="B208:B209"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C209:E209"/>
-    <mergeCell ref="B210:B211"/>
-    <mergeCell ref="C210:E210"/>
-    <mergeCell ref="C211:E211"/>
-    <mergeCell ref="D229:F229"/>
-    <mergeCell ref="A212:A215"/>
-    <mergeCell ref="B212:B213"/>
-    <mergeCell ref="C212:E212"/>
-    <mergeCell ref="C213:E213"/>
-    <mergeCell ref="B214:B215"/>
-    <mergeCell ref="C214:E214"/>
-    <mergeCell ref="C215:E215"/>
-    <mergeCell ref="B220:E220"/>
-    <mergeCell ref="B221:E221"/>
-    <mergeCell ref="B222:E222"/>
-    <mergeCell ref="B223:E223"/>
-    <mergeCell ref="B224:E224"/>
-    <mergeCell ref="D236:F236"/>
-    <mergeCell ref="D237:F237"/>
-    <mergeCell ref="D243:F243"/>
-    <mergeCell ref="D230:F230"/>
-    <mergeCell ref="D231:F231"/>
-    <mergeCell ref="D232:F232"/>
-    <mergeCell ref="D233:F233"/>
-    <mergeCell ref="D234:F234"/>
-    <mergeCell ref="D235:F235"/>
+    <mergeCell ref="B174:B176"/>
+    <mergeCell ref="F111:N111"/>
+    <mergeCell ref="B148:B160"/>
+    <mergeCell ref="B161:B162"/>
+    <mergeCell ref="B163:B165"/>
+    <mergeCell ref="B166:B173"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -11892,18 +11890,18 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
+      <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
-      <selection activeCell="E26" sqref="E26"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
i404--Update Apollo EIT2 suite file
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/radiant/silicon_07_apollo.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/radiant/silicon_07_apollo.xlsx
@@ -27,10 +27,10 @@
   </definedNames>
   <calcPr calcId="122211"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
+    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
     <customWorkbookView name="Jeffrey Ye - Personal View" guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="3"/>
-    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
-    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
-    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -1779,7 +1779,7 @@
     <t>silicon_07_apollo_v1.05</t>
   </si>
   <si>
-    <t xml:space="preserve">cmd = --check-conf=impl.conf --synthesis=synplify </t>
+    <t>cmd = --check-conf=impl.conf --synthesis=synplify --check-smart</t>
   </si>
 </sst>
 </file>
@@ -3094,76 +3094,49 @@
     <xf numFmtId="49" fontId="12" fillId="7" borderId="7" xfId="13" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
@@ -3183,17 +3156,44 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="48" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -6071,7 +6071,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -6295,23 +6297,23 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
-    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" topLeftCell="A2">
-      <selection activeCell="C52" sqref="C52"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
+      <selection activeCell="B35" sqref="B35"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
       <selection activeCell="B4" sqref="B4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-    </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
-      <selection activeCell="B35" sqref="B35"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="G15" sqref="G15"/>
+    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" topLeftCell="A2">
+      <selection activeCell="C52" sqref="C52"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
@@ -9245,17 +9247,17 @@
       <c r="E111" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F111" s="106" t="s">
+      <c r="F111" s="75" t="s">
         <v>87</v>
       </c>
-      <c r="G111" s="107"/>
-      <c r="H111" s="107"/>
-      <c r="I111" s="107"/>
-      <c r="J111" s="107"/>
-      <c r="K111" s="107"/>
-      <c r="L111" s="107"/>
-      <c r="M111" s="107"/>
-      <c r="N111" s="108"/>
+      <c r="G111" s="76"/>
+      <c r="H111" s="76"/>
+      <c r="I111" s="76"/>
+      <c r="J111" s="76"/>
+      <c r="K111" s="76"/>
+      <c r="L111" s="76"/>
+      <c r="M111" s="76"/>
+      <c r="N111" s="77"/>
     </row>
     <row r="112" spans="1:14">
       <c r="A112" s="11" t="s">
@@ -10145,7 +10147,7 @@
       <c r="A148" s="26">
         <v>1</v>
       </c>
-      <c r="B148" s="91" t="s">
+      <c r="B148" s="78" t="s">
         <v>3</v>
       </c>
       <c r="C148" s="27" t="s">
@@ -10171,7 +10173,7 @@
       <c r="A149" s="26">
         <v>2</v>
       </c>
-      <c r="B149" s="92"/>
+      <c r="B149" s="79"/>
       <c r="C149" s="28" t="s">
         <v>136</v>
       </c>
@@ -10193,7 +10195,7 @@
       <c r="A150" s="26">
         <v>3</v>
       </c>
-      <c r="B150" s="92"/>
+      <c r="B150" s="79"/>
       <c r="C150" s="28" t="s">
         <v>9</v>
       </c>
@@ -10213,7 +10215,7 @@
       <c r="A151" s="26">
         <v>4</v>
       </c>
-      <c r="B151" s="92"/>
+      <c r="B151" s="79"/>
       <c r="C151" s="28" t="s">
         <v>138</v>
       </c>
@@ -10237,7 +10239,7 @@
       <c r="A152" s="26">
         <v>5</v>
       </c>
-      <c r="B152" s="92"/>
+      <c r="B152" s="79"/>
       <c r="C152" s="27" t="s">
         <v>140</v>
       </c>
@@ -10261,7 +10263,7 @@
       <c r="A153" s="26">
         <v>6</v>
       </c>
-      <c r="B153" s="92"/>
+      <c r="B153" s="79"/>
       <c r="C153" s="27" t="s">
         <v>144</v>
       </c>
@@ -10285,7 +10287,7 @@
       <c r="A154" s="26">
         <v>7</v>
       </c>
-      <c r="B154" s="92"/>
+      <c r="B154" s="79"/>
       <c r="C154" s="28" t="s">
         <v>147</v>
       </c>
@@ -10307,7 +10309,7 @@
       <c r="A155" s="26">
         <v>8</v>
       </c>
-      <c r="B155" s="92"/>
+      <c r="B155" s="79"/>
       <c r="C155" s="27" t="s">
         <v>148</v>
       </c>
@@ -10331,7 +10333,7 @@
       <c r="A156" s="26">
         <v>9</v>
       </c>
-      <c r="B156" s="92"/>
+      <c r="B156" s="79"/>
       <c r="C156" s="27" t="s">
         <v>149</v>
       </c>
@@ -10355,7 +10357,7 @@
       <c r="A157" s="26">
         <v>10</v>
       </c>
-      <c r="B157" s="92"/>
+      <c r="B157" s="79"/>
       <c r="C157" s="28" t="s">
         <v>150</v>
       </c>
@@ -10379,7 +10381,7 @@
       <c r="A158" s="26">
         <v>11</v>
       </c>
-      <c r="B158" s="92"/>
+      <c r="B158" s="79"/>
       <c r="C158" s="68" t="s">
         <v>151</v>
       </c>
@@ -10403,7 +10405,7 @@
       <c r="A159" s="26">
         <v>12</v>
       </c>
-      <c r="B159" s="92"/>
+      <c r="B159" s="79"/>
       <c r="C159" s="28" t="s">
         <v>153</v>
       </c>
@@ -10425,7 +10427,7 @@
       <c r="A160" s="26">
         <v>13</v>
       </c>
-      <c r="B160" s="86"/>
+      <c r="B160" s="80"/>
       <c r="C160" s="28" t="s">
         <v>56</v>
       </c>
@@ -10449,7 +10451,7 @@
       <c r="A161" s="26">
         <v>14</v>
       </c>
-      <c r="B161" s="82" t="s">
+      <c r="B161" s="73" t="s">
         <v>4</v>
       </c>
       <c r="C161" s="28" t="s">
@@ -10475,7 +10477,7 @@
       <c r="A162" s="26">
         <v>15</v>
       </c>
-      <c r="B162" s="81"/>
+      <c r="B162" s="74"/>
       <c r="C162" s="28" t="s">
         <v>161</v>
       </c>
@@ -10499,7 +10501,7 @@
       <c r="A163" s="26">
         <v>16</v>
       </c>
-      <c r="B163" s="91" t="s">
+      <c r="B163" s="78" t="s">
         <v>5</v>
       </c>
       <c r="C163" s="28" t="s">
@@ -10523,7 +10525,7 @@
       <c r="A164" s="26">
         <v>17</v>
       </c>
-      <c r="B164" s="109"/>
+      <c r="B164" s="81"/>
       <c r="C164" s="27" t="s">
         <v>165</v>
       </c>
@@ -10545,7 +10547,7 @@
       <c r="A165" s="26">
         <v>18</v>
       </c>
-      <c r="B165" s="86"/>
+      <c r="B165" s="80"/>
       <c r="C165" s="27" t="s">
         <v>167</v>
       </c>
@@ -10565,7 +10567,7 @@
       <c r="A166" s="26">
         <v>19</v>
       </c>
-      <c r="B166" s="82" t="s">
+      <c r="B166" s="73" t="s">
         <v>6</v>
       </c>
       <c r="C166" s="28" t="s">
@@ -10589,7 +10591,7 @@
       <c r="A167" s="26">
         <v>20</v>
       </c>
-      <c r="B167" s="81"/>
+      <c r="B167" s="74"/>
       <c r="C167" s="28" t="s">
         <v>172</v>
       </c>
@@ -10609,7 +10611,7 @@
       <c r="A168" s="26">
         <v>21</v>
       </c>
-      <c r="B168" s="81"/>
+      <c r="B168" s="74"/>
       <c r="C168" s="28" t="s">
         <v>173</v>
       </c>
@@ -10629,7 +10631,7 @@
       <c r="A169" s="26">
         <v>22</v>
       </c>
-      <c r="B169" s="81"/>
+      <c r="B169" s="74"/>
       <c r="C169" s="28" t="s">
         <v>174</v>
       </c>
@@ -10649,7 +10651,7 @@
       <c r="A170" s="26">
         <v>23</v>
       </c>
-      <c r="B170" s="81"/>
+      <c r="B170" s="74"/>
       <c r="C170" s="28" t="s">
         <v>175</v>
       </c>
@@ -10669,7 +10671,7 @@
       <c r="A171" s="26">
         <v>24</v>
       </c>
-      <c r="B171" s="81"/>
+      <c r="B171" s="74"/>
       <c r="C171" s="28" t="s">
         <v>176</v>
       </c>
@@ -10689,7 +10691,7 @@
       <c r="A172" s="26">
         <v>25</v>
       </c>
-      <c r="B172" s="81"/>
+      <c r="B172" s="74"/>
       <c r="C172" s="28" t="s">
         <v>177</v>
       </c>
@@ -10709,7 +10711,7 @@
       <c r="A173" s="26">
         <v>26</v>
       </c>
-      <c r="B173" s="81"/>
+      <c r="B173" s="74"/>
       <c r="C173" s="28" t="s">
         <v>41</v>
       </c>
@@ -10729,7 +10731,7 @@
       <c r="A174" s="26">
         <v>27</v>
       </c>
-      <c r="B174" s="82" t="s">
+      <c r="B174" s="73" t="s">
         <v>7</v>
       </c>
       <c r="C174" s="28" t="s">
@@ -10753,7 +10755,7 @@
       <c r="A175" s="26">
         <v>28</v>
       </c>
-      <c r="B175" s="81"/>
+      <c r="B175" s="74"/>
       <c r="C175" s="27" t="s">
         <v>181</v>
       </c>
@@ -10775,7 +10777,7 @@
       <c r="A176" s="26">
         <v>29</v>
       </c>
-      <c r="B176" s="81"/>
+      <c r="B176" s="74"/>
       <c r="C176" s="28" t="s">
         <v>184</v>
       </c>
@@ -10797,7 +10799,7 @@
       <c r="A177" s="26">
         <v>30</v>
       </c>
-      <c r="B177" s="91" t="s">
+      <c r="B177" s="78" t="s">
         <v>8</v>
       </c>
       <c r="C177" s="28" t="s">
@@ -10823,7 +10825,7 @@
       <c r="A178" s="31">
         <v>31</v>
       </c>
-      <c r="B178" s="92"/>
+      <c r="B178" s="79"/>
       <c r="C178" s="32" t="s">
         <v>189</v>
       </c>
@@ -10847,7 +10849,7 @@
       <c r="A179" s="23">
         <v>32</v>
       </c>
-      <c r="B179" s="93" t="s">
+      <c r="B179" s="82" t="s">
         <v>191</v>
       </c>
       <c r="C179" s="33" t="s">
@@ -10871,7 +10873,7 @@
       <c r="A180" s="26">
         <v>33</v>
       </c>
-      <c r="B180" s="94"/>
+      <c r="B180" s="83"/>
       <c r="C180" s="27" t="s">
         <v>195</v>
       </c>
@@ -10893,7 +10895,7 @@
       <c r="A181" s="26">
         <v>34</v>
       </c>
-      <c r="B181" s="95"/>
+      <c r="B181" s="84"/>
       <c r="C181" s="34" t="s">
         <v>198</v>
       </c>
@@ -10915,7 +10917,7 @@
       <c r="A182" s="31">
         <v>35</v>
       </c>
-      <c r="B182" s="95"/>
+      <c r="B182" s="84"/>
       <c r="C182" s="34" t="s">
         <v>199</v>
       </c>
@@ -10937,7 +10939,7 @@
       <c r="A183" s="31">
         <v>36</v>
       </c>
-      <c r="B183" s="95"/>
+      <c r="B183" s="84"/>
       <c r="C183" s="34" t="s">
         <v>202</v>
       </c>
@@ -10957,7 +10959,7 @@
       <c r="A184" s="31">
         <v>37</v>
       </c>
-      <c r="B184" s="95"/>
+      <c r="B184" s="84"/>
       <c r="C184" s="34" t="s">
         <v>254</v>
       </c>
@@ -10979,7 +10981,7 @@
       <c r="A185" s="35">
         <v>38</v>
       </c>
-      <c r="B185" s="90"/>
+      <c r="B185" s="85"/>
       <c r="C185" s="36" t="s">
         <v>258</v>
       </c>
@@ -11030,11 +11032,11 @@
       <c r="B199" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="C199" s="96" t="s">
+      <c r="C199" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="D199" s="96"/>
-      <c r="E199" s="96"/>
+      <c r="D199" s="86"/>
+      <c r="E199" s="86"/>
       <c r="F199" s="39" t="s">
         <v>43</v>
       </c>
@@ -11043,17 +11045,17 @@
       </c>
     </row>
     <row r="200" spans="1:7">
-      <c r="A200" s="79" t="s">
+      <c r="A200" s="87" t="s">
         <v>212</v>
       </c>
-      <c r="B200" s="81" t="s">
+      <c r="B200" s="74" t="s">
         <v>213</v>
       </c>
-      <c r="C200" s="98" t="s">
+      <c r="C200" s="89" t="s">
         <v>57</v>
       </c>
-      <c r="D200" s="99"/>
-      <c r="E200" s="99"/>
+      <c r="D200" s="90"/>
+      <c r="E200" s="90"/>
       <c r="F200" s="28" t="s">
         <v>214</v>
       </c>
@@ -11062,13 +11064,13 @@
       </c>
     </row>
     <row r="201" spans="1:7">
-      <c r="A201" s="79"/>
-      <c r="B201" s="97"/>
-      <c r="C201" s="100" t="s">
+      <c r="A201" s="87"/>
+      <c r="B201" s="88"/>
+      <c r="C201" s="91" t="s">
         <v>57</v>
       </c>
-      <c r="D201" s="101"/>
-      <c r="E201" s="101"/>
+      <c r="D201" s="92"/>
+      <c r="E201" s="92"/>
       <c r="F201" s="32" t="s">
         <v>215</v>
       </c>
@@ -11077,15 +11079,15 @@
       </c>
     </row>
     <row r="202" spans="1:7">
-      <c r="A202" s="79"/>
-      <c r="B202" s="81" t="s">
+      <c r="A202" s="87"/>
+      <c r="B202" s="74" t="s">
         <v>216</v>
       </c>
-      <c r="C202" s="102" t="s">
+      <c r="C202" s="93" t="s">
         <v>217</v>
       </c>
-      <c r="D202" s="102"/>
-      <c r="E202" s="102"/>
+      <c r="D202" s="93"/>
+      <c r="E202" s="93"/>
       <c r="F202" s="28" t="s">
         <v>214</v>
       </c>
@@ -11094,13 +11096,13 @@
       </c>
     </row>
     <row r="203" spans="1:7">
-      <c r="A203" s="79"/>
-      <c r="B203" s="81"/>
-      <c r="C203" s="100" t="s">
+      <c r="A203" s="87"/>
+      <c r="B203" s="74"/>
+      <c r="C203" s="91" t="s">
         <v>217</v>
       </c>
-      <c r="D203" s="100"/>
-      <c r="E203" s="100"/>
+      <c r="D203" s="91"/>
+      <c r="E203" s="91"/>
       <c r="F203" s="28" t="s">
         <v>215</v>
       </c>
@@ -11109,15 +11111,15 @@
       </c>
     </row>
     <row r="204" spans="1:7">
-      <c r="A204" s="79"/>
-      <c r="B204" s="97" t="s">
+      <c r="A204" s="87"/>
+      <c r="B204" s="88" t="s">
         <v>218</v>
       </c>
-      <c r="C204" s="103" t="s">
+      <c r="C204" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="D204" s="104"/>
-      <c r="E204" s="105"/>
+      <c r="D204" s="95"/>
+      <c r="E204" s="96"/>
       <c r="F204" s="28" t="s">
         <v>214</v>
       </c>
@@ -11126,13 +11128,13 @@
       </c>
     </row>
     <row r="205" spans="1:7">
-      <c r="A205" s="79"/>
-      <c r="B205" s="86"/>
-      <c r="C205" s="103" t="s">
+      <c r="A205" s="87"/>
+      <c r="B205" s="80"/>
+      <c r="C205" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="D205" s="104"/>
-      <c r="E205" s="105"/>
+      <c r="D205" s="95"/>
+      <c r="E205" s="96"/>
       <c r="F205" s="28" t="s">
         <v>215</v>
       </c>
@@ -11141,15 +11143,15 @@
       </c>
     </row>
     <row r="206" spans="1:7">
-      <c r="A206" s="79"/>
-      <c r="B206" s="81" t="s">
+      <c r="A206" s="87"/>
+      <c r="B206" s="74" t="s">
         <v>219</v>
       </c>
-      <c r="C206" s="102" t="s">
+      <c r="C206" s="93" t="s">
         <v>220</v>
       </c>
-      <c r="D206" s="102"/>
-      <c r="E206" s="102"/>
+      <c r="D206" s="93"/>
+      <c r="E206" s="93"/>
       <c r="F206" s="28" t="s">
         <v>214</v>
       </c>
@@ -11158,13 +11160,13 @@
       </c>
     </row>
     <row r="207" spans="1:7">
-      <c r="A207" s="79"/>
-      <c r="B207" s="81"/>
-      <c r="C207" s="102" t="s">
+      <c r="A207" s="87"/>
+      <c r="B207" s="74"/>
+      <c r="C207" s="93" t="s">
         <v>220</v>
       </c>
-      <c r="D207" s="102"/>
-      <c r="E207" s="102"/>
+      <c r="D207" s="93"/>
+      <c r="E207" s="93"/>
       <c r="F207" s="28" t="s">
         <v>215</v>
       </c>
@@ -11173,17 +11175,17 @@
       </c>
     </row>
     <row r="208" spans="1:7">
-      <c r="A208" s="79" t="s">
+      <c r="A208" s="87" t="s">
         <v>221</v>
       </c>
-      <c r="B208" s="81" t="s">
+      <c r="B208" s="74" t="s">
         <v>222</v>
       </c>
-      <c r="C208" s="82" t="s">
+      <c r="C208" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="D208" s="81"/>
-      <c r="E208" s="81"/>
+      <c r="D208" s="74"/>
+      <c r="E208" s="74"/>
       <c r="F208" s="28" t="s">
         <v>214</v>
       </c>
@@ -11192,13 +11194,13 @@
       </c>
     </row>
     <row r="209" spans="1:7">
-      <c r="A209" s="79"/>
-      <c r="B209" s="81"/>
-      <c r="C209" s="81" t="s">
+      <c r="A209" s="87"/>
+      <c r="B209" s="74"/>
+      <c r="C209" s="74" t="s">
         <v>46</v>
       </c>
-      <c r="D209" s="81"/>
-      <c r="E209" s="81"/>
+      <c r="D209" s="74"/>
+      <c r="E209" s="74"/>
       <c r="F209" s="28" t="s">
         <v>215</v>
       </c>
@@ -11207,15 +11209,15 @@
       </c>
     </row>
     <row r="210" spans="1:7">
-      <c r="A210" s="79"/>
-      <c r="B210" s="81" t="s">
+      <c r="A210" s="87"/>
+      <c r="B210" s="74" t="s">
         <v>224</v>
       </c>
-      <c r="C210" s="82" t="s">
+      <c r="C210" s="73" t="s">
         <v>47</v>
       </c>
-      <c r="D210" s="81"/>
-      <c r="E210" s="81"/>
+      <c r="D210" s="74"/>
+      <c r="E210" s="74"/>
       <c r="F210" s="28" t="s">
         <v>214</v>
       </c>
@@ -11224,13 +11226,13 @@
       </c>
     </row>
     <row r="211" spans="1:7">
-      <c r="A211" s="79"/>
-      <c r="B211" s="81"/>
-      <c r="C211" s="81" t="s">
+      <c r="A211" s="87"/>
+      <c r="B211" s="74"/>
+      <c r="C211" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="D211" s="81"/>
-      <c r="E211" s="81"/>
+      <c r="D211" s="74"/>
+      <c r="E211" s="74"/>
       <c r="F211" s="28" t="s">
         <v>215</v>
       </c>
@@ -11239,17 +11241,17 @@
       </c>
     </row>
     <row r="212" spans="1:7">
-      <c r="A212" s="79" t="s">
+      <c r="A212" s="87" t="s">
         <v>225</v>
       </c>
-      <c r="B212" s="81" t="s">
+      <c r="B212" s="74" t="s">
         <v>226</v>
       </c>
-      <c r="C212" s="82" t="s">
+      <c r="C212" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="D212" s="81"/>
-      <c r="E212" s="81"/>
+      <c r="D212" s="74"/>
+      <c r="E212" s="74"/>
       <c r="F212" s="28" t="s">
         <v>214</v>
       </c>
@@ -11258,13 +11260,13 @@
       </c>
     </row>
     <row r="213" spans="1:7">
-      <c r="A213" s="79"/>
-      <c r="B213" s="81"/>
-      <c r="C213" s="81" t="s">
+      <c r="A213" s="87"/>
+      <c r="B213" s="74"/>
+      <c r="C213" s="74" t="s">
         <v>50</v>
       </c>
-      <c r="D213" s="81"/>
-      <c r="E213" s="81"/>
+      <c r="D213" s="74"/>
+      <c r="E213" s="74"/>
       <c r="F213" s="28" t="s">
         <v>215</v>
       </c>
@@ -11273,15 +11275,15 @@
       </c>
     </row>
     <row r="214" spans="1:7">
-      <c r="A214" s="79"/>
-      <c r="B214" s="81" t="s">
+      <c r="A214" s="87"/>
+      <c r="B214" s="74" t="s">
         <v>227</v>
       </c>
-      <c r="C214" s="82" t="s">
+      <c r="C214" s="73" t="s">
         <v>228</v>
       </c>
-      <c r="D214" s="81"/>
-      <c r="E214" s="81"/>
+      <c r="D214" s="74"/>
+      <c r="E214" s="74"/>
       <c r="F214" s="28" t="s">
         <v>214</v>
       </c>
@@ -11290,13 +11292,13 @@
       </c>
     </row>
     <row r="215" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A215" s="80"/>
-      <c r="B215" s="83"/>
-      <c r="C215" s="83" t="s">
+      <c r="A215" s="98"/>
+      <c r="B215" s="99"/>
+      <c r="C215" s="99" t="s">
         <v>229</v>
       </c>
-      <c r="D215" s="83"/>
-      <c r="E215" s="83"/>
+      <c r="D215" s="99"/>
+      <c r="E215" s="99"/>
       <c r="F215" s="36" t="s">
         <v>215</v>
       </c>
@@ -11335,12 +11337,12 @@
       <c r="A220" s="45" t="s">
         <v>232</v>
       </c>
-      <c r="B220" s="84" t="s">
+      <c r="B220" s="100" t="s">
         <v>52</v>
       </c>
-      <c r="C220" s="84"/>
-      <c r="D220" s="84"/>
-      <c r="E220" s="84"/>
+      <c r="C220" s="100"/>
+      <c r="D220" s="100"/>
+      <c r="E220" s="100"/>
       <c r="F220" s="46" t="s">
         <v>233</v>
       </c>
@@ -11352,12 +11354,12 @@
       <c r="A221" s="48" t="s">
         <v>235</v>
       </c>
-      <c r="B221" s="85" t="s">
+      <c r="B221" s="101" t="s">
         <v>236</v>
       </c>
-      <c r="C221" s="86"/>
-      <c r="D221" s="86"/>
-      <c r="E221" s="86"/>
+      <c r="C221" s="80"/>
+      <c r="D221" s="80"/>
+      <c r="E221" s="80"/>
       <c r="F221" s="49" t="s">
         <v>111</v>
       </c>
@@ -11369,12 +11371,12 @@
       <c r="A222" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="B222" s="87" t="s">
+      <c r="B222" s="102" t="s">
         <v>238</v>
       </c>
-      <c r="C222" s="88"/>
-      <c r="D222" s="88"/>
-      <c r="E222" s="89"/>
+      <c r="C222" s="103"/>
+      <c r="D222" s="103"/>
+      <c r="E222" s="104"/>
       <c r="F222" s="15" t="s">
         <v>63</v>
       </c>
@@ -11386,12 +11388,12 @@
       <c r="A223" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B223" s="87" t="s">
+      <c r="B223" s="102" t="s">
         <v>239</v>
       </c>
-      <c r="C223" s="88"/>
-      <c r="D223" s="88"/>
-      <c r="E223" s="89"/>
+      <c r="C223" s="103"/>
+      <c r="D223" s="103"/>
+      <c r="E223" s="104"/>
       <c r="F223" s="18" t="s">
         <v>63</v>
       </c>
@@ -11403,12 +11405,12 @@
       <c r="A224" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="B224" s="90" t="s">
+      <c r="B224" s="85" t="s">
         <v>241</v>
       </c>
-      <c r="C224" s="83"/>
-      <c r="D224" s="83"/>
-      <c r="E224" s="83"/>
+      <c r="C224" s="99"/>
+      <c r="D224" s="99"/>
+      <c r="E224" s="99"/>
       <c r="F224" s="21" t="s">
         <v>63</v>
       </c>
@@ -11453,11 +11455,11 @@
       <c r="C229" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D229" s="78" t="s">
+      <c r="D229" s="97" t="s">
         <v>54</v>
       </c>
-      <c r="E229" s="78"/>
-      <c r="F229" s="78"/>
+      <c r="E229" s="97"/>
+      <c r="F229" s="97"/>
       <c r="G229" s="57"/>
     </row>
     <row r="230" spans="1:7">
@@ -11470,11 +11472,11 @@
       <c r="C230" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D230" s="77" t="s">
+      <c r="D230" s="109" t="s">
         <v>55</v>
       </c>
-      <c r="E230" s="77"/>
-      <c r="F230" s="77"/>
+      <c r="E230" s="109"/>
+      <c r="F230" s="109"/>
       <c r="G230" s="41"/>
     </row>
     <row r="231" spans="1:7">
@@ -11487,11 +11489,11 @@
       <c r="C231" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D231" s="77" t="s">
+      <c r="D231" s="109" t="s">
         <v>245</v>
       </c>
-      <c r="E231" s="77"/>
-      <c r="F231" s="77"/>
+      <c r="E231" s="109"/>
+      <c r="F231" s="109"/>
       <c r="G231" s="41"/>
     </row>
     <row r="232" spans="1:7">
@@ -11504,11 +11506,11 @@
       <c r="C232" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D232" s="77" t="s">
+      <c r="D232" s="109" t="s">
         <v>246</v>
       </c>
-      <c r="E232" s="77"/>
-      <c r="F232" s="77"/>
+      <c r="E232" s="109"/>
+      <c r="F232" s="109"/>
       <c r="G232" s="41"/>
     </row>
     <row r="233" spans="1:7">
@@ -11521,11 +11523,11 @@
       <c r="C233" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D233" s="77" t="s">
+      <c r="D233" s="109" t="s">
         <v>247</v>
       </c>
-      <c r="E233" s="77"/>
-      <c r="F233" s="77"/>
+      <c r="E233" s="109"/>
+      <c r="F233" s="109"/>
       <c r="G233" s="41"/>
     </row>
     <row r="234" spans="1:7">
@@ -11538,11 +11540,11 @@
       <c r="C234" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D234" s="77" t="s">
+      <c r="D234" s="109" t="s">
         <v>248</v>
       </c>
-      <c r="E234" s="77"/>
-      <c r="F234" s="77"/>
+      <c r="E234" s="109"/>
+      <c r="F234" s="109"/>
       <c r="G234" s="41"/>
     </row>
     <row r="235" spans="1:7">
@@ -11555,11 +11557,11 @@
       <c r="C235" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D235" s="73" t="s">
+      <c r="D235" s="105" t="s">
         <v>64</v>
       </c>
-      <c r="E235" s="74"/>
-      <c r="F235" s="75"/>
+      <c r="E235" s="106"/>
+      <c r="F235" s="107"/>
       <c r="G235" s="43"/>
     </row>
     <row r="236" spans="1:7">
@@ -11572,11 +11574,11 @@
       <c r="C236" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D236" s="73" t="s">
+      <c r="D236" s="105" t="s">
         <v>65</v>
       </c>
-      <c r="E236" s="74"/>
-      <c r="F236" s="75"/>
+      <c r="E236" s="106"/>
+      <c r="F236" s="107"/>
       <c r="G236" s="43"/>
     </row>
     <row r="237" spans="1:7">
@@ -11589,11 +11591,11 @@
       <c r="C237" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D237" s="73" t="s">
+      <c r="D237" s="105" t="s">
         <v>69</v>
       </c>
-      <c r="E237" s="74"/>
-      <c r="F237" s="75"/>
+      <c r="E237" s="106"/>
+      <c r="F237" s="107"/>
       <c r="G237" s="43"/>
     </row>
     <row r="238" spans="1:7">
@@ -11691,33 +11693,56 @@
       <c r="C243" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="D243" s="76" t="s">
+      <c r="D243" s="108" t="s">
         <v>264</v>
       </c>
-      <c r="E243" s="76"/>
-      <c r="F243" s="76"/>
+      <c r="E243" s="108"/>
+      <c r="F243" s="108"/>
       <c r="G243" s="44"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" scale="115">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
       <selection activeCell="C4" sqref="C4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
+    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" scale="115">
       <selection activeCell="C4" sqref="C4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="51">
-    <mergeCell ref="B174:B176"/>
-    <mergeCell ref="F111:N111"/>
-    <mergeCell ref="B148:B160"/>
-    <mergeCell ref="B161:B162"/>
-    <mergeCell ref="B163:B165"/>
-    <mergeCell ref="B166:B173"/>
+    <mergeCell ref="D236:F236"/>
+    <mergeCell ref="D237:F237"/>
+    <mergeCell ref="D243:F243"/>
+    <mergeCell ref="D230:F230"/>
+    <mergeCell ref="D231:F231"/>
+    <mergeCell ref="D232:F232"/>
+    <mergeCell ref="D233:F233"/>
+    <mergeCell ref="D234:F234"/>
+    <mergeCell ref="D235:F235"/>
+    <mergeCell ref="D229:F229"/>
+    <mergeCell ref="A212:A215"/>
+    <mergeCell ref="B212:B213"/>
+    <mergeCell ref="C212:E212"/>
+    <mergeCell ref="C213:E213"/>
+    <mergeCell ref="B214:B215"/>
+    <mergeCell ref="C214:E214"/>
+    <mergeCell ref="C215:E215"/>
+    <mergeCell ref="B220:E220"/>
+    <mergeCell ref="B221:E221"/>
+    <mergeCell ref="B222:E222"/>
+    <mergeCell ref="B223:E223"/>
+    <mergeCell ref="B224:E224"/>
+    <mergeCell ref="A208:A211"/>
+    <mergeCell ref="B208:B209"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C209:E209"/>
+    <mergeCell ref="B210:B211"/>
+    <mergeCell ref="C210:E210"/>
+    <mergeCell ref="C211:E211"/>
     <mergeCell ref="B177:B178"/>
     <mergeCell ref="B179:B185"/>
     <mergeCell ref="C199:E199"/>
@@ -11734,35 +11759,12 @@
     <mergeCell ref="B206:B207"/>
     <mergeCell ref="C206:E206"/>
     <mergeCell ref="C207:E207"/>
-    <mergeCell ref="A208:A211"/>
-    <mergeCell ref="B208:B209"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C209:E209"/>
-    <mergeCell ref="B210:B211"/>
-    <mergeCell ref="C210:E210"/>
-    <mergeCell ref="C211:E211"/>
-    <mergeCell ref="D229:F229"/>
-    <mergeCell ref="A212:A215"/>
-    <mergeCell ref="B212:B213"/>
-    <mergeCell ref="C212:E212"/>
-    <mergeCell ref="C213:E213"/>
-    <mergeCell ref="B214:B215"/>
-    <mergeCell ref="C214:E214"/>
-    <mergeCell ref="C215:E215"/>
-    <mergeCell ref="B220:E220"/>
-    <mergeCell ref="B221:E221"/>
-    <mergeCell ref="B222:E222"/>
-    <mergeCell ref="B223:E223"/>
-    <mergeCell ref="B224:E224"/>
-    <mergeCell ref="D236:F236"/>
-    <mergeCell ref="D237:F237"/>
-    <mergeCell ref="D243:F243"/>
-    <mergeCell ref="D230:F230"/>
-    <mergeCell ref="D231:F231"/>
-    <mergeCell ref="D232:F232"/>
-    <mergeCell ref="D233:F233"/>
-    <mergeCell ref="D234:F234"/>
-    <mergeCell ref="D235:F235"/>
+    <mergeCell ref="B174:B176"/>
+    <mergeCell ref="F111:N111"/>
+    <mergeCell ref="B148:B160"/>
+    <mergeCell ref="B161:B162"/>
+    <mergeCell ref="B163:B165"/>
+    <mergeCell ref="B166:B173"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -11785,18 +11787,18 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
+      <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
-      <selection activeCell="E26" sqref="E26"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
i408--Apollo eit2 suite added
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/radiant/silicon_07_apollo.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/radiant/silicon_07_apollo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\repository\tmp_client\doc\TMP_EIT_suites\radiant\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="pSvbrBtM5D7J1tTbaFvNMFAx+gsFF1+zjWgivCK1irAkzVtGcdIaviGYDMewqTuAFCctlIpswoSn4Z8ezPPc6w==" workbookSaltValue="fuR2EkRIGc7n0eTkIKsWWA==" workbookSpinCount="100000" lockStructure="1"/>
@@ -27,10 +27,10 @@
   </definedNames>
   <calcPr calcId="122211"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jeffrey Ye - Personal View" guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="3"/>
+    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
+    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
     <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
-    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
-    <customWorkbookView name="Jeffrey Ye - Personal View" guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="3"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -1164,9 +1164,6 @@
     <t>=SoftIP</t>
   </si>
   <si>
-    <t xml:space="preserve">cmd = python DEV/bin/run_radiant.py  --run-map-trce --run-par-trce  --run-export-bitstream --set-strategy="{par_disable_timing_driven=True}" </t>
-  </si>
-  <si>
     <t>ITR1/01_Logic/01_impl/101_LUT4</t>
   </si>
   <si>
@@ -1780,6 +1777,9 @@
   </si>
   <si>
     <t>cmd = --check-conf=impl.conf --synthesis=synplify --check-smart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cmd = python DEV/bin/run_radiant.py  --run-map-trce --run-par-trce  --set-strategy="{par_disable_timing_driven=True}" </t>
   </si>
 </sst>
 </file>
@@ -3094,20 +3094,59 @@
     <xf numFmtId="49" fontId="12" fillId="7" borderId="7" xfId="13" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3115,12 +3154,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3130,13 +3163,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
@@ -3156,44 +3183,17 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="48" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -6071,11 +6071,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28" style="2" customWidth="1"/>
@@ -6103,7 +6103,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -6111,12 +6111,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="B5" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -6129,7 +6129,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>365</v>
+        <v>570</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -6248,7 +6248,7 @@
         <v>5</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -6297,23 +6297,23 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="G15" sqref="G15"/>
+    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" topLeftCell="A2">
+      <selection activeCell="C52" sqref="C52"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="B4" sqref="B4"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="B35" sqref="B35"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-    </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="B4" sqref="B4"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" topLeftCell="A2">
-      <selection activeCell="C52" sqref="C52"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
@@ -6336,36 +6336,36 @@
       <selection pane="bottomRight" activeCell="E120" sqref="E120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="2" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="60.140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="60.109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20.88671875" style="2" customWidth="1"/>
     <col min="7" max="7" width="24" style="2" customWidth="1"/>
     <col min="8" max="8" width="37" style="2" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" style="2" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5546875" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="38" style="2" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="30.28515625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="19.44140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="30.33203125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="17.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.44140625" style="2" customWidth="1"/>
     <col min="18" max="18" width="13" style="2" customWidth="1"/>
-    <col min="19" max="20" width="9.7109375" style="2" customWidth="1"/>
-    <col min="21" max="21" width="9.42578125" style="2" customWidth="1"/>
+    <col min="19" max="20" width="9.6640625" style="2" customWidth="1"/>
+    <col min="21" max="21" width="9.44140625" style="2" customWidth="1"/>
     <col min="22" max="22" width="11" style="2" customWidth="1"/>
-    <col min="23" max="23" width="11.7109375" style="2" customWidth="1"/>
+    <col min="23" max="23" width="11.6640625" style="2" customWidth="1"/>
     <col min="24" max="29" width="9" style="2"/>
-    <col min="30" max="30" width="10.140625" style="2" customWidth="1"/>
+    <col min="30" max="30" width="10.109375" style="2" customWidth="1"/>
     <col min="31" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
+    <row r="1" spans="1:31" s="3" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="A1" s="69" t="s">
         <v>15</v>
       </c>
@@ -6402,7 +6402,7 @@
       <c r="AD1" s="72"/>
       <c r="AE1" s="72"/>
     </row>
-    <row r="2" spans="1:31" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
+    <row r="2" spans="1:31" s="3" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -6497,7 +6497,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="15.75" thickTop="1">
+    <row r="3" spans="1:31" ht="15" thickTop="1">
       <c r="A3" s="2" t="s">
         <v>40</v>
       </c>
@@ -6505,7 +6505,7 @@
         <v>296</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F3" s="2">
         <v>1</v>
@@ -6534,7 +6534,7 @@
         <v>296</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
@@ -6563,7 +6563,7 @@
         <v>296</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>40</v>
@@ -6592,7 +6592,7 @@
         <v>296</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>40</v>
@@ -6621,7 +6621,7 @@
         <v>296</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>40</v>
@@ -6650,7 +6650,7 @@
         <v>296</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>40</v>
@@ -6679,7 +6679,7 @@
         <v>296</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>40</v>
@@ -6708,7 +6708,7 @@
         <v>296</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>40</v>
@@ -6737,7 +6737,7 @@
         <v>296</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>40</v>
@@ -6766,7 +6766,7 @@
         <v>296</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>40</v>
@@ -6795,7 +6795,7 @@
         <v>296</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>40</v>
@@ -6824,7 +6824,7 @@
         <v>296</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>40</v>
@@ -6853,7 +6853,7 @@
         <v>296</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>40</v>
@@ -6882,7 +6882,7 @@
         <v>296</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>40</v>
@@ -6911,7 +6911,7 @@
         <v>296</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>40</v>
@@ -6940,7 +6940,7 @@
         <v>296</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>40</v>
@@ -6969,7 +6969,7 @@
         <v>296</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>40</v>
@@ -6998,7 +6998,7 @@
         <v>296</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>40</v>
@@ -7027,7 +7027,7 @@
         <v>296</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>40</v>
@@ -7056,7 +7056,7 @@
         <v>296</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>40</v>
@@ -7085,7 +7085,7 @@
         <v>296</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>40</v>
@@ -7114,7 +7114,7 @@
         <v>296</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>40</v>
@@ -7143,7 +7143,7 @@
         <v>327</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>40</v>
@@ -7172,7 +7172,7 @@
         <v>330</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>40</v>
@@ -7198,7 +7198,7 @@
         <v>330</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>40</v>
@@ -7224,7 +7224,7 @@
         <v>330</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>40</v>
@@ -7250,7 +7250,7 @@
         <v>330</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>40</v>
@@ -7276,7 +7276,7 @@
         <v>330</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>40</v>
@@ -7302,7 +7302,7 @@
         <v>330</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>40</v>
@@ -7328,7 +7328,7 @@
         <v>330</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>40</v>
@@ -7354,7 +7354,7 @@
         <v>329</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>40</v>
@@ -7377,7 +7377,7 @@
         <v>329</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>40</v>
@@ -7400,7 +7400,7 @@
         <v>329</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>40</v>
@@ -7423,7 +7423,7 @@
         <v>329</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>40</v>
@@ -7446,7 +7446,7 @@
         <v>343</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>40</v>
@@ -7469,7 +7469,7 @@
         <v>343</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>40</v>
@@ -7492,7 +7492,7 @@
         <v>343</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>40</v>
@@ -7515,7 +7515,7 @@
         <v>343</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>40</v>
@@ -7538,7 +7538,7 @@
         <v>343</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>40</v>
@@ -7561,7 +7561,7 @@
         <v>343</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>40</v>
@@ -7584,7 +7584,7 @@
         <v>343</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>40</v>
@@ -7607,7 +7607,7 @@
         <v>343</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>40</v>
@@ -7630,7 +7630,7 @@
         <v>343</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>40</v>
@@ -7653,7 +7653,7 @@
         <v>343</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>40</v>
@@ -7676,7 +7676,7 @@
         <v>343</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>40</v>
@@ -7699,7 +7699,7 @@
         <v>343</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>40</v>
@@ -7722,7 +7722,7 @@
         <v>343</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>40</v>
@@ -7745,7 +7745,7 @@
         <v>343</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>40</v>
@@ -7768,7 +7768,7 @@
         <v>343</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>40</v>
@@ -7791,7 +7791,7 @@
         <v>343</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>40</v>
@@ -7814,7 +7814,7 @@
         <v>343</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>40</v>
@@ -7837,7 +7837,7 @@
         <v>343</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>40</v>
@@ -7854,19 +7854,19 @@
     </row>
     <row r="55" spans="1:31">
       <c r="A55" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D55" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="G55" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="G55" s="2" t="s">
+      <c r="H55" s="2" t="s">
         <v>432</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>433</v>
       </c>
       <c r="S55" s="2" t="s">
         <v>301</v>
@@ -7880,19 +7880,19 @@
     </row>
     <row r="56" spans="1:31">
       <c r="A56" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E56" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="G56" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="G56" s="2" t="s">
+      <c r="H56" s="2" t="s">
         <v>435</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>436</v>
       </c>
       <c r="S56" s="2" t="s">
         <v>301</v>
@@ -7906,19 +7906,19 @@
     </row>
     <row r="57" spans="1:31">
       <c r="A57" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E57" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="G57" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="G57" s="2" t="s">
+      <c r="H57" s="2" t="s">
         <v>438</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>439</v>
       </c>
       <c r="S57" s="2" t="s">
         <v>301</v>
@@ -7932,19 +7932,19 @@
     </row>
     <row r="58" spans="1:31">
       <c r="A58" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E58" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="G58" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="G58" s="2" t="s">
+      <c r="H58" s="2" t="s">
         <v>441</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>442</v>
       </c>
       <c r="S58" s="2" t="s">
         <v>301</v>
@@ -7958,19 +7958,19 @@
     </row>
     <row r="59" spans="1:31">
       <c r="A59" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E59" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="G59" s="2" t="s">
         <v>443</v>
       </c>
-      <c r="G59" s="2" t="s">
+      <c r="H59" s="2" t="s">
         <v>444</v>
-      </c>
-      <c r="H59" s="2" t="s">
-        <v>445</v>
       </c>
       <c r="S59" s="2" t="s">
         <v>301</v>
@@ -7984,19 +7984,19 @@
     </row>
     <row r="60" spans="1:31">
       <c r="A60" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E60" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="G60" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="G60" s="2" t="s">
+      <c r="H60" s="2" t="s">
         <v>447</v>
-      </c>
-      <c r="H60" s="2" t="s">
-        <v>448</v>
       </c>
       <c r="S60" s="2" t="s">
         <v>301</v>
@@ -8010,19 +8010,19 @@
     </row>
     <row r="61" spans="1:31">
       <c r="A61" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E61" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="G61" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="G61" s="2" t="s">
+      <c r="H61" s="2" t="s">
         <v>450</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>451</v>
       </c>
       <c r="S61" s="2" t="s">
         <v>301</v>
@@ -8036,19 +8036,19 @@
     </row>
     <row r="62" spans="1:31">
       <c r="A62" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E62" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="G62" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="G62" s="2" t="s">
+      <c r="H62" s="2" t="s">
         <v>453</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>454</v>
       </c>
       <c r="S62" s="2" t="s">
         <v>301</v>
@@ -8062,19 +8062,19 @@
     </row>
     <row r="63" spans="1:31">
       <c r="A63" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G63" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="H63" s="2" t="s">
         <v>432</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>433</v>
       </c>
       <c r="S63" s="2" t="s">
         <v>301</v>
@@ -8088,19 +8088,19 @@
     </row>
     <row r="64" spans="1:31">
       <c r="A64" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G64" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="H64" s="2" t="s">
         <v>435</v>
-      </c>
-      <c r="H64" s="2" t="s">
-        <v>436</v>
       </c>
       <c r="S64" s="2" t="s">
         <v>301</v>
@@ -8114,19 +8114,19 @@
     </row>
     <row r="65" spans="1:31">
       <c r="A65" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E65" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="H65" s="2" t="s">
         <v>457</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="H65" s="2" t="s">
-        <v>458</v>
       </c>
       <c r="S65" s="2" t="s">
         <v>301</v>
@@ -8140,19 +8140,19 @@
     </row>
     <row r="66" spans="1:31">
       <c r="A66" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D66" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="D66" s="2" t="s">
-        <v>430</v>
-      </c>
       <c r="E66" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="H66" s="2" t="s">
         <v>459</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="H66" s="2" t="s">
-        <v>460</v>
       </c>
       <c r="S66" s="2" t="s">
         <v>301</v>
@@ -8166,19 +8166,19 @@
     </row>
     <row r="67" spans="1:31">
       <c r="A67" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G67" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="H67" s="2" t="s">
         <v>444</v>
-      </c>
-      <c r="H67" s="2" t="s">
-        <v>445</v>
       </c>
       <c r="S67" s="2" t="s">
         <v>301</v>
@@ -8192,19 +8192,19 @@
     </row>
     <row r="68" spans="1:31">
       <c r="A68" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="G68" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="H68" s="2" t="s">
         <v>447</v>
-      </c>
-      <c r="H68" s="2" t="s">
-        <v>448</v>
       </c>
       <c r="S68" s="2" t="s">
         <v>301</v>
@@ -8218,19 +8218,19 @@
     </row>
     <row r="69" spans="1:31">
       <c r="A69" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E69" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="H69" s="2" t="s">
         <v>463</v>
-      </c>
-      <c r="G69" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="H69" s="2" t="s">
-        <v>464</v>
       </c>
       <c r="S69" s="2" t="s">
         <v>301</v>
@@ -8244,19 +8244,19 @@
     </row>
     <row r="70" spans="1:31">
       <c r="A70" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E70" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="H70" s="2" t="s">
         <v>465</v>
-      </c>
-      <c r="G70" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="H70" s="2" t="s">
-        <v>466</v>
       </c>
       <c r="S70" s="2" t="s">
         <v>301</v>
@@ -8270,16 +8270,16 @@
     </row>
     <row r="71" spans="1:31">
       <c r="A71" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>117</v>
       </c>
       <c r="E71" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="H71" s="2" t="s">
         <v>467</v>
-      </c>
-      <c r="H71" s="2" t="s">
-        <v>468</v>
       </c>
       <c r="S71" s="2" t="s">
         <v>301</v>
@@ -8293,16 +8293,16 @@
     </row>
     <row r="72" spans="1:31">
       <c r="A72" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>117</v>
       </c>
       <c r="E72" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="H72" s="2" t="s">
         <v>469</v>
-      </c>
-      <c r="H72" s="2" t="s">
-        <v>470</v>
       </c>
       <c r="S72" s="2" t="s">
         <v>301</v>
@@ -8316,19 +8316,19 @@
     </row>
     <row r="73" spans="1:31">
       <c r="A73" s="2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>117</v>
       </c>
       <c r="E73" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="G73" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="G73" s="2" t="s">
+      <c r="H73" s="2" t="s">
         <v>472</v>
-      </c>
-      <c r="H73" s="2" t="s">
-        <v>473</v>
       </c>
       <c r="S73" s="2" t="s">
         <v>301</v>
@@ -8342,19 +8342,19 @@
     </row>
     <row r="74" spans="1:31">
       <c r="A74" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>117</v>
       </c>
       <c r="E74" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="G74" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="G74" s="2" t="s">
+      <c r="H74" s="2" t="s">
         <v>476</v>
-      </c>
-      <c r="H74" s="2" t="s">
-        <v>477</v>
       </c>
       <c r="S74" s="2" t="s">
         <v>301</v>
@@ -8368,16 +8368,16 @@
     </row>
     <row r="75" spans="1:31">
       <c r="A75" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>117</v>
       </c>
       <c r="E75" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="H75" s="2" t="s">
         <v>478</v>
-      </c>
-      <c r="H75" s="2" t="s">
-        <v>479</v>
       </c>
       <c r="S75" s="2" t="s">
         <v>301</v>
@@ -8391,16 +8391,16 @@
     </row>
     <row r="76" spans="1:31">
       <c r="A76" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>117</v>
       </c>
       <c r="E76" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="H76" s="2" t="s">
         <v>481</v>
-      </c>
-      <c r="H76" s="2" t="s">
-        <v>482</v>
       </c>
       <c r="S76" s="2" t="s">
         <v>301</v>
@@ -8414,16 +8414,16 @@
     </row>
     <row r="77" spans="1:31">
       <c r="A77" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>117</v>
       </c>
       <c r="E77" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="H77" s="2" t="s">
         <v>483</v>
-      </c>
-      <c r="H77" s="2" t="s">
-        <v>484</v>
       </c>
       <c r="S77" s="2" t="s">
         <v>301</v>
@@ -8437,16 +8437,16 @@
     </row>
     <row r="78" spans="1:31">
       <c r="A78" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>117</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="S78" s="2" t="s">
         <v>301</v>
@@ -8460,19 +8460,19 @@
     </row>
     <row r="79" spans="1:31">
       <c r="A79" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>117</v>
       </c>
       <c r="E79" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="H79" s="2" t="s">
         <v>562</v>
-      </c>
-      <c r="G79" s="2" t="s">
-        <v>472</v>
-      </c>
-      <c r="H79" s="2" t="s">
-        <v>563</v>
       </c>
       <c r="S79" s="2" t="s">
         <v>301</v>
@@ -8486,19 +8486,19 @@
     </row>
     <row r="80" spans="1:31">
       <c r="A80" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>117</v>
       </c>
       <c r="E80" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="H80" s="2" t="s">
         <v>564</v>
-      </c>
-      <c r="G80" s="2" t="s">
-        <v>476</v>
-      </c>
-      <c r="H80" s="2" t="s">
-        <v>565</v>
       </c>
       <c r="S80" s="2" t="s">
         <v>301</v>
@@ -8512,16 +8512,16 @@
     </row>
     <row r="81" spans="1:31">
       <c r="A81" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>117</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="S81" s="2" t="s">
         <v>301</v>
@@ -8535,16 +8535,16 @@
     </row>
     <row r="82" spans="1:31">
       <c r="A82" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>117</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="S82" s="2" t="s">
         <v>301</v>
@@ -8558,13 +8558,13 @@
     </row>
     <row r="83" spans="1:31">
       <c r="A83" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="S83" s="2" t="s">
         <v>301</v>
@@ -8578,13 +8578,13 @@
     </row>
     <row r="84" spans="1:31">
       <c r="A84" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="S84" s="2" t="s">
         <v>301</v>
@@ -8598,13 +8598,13 @@
     </row>
     <row r="85" spans="1:31">
       <c r="A85" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="S85" s="2" t="s">
         <v>301</v>
@@ -8618,16 +8618,16 @@
     </row>
     <row r="86" spans="1:31">
       <c r="A86" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E86" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="H86" s="2" t="s">
         <v>488</v>
-      </c>
-      <c r="H86" s="2" t="s">
-        <v>489</v>
       </c>
       <c r="S86" s="2" t="s">
         <v>301</v>
@@ -8641,16 +8641,16 @@
     </row>
     <row r="87" spans="1:31">
       <c r="A87" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="S87" s="2" t="s">
         <v>301</v>
@@ -8664,13 +8664,13 @@
     </row>
     <row r="88" spans="1:31">
       <c r="A88" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="S88" s="2" t="s">
         <v>301</v>
@@ -8684,13 +8684,13 @@
     </row>
     <row r="89" spans="1:31">
       <c r="A89" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="S89" s="2" t="s">
         <v>301</v>
@@ -8704,13 +8704,13 @@
     </row>
     <row r="90" spans="1:31">
       <c r="A90" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="S90" s="2" t="s">
         <v>301</v>
@@ -8724,13 +8724,13 @@
     </row>
     <row r="91" spans="1:31">
       <c r="A91" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="S91" s="2" t="s">
         <v>301</v>
@@ -8744,16 +8744,16 @@
     </row>
     <row r="92" spans="1:31">
       <c r="A92" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E92" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="H92" s="2" t="s">
         <v>491</v>
-      </c>
-      <c r="H92" s="2" t="s">
-        <v>492</v>
       </c>
       <c r="S92" s="2" t="s">
         <v>301</v>
@@ -8767,16 +8767,16 @@
     </row>
     <row r="93" spans="1:31">
       <c r="A93" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="S93" s="2" t="s">
         <v>301</v>
@@ -8790,13 +8790,13 @@
     </row>
     <row r="94" spans="1:31">
       <c r="A94" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="S94" s="2" t="s">
         <v>301</v>
@@ -8810,16 +8810,16 @@
     </row>
     <row r="95" spans="1:31">
       <c r="A95" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>343</v>
       </c>
       <c r="E95" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="H95" s="2" t="s">
         <v>498</v>
-      </c>
-      <c r="H95" s="2" t="s">
-        <v>499</v>
       </c>
       <c r="S95" s="2" t="s">
         <v>343</v>
@@ -8833,16 +8833,16 @@
     </row>
     <row r="96" spans="1:31">
       <c r="A96" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>343</v>
       </c>
       <c r="E96" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="H96" s="2" t="s">
         <v>500</v>
-      </c>
-      <c r="H96" s="2" t="s">
-        <v>501</v>
       </c>
       <c r="S96" s="2" t="s">
         <v>343</v>
@@ -8856,16 +8856,16 @@
     </row>
     <row r="97" spans="1:31">
       <c r="A97" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>343</v>
       </c>
       <c r="E97" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="H97" s="2" t="s">
         <v>502</v>
-      </c>
-      <c r="H97" s="2" t="s">
-        <v>503</v>
       </c>
       <c r="S97" s="2" t="s">
         <v>343</v>
@@ -8879,16 +8879,16 @@
     </row>
     <row r="98" spans="1:31">
       <c r="A98" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>343</v>
       </c>
       <c r="E98" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="H98" s="2" t="s">
         <v>504</v>
-      </c>
-      <c r="H98" s="2" t="s">
-        <v>505</v>
       </c>
       <c r="S98" s="2" t="s">
         <v>343</v>
@@ -8902,16 +8902,16 @@
     </row>
     <row r="99" spans="1:31">
       <c r="A99" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>343</v>
       </c>
       <c r="E99" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="H99" s="2" t="s">
         <v>506</v>
-      </c>
-      <c r="H99" s="2" t="s">
-        <v>507</v>
       </c>
       <c r="S99" s="2" t="s">
         <v>343</v>
@@ -8925,16 +8925,16 @@
     </row>
     <row r="100" spans="1:31">
       <c r="A100" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>343</v>
       </c>
       <c r="E100" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="H100" s="2" t="s">
         <v>508</v>
-      </c>
-      <c r="H100" s="2" t="s">
-        <v>509</v>
       </c>
       <c r="S100" s="2" t="s">
         <v>343</v>
@@ -8948,16 +8948,16 @@
     </row>
     <row r="101" spans="1:31">
       <c r="A101" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>343</v>
       </c>
       <c r="E101" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H101" s="2" t="s">
         <v>510</v>
-      </c>
-      <c r="H101" s="2" t="s">
-        <v>511</v>
       </c>
       <c r="S101" s="2" t="s">
         <v>343</v>
@@ -8971,13 +8971,13 @@
     </row>
     <row r="102" spans="1:31">
       <c r="A102" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>343</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="S102" s="2" t="s">
         <v>343</v>
@@ -8991,13 +8991,13 @@
     </row>
     <row r="103" spans="1:31">
       <c r="A103" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>343</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="S103" s="2" t="s">
         <v>343</v>
@@ -9011,13 +9011,13 @@
     </row>
     <row r="104" spans="1:31">
       <c r="A104" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>343</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="S104" s="2" t="s">
         <v>343</v>
@@ -9031,13 +9031,13 @@
     </row>
     <row r="105" spans="1:31">
       <c r="A105" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>343</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="S105" s="2" t="s">
         <v>343</v>
@@ -9051,13 +9051,13 @@
     </row>
     <row r="106" spans="1:31">
       <c r="A106" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>343</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="S106" s="2" t="s">
         <v>343</v>
@@ -9071,13 +9071,13 @@
     </row>
     <row r="107" spans="1:31">
       <c r="A107" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>343</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="S107" s="2" t="s">
         <v>343</v>
@@ -9091,13 +9091,13 @@
     </row>
     <row r="108" spans="1:31">
       <c r="A108" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>343</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="S108" s="2" t="s">
         <v>343</v>
@@ -9189,18 +9189,18 @@
       <selection activeCell="C210" sqref="C210:E210"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="6" customWidth="1"/>
     <col min="2" max="2" width="19" style="6" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="15" style="6" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="24.88671875" style="6" customWidth="1"/>
     <col min="6" max="6" width="32" style="6" customWidth="1"/>
-    <col min="7" max="7" width="31.7109375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="28.140625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="31.6640625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="28.109375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" style="6" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" style="6" customWidth="1"/>
     <col min="11" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
@@ -9223,7 +9223,7 @@
     <row r="107" spans="1:14" ht="12.75" customHeight="1"/>
     <row r="108" spans="1:14" ht="12.75" customHeight="1"/>
     <row r="109" spans="1:14" ht="12.75" customHeight="1"/>
-    <row r="110" spans="1:14" ht="15.75" thickBot="1">
+    <row r="110" spans="1:14" ht="15" thickBot="1">
       <c r="A110" s="6" t="s">
         <v>81</v>
       </c>
@@ -9231,7 +9231,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="15.75" thickBot="1">
+    <row r="111" spans="1:14" ht="15" thickBot="1">
       <c r="A111" s="9" t="s">
         <v>83</v>
       </c>
@@ -9247,17 +9247,17 @@
       <c r="E111" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F111" s="75" t="s">
+      <c r="F111" s="106" t="s">
         <v>87</v>
       </c>
-      <c r="G111" s="76"/>
-      <c r="H111" s="76"/>
-      <c r="I111" s="76"/>
-      <c r="J111" s="76"/>
-      <c r="K111" s="76"/>
-      <c r="L111" s="76"/>
-      <c r="M111" s="76"/>
-      <c r="N111" s="77"/>
+      <c r="G111" s="107"/>
+      <c r="H111" s="107"/>
+      <c r="I111" s="107"/>
+      <c r="J111" s="107"/>
+      <c r="K111" s="107"/>
+      <c r="L111" s="107"/>
+      <c r="M111" s="107"/>
+      <c r="N111" s="108"/>
     </row>
     <row r="112" spans="1:14">
       <c r="A112" s="11" t="s">
@@ -10085,7 +10085,7 @@
       <c r="M142" s="18"/>
       <c r="N142" s="19"/>
     </row>
-    <row r="143" spans="1:14" ht="15.75" thickBot="1">
+    <row r="143" spans="1:14" ht="15" thickBot="1">
       <c r="A143" s="20" t="s">
         <v>122</v>
       </c>
@@ -10109,7 +10109,7 @@
       <c r="M143" s="21"/>
       <c r="N143" s="22"/>
     </row>
-    <row r="146" spans="1:8" ht="15.75" thickBot="1">
+    <row r="146" spans="1:8" ht="15" thickBot="1">
       <c r="A146" s="6" t="s">
         <v>123</v>
       </c>
@@ -10147,7 +10147,7 @@
       <c r="A148" s="26">
         <v>1</v>
       </c>
-      <c r="B148" s="78" t="s">
+      <c r="B148" s="91" t="s">
         <v>3</v>
       </c>
       <c r="C148" s="27" t="s">
@@ -10173,7 +10173,7 @@
       <c r="A149" s="26">
         <v>2</v>
       </c>
-      <c r="B149" s="79"/>
+      <c r="B149" s="92"/>
       <c r="C149" s="28" t="s">
         <v>136</v>
       </c>
@@ -10195,7 +10195,7 @@
       <c r="A150" s="26">
         <v>3</v>
       </c>
-      <c r="B150" s="79"/>
+      <c r="B150" s="92"/>
       <c r="C150" s="28" t="s">
         <v>9</v>
       </c>
@@ -10215,7 +10215,7 @@
       <c r="A151" s="26">
         <v>4</v>
       </c>
-      <c r="B151" s="79"/>
+      <c r="B151" s="92"/>
       <c r="C151" s="28" t="s">
         <v>138</v>
       </c>
@@ -10239,7 +10239,7 @@
       <c r="A152" s="26">
         <v>5</v>
       </c>
-      <c r="B152" s="79"/>
+      <c r="B152" s="92"/>
       <c r="C152" s="27" t="s">
         <v>140</v>
       </c>
@@ -10263,7 +10263,7 @@
       <c r="A153" s="26">
         <v>6</v>
       </c>
-      <c r="B153" s="79"/>
+      <c r="B153" s="92"/>
       <c r="C153" s="27" t="s">
         <v>144</v>
       </c>
@@ -10287,7 +10287,7 @@
       <c r="A154" s="26">
         <v>7</v>
       </c>
-      <c r="B154" s="79"/>
+      <c r="B154" s="92"/>
       <c r="C154" s="28" t="s">
         <v>147</v>
       </c>
@@ -10309,7 +10309,7 @@
       <c r="A155" s="26">
         <v>8</v>
       </c>
-      <c r="B155" s="79"/>
+      <c r="B155" s="92"/>
       <c r="C155" s="27" t="s">
         <v>148</v>
       </c>
@@ -10333,7 +10333,7 @@
       <c r="A156" s="26">
         <v>9</v>
       </c>
-      <c r="B156" s="79"/>
+      <c r="B156" s="92"/>
       <c r="C156" s="27" t="s">
         <v>149</v>
       </c>
@@ -10357,7 +10357,7 @@
       <c r="A157" s="26">
         <v>10</v>
       </c>
-      <c r="B157" s="79"/>
+      <c r="B157" s="92"/>
       <c r="C157" s="28" t="s">
         <v>150</v>
       </c>
@@ -10381,7 +10381,7 @@
       <c r="A158" s="26">
         <v>11</v>
       </c>
-      <c r="B158" s="79"/>
+      <c r="B158" s="92"/>
       <c r="C158" s="68" t="s">
         <v>151</v>
       </c>
@@ -10405,7 +10405,7 @@
       <c r="A159" s="26">
         <v>12</v>
       </c>
-      <c r="B159" s="79"/>
+      <c r="B159" s="92"/>
       <c r="C159" s="28" t="s">
         <v>153</v>
       </c>
@@ -10427,7 +10427,7 @@
       <c r="A160" s="26">
         <v>13</v>
       </c>
-      <c r="B160" s="80"/>
+      <c r="B160" s="86"/>
       <c r="C160" s="28" t="s">
         <v>56</v>
       </c>
@@ -10451,7 +10451,7 @@
       <c r="A161" s="26">
         <v>14</v>
       </c>
-      <c r="B161" s="73" t="s">
+      <c r="B161" s="82" t="s">
         <v>4</v>
       </c>
       <c r="C161" s="28" t="s">
@@ -10477,7 +10477,7 @@
       <c r="A162" s="26">
         <v>15</v>
       </c>
-      <c r="B162" s="74"/>
+      <c r="B162" s="81"/>
       <c r="C162" s="28" t="s">
         <v>161</v>
       </c>
@@ -10501,7 +10501,7 @@
       <c r="A163" s="26">
         <v>16</v>
       </c>
-      <c r="B163" s="78" t="s">
+      <c r="B163" s="91" t="s">
         <v>5</v>
       </c>
       <c r="C163" s="28" t="s">
@@ -10525,7 +10525,7 @@
       <c r="A164" s="26">
         <v>17</v>
       </c>
-      <c r="B164" s="81"/>
+      <c r="B164" s="109"/>
       <c r="C164" s="27" t="s">
         <v>165</v>
       </c>
@@ -10547,7 +10547,7 @@
       <c r="A165" s="26">
         <v>18</v>
       </c>
-      <c r="B165" s="80"/>
+      <c r="B165" s="86"/>
       <c r="C165" s="27" t="s">
         <v>167</v>
       </c>
@@ -10567,7 +10567,7 @@
       <c r="A166" s="26">
         <v>19</v>
       </c>
-      <c r="B166" s="73" t="s">
+      <c r="B166" s="82" t="s">
         <v>6</v>
       </c>
       <c r="C166" s="28" t="s">
@@ -10591,7 +10591,7 @@
       <c r="A167" s="26">
         <v>20</v>
       </c>
-      <c r="B167" s="74"/>
+      <c r="B167" s="81"/>
       <c r="C167" s="28" t="s">
         <v>172</v>
       </c>
@@ -10611,7 +10611,7 @@
       <c r="A168" s="26">
         <v>21</v>
       </c>
-      <c r="B168" s="74"/>
+      <c r="B168" s="81"/>
       <c r="C168" s="28" t="s">
         <v>173</v>
       </c>
@@ -10631,7 +10631,7 @@
       <c r="A169" s="26">
         <v>22</v>
       </c>
-      <c r="B169" s="74"/>
+      <c r="B169" s="81"/>
       <c r="C169" s="28" t="s">
         <v>174</v>
       </c>
@@ -10651,7 +10651,7 @@
       <c r="A170" s="26">
         <v>23</v>
       </c>
-      <c r="B170" s="74"/>
+      <c r="B170" s="81"/>
       <c r="C170" s="28" t="s">
         <v>175</v>
       </c>
@@ -10671,7 +10671,7 @@
       <c r="A171" s="26">
         <v>24</v>
       </c>
-      <c r="B171" s="74"/>
+      <c r="B171" s="81"/>
       <c r="C171" s="28" t="s">
         <v>176</v>
       </c>
@@ -10691,7 +10691,7 @@
       <c r="A172" s="26">
         <v>25</v>
       </c>
-      <c r="B172" s="74"/>
+      <c r="B172" s="81"/>
       <c r="C172" s="28" t="s">
         <v>177</v>
       </c>
@@ -10711,7 +10711,7 @@
       <c r="A173" s="26">
         <v>26</v>
       </c>
-      <c r="B173" s="74"/>
+      <c r="B173" s="81"/>
       <c r="C173" s="28" t="s">
         <v>41</v>
       </c>
@@ -10727,11 +10727,11 @@
       </c>
       <c r="H173" s="16"/>
     </row>
-    <row r="174" spans="1:8" ht="90">
+    <row r="174" spans="1:8" ht="86.4">
       <c r="A174" s="26">
         <v>27</v>
       </c>
-      <c r="B174" s="73" t="s">
+      <c r="B174" s="82" t="s">
         <v>7</v>
       </c>
       <c r="C174" s="28" t="s">
@@ -10755,7 +10755,7 @@
       <c r="A175" s="26">
         <v>28</v>
       </c>
-      <c r="B175" s="74"/>
+      <c r="B175" s="81"/>
       <c r="C175" s="27" t="s">
         <v>181</v>
       </c>
@@ -10777,7 +10777,7 @@
       <c r="A176" s="26">
         <v>29</v>
       </c>
-      <c r="B176" s="74"/>
+      <c r="B176" s="81"/>
       <c r="C176" s="28" t="s">
         <v>184</v>
       </c>
@@ -10799,7 +10799,7 @@
       <c r="A177" s="26">
         <v>30</v>
       </c>
-      <c r="B177" s="78" t="s">
+      <c r="B177" s="91" t="s">
         <v>8</v>
       </c>
       <c r="C177" s="28" t="s">
@@ -10821,11 +10821,11 @@
         <v>38</v>
       </c>
     </row>
-    <row r="178" spans="1:8" ht="15.75" thickBot="1">
+    <row r="178" spans="1:8" ht="15" thickBot="1">
       <c r="A178" s="31">
         <v>31</v>
       </c>
-      <c r="B178" s="79"/>
+      <c r="B178" s="92"/>
       <c r="C178" s="32" t="s">
         <v>189</v>
       </c>
@@ -10849,7 +10849,7 @@
       <c r="A179" s="23">
         <v>32</v>
       </c>
-      <c r="B179" s="82" t="s">
+      <c r="B179" s="93" t="s">
         <v>191</v>
       </c>
       <c r="C179" s="33" t="s">
@@ -10873,7 +10873,7 @@
       <c r="A180" s="26">
         <v>33</v>
       </c>
-      <c r="B180" s="83"/>
+      <c r="B180" s="94"/>
       <c r="C180" s="27" t="s">
         <v>195</v>
       </c>
@@ -10895,7 +10895,7 @@
       <c r="A181" s="26">
         <v>34</v>
       </c>
-      <c r="B181" s="84"/>
+      <c r="B181" s="95"/>
       <c r="C181" s="34" t="s">
         <v>198</v>
       </c>
@@ -10917,7 +10917,7 @@
       <c r="A182" s="31">
         <v>35</v>
       </c>
-      <c r="B182" s="84"/>
+      <c r="B182" s="95"/>
       <c r="C182" s="34" t="s">
         <v>199</v>
       </c>
@@ -10939,7 +10939,7 @@
       <c r="A183" s="31">
         <v>36</v>
       </c>
-      <c r="B183" s="84"/>
+      <c r="B183" s="95"/>
       <c r="C183" s="34" t="s">
         <v>202</v>
       </c>
@@ -10959,7 +10959,7 @@
       <c r="A184" s="31">
         <v>37</v>
       </c>
-      <c r="B184" s="84"/>
+      <c r="B184" s="95"/>
       <c r="C184" s="34" t="s">
         <v>254</v>
       </c>
@@ -10977,11 +10977,11 @@
         <v>257</v>
       </c>
     </row>
-    <row r="185" spans="1:8" ht="15.75" thickBot="1">
+    <row r="185" spans="1:8" ht="15" thickBot="1">
       <c r="A185" s="35">
         <v>38</v>
       </c>
-      <c r="B185" s="85"/>
+      <c r="B185" s="90"/>
       <c r="C185" s="36" t="s">
         <v>258</v>
       </c>
@@ -11017,7 +11017,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="198" spans="1:7" ht="15.75" thickBot="1">
+    <row r="198" spans="1:7" ht="15" thickBot="1">
       <c r="A198" s="6" t="s">
         <v>207</v>
       </c>
@@ -11032,11 +11032,11 @@
       <c r="B199" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="C199" s="86" t="s">
+      <c r="C199" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="D199" s="86"/>
-      <c r="E199" s="86"/>
+      <c r="D199" s="96"/>
+      <c r="E199" s="96"/>
       <c r="F199" s="39" t="s">
         <v>43</v>
       </c>
@@ -11045,17 +11045,17 @@
       </c>
     </row>
     <row r="200" spans="1:7">
-      <c r="A200" s="87" t="s">
+      <c r="A200" s="79" t="s">
         <v>212</v>
       </c>
-      <c r="B200" s="74" t="s">
+      <c r="B200" s="81" t="s">
         <v>213</v>
       </c>
-      <c r="C200" s="89" t="s">
+      <c r="C200" s="98" t="s">
         <v>57</v>
       </c>
-      <c r="D200" s="90"/>
-      <c r="E200" s="90"/>
+      <c r="D200" s="99"/>
+      <c r="E200" s="99"/>
       <c r="F200" s="28" t="s">
         <v>214</v>
       </c>
@@ -11064,13 +11064,13 @@
       </c>
     </row>
     <row r="201" spans="1:7">
-      <c r="A201" s="87"/>
-      <c r="B201" s="88"/>
-      <c r="C201" s="91" t="s">
+      <c r="A201" s="79"/>
+      <c r="B201" s="97"/>
+      <c r="C201" s="100" t="s">
         <v>57</v>
       </c>
-      <c r="D201" s="92"/>
-      <c r="E201" s="92"/>
+      <c r="D201" s="101"/>
+      <c r="E201" s="101"/>
       <c r="F201" s="32" t="s">
         <v>215</v>
       </c>
@@ -11079,15 +11079,15 @@
       </c>
     </row>
     <row r="202" spans="1:7">
-      <c r="A202" s="87"/>
-      <c r="B202" s="74" t="s">
+      <c r="A202" s="79"/>
+      <c r="B202" s="81" t="s">
         <v>216</v>
       </c>
-      <c r="C202" s="93" t="s">
+      <c r="C202" s="102" t="s">
         <v>217</v>
       </c>
-      <c r="D202" s="93"/>
-      <c r="E202" s="93"/>
+      <c r="D202" s="102"/>
+      <c r="E202" s="102"/>
       <c r="F202" s="28" t="s">
         <v>214</v>
       </c>
@@ -11096,13 +11096,13 @@
       </c>
     </row>
     <row r="203" spans="1:7">
-      <c r="A203" s="87"/>
-      <c r="B203" s="74"/>
-      <c r="C203" s="91" t="s">
+      <c r="A203" s="79"/>
+      <c r="B203" s="81"/>
+      <c r="C203" s="100" t="s">
         <v>217</v>
       </c>
-      <c r="D203" s="91"/>
-      <c r="E203" s="91"/>
+      <c r="D203" s="100"/>
+      <c r="E203" s="100"/>
       <c r="F203" s="28" t="s">
         <v>215</v>
       </c>
@@ -11111,15 +11111,15 @@
       </c>
     </row>
     <row r="204" spans="1:7">
-      <c r="A204" s="87"/>
-      <c r="B204" s="88" t="s">
+      <c r="A204" s="79"/>
+      <c r="B204" s="97" t="s">
         <v>218</v>
       </c>
-      <c r="C204" s="94" t="s">
+      <c r="C204" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="D204" s="95"/>
-      <c r="E204" s="96"/>
+      <c r="D204" s="104"/>
+      <c r="E204" s="105"/>
       <c r="F204" s="28" t="s">
         <v>214</v>
       </c>
@@ -11128,13 +11128,13 @@
       </c>
     </row>
     <row r="205" spans="1:7">
-      <c r="A205" s="87"/>
-      <c r="B205" s="80"/>
-      <c r="C205" s="94" t="s">
+      <c r="A205" s="79"/>
+      <c r="B205" s="86"/>
+      <c r="C205" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="D205" s="95"/>
-      <c r="E205" s="96"/>
+      <c r="D205" s="104"/>
+      <c r="E205" s="105"/>
       <c r="F205" s="28" t="s">
         <v>215</v>
       </c>
@@ -11143,15 +11143,15 @@
       </c>
     </row>
     <row r="206" spans="1:7">
-      <c r="A206" s="87"/>
-      <c r="B206" s="74" t="s">
+      <c r="A206" s="79"/>
+      <c r="B206" s="81" t="s">
         <v>219</v>
       </c>
-      <c r="C206" s="93" t="s">
+      <c r="C206" s="102" t="s">
         <v>220</v>
       </c>
-      <c r="D206" s="93"/>
-      <c r="E206" s="93"/>
+      <c r="D206" s="102"/>
+      <c r="E206" s="102"/>
       <c r="F206" s="28" t="s">
         <v>214</v>
       </c>
@@ -11160,13 +11160,13 @@
       </c>
     </row>
     <row r="207" spans="1:7">
-      <c r="A207" s="87"/>
-      <c r="B207" s="74"/>
-      <c r="C207" s="93" t="s">
+      <c r="A207" s="79"/>
+      <c r="B207" s="81"/>
+      <c r="C207" s="102" t="s">
         <v>220</v>
       </c>
-      <c r="D207" s="93"/>
-      <c r="E207" s="93"/>
+      <c r="D207" s="102"/>
+      <c r="E207" s="102"/>
       <c r="F207" s="28" t="s">
         <v>215</v>
       </c>
@@ -11175,17 +11175,17 @@
       </c>
     </row>
     <row r="208" spans="1:7">
-      <c r="A208" s="87" t="s">
+      <c r="A208" s="79" t="s">
         <v>221</v>
       </c>
-      <c r="B208" s="74" t="s">
+      <c r="B208" s="81" t="s">
         <v>222</v>
       </c>
-      <c r="C208" s="73" t="s">
+      <c r="C208" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="D208" s="74"/>
-      <c r="E208" s="74"/>
+      <c r="D208" s="81"/>
+      <c r="E208" s="81"/>
       <c r="F208" s="28" t="s">
         <v>214</v>
       </c>
@@ -11194,13 +11194,13 @@
       </c>
     </row>
     <row r="209" spans="1:7">
-      <c r="A209" s="87"/>
-      <c r="B209" s="74"/>
-      <c r="C209" s="74" t="s">
+      <c r="A209" s="79"/>
+      <c r="B209" s="81"/>
+      <c r="C209" s="81" t="s">
         <v>46</v>
       </c>
-      <c r="D209" s="74"/>
-      <c r="E209" s="74"/>
+      <c r="D209" s="81"/>
+      <c r="E209" s="81"/>
       <c r="F209" s="28" t="s">
         <v>215</v>
       </c>
@@ -11209,15 +11209,15 @@
       </c>
     </row>
     <row r="210" spans="1:7">
-      <c r="A210" s="87"/>
-      <c r="B210" s="74" t="s">
+      <c r="A210" s="79"/>
+      <c r="B210" s="81" t="s">
         <v>224</v>
       </c>
-      <c r="C210" s="73" t="s">
+      <c r="C210" s="82" t="s">
         <v>47</v>
       </c>
-      <c r="D210" s="74"/>
-      <c r="E210" s="74"/>
+      <c r="D210" s="81"/>
+      <c r="E210" s="81"/>
       <c r="F210" s="28" t="s">
         <v>214</v>
       </c>
@@ -11226,13 +11226,13 @@
       </c>
     </row>
     <row r="211" spans="1:7">
-      <c r="A211" s="87"/>
-      <c r="B211" s="74"/>
-      <c r="C211" s="74" t="s">
+      <c r="A211" s="79"/>
+      <c r="B211" s="81"/>
+      <c r="C211" s="81" t="s">
         <v>48</v>
       </c>
-      <c r="D211" s="74"/>
-      <c r="E211" s="74"/>
+      <c r="D211" s="81"/>
+      <c r="E211" s="81"/>
       <c r="F211" s="28" t="s">
         <v>215</v>
       </c>
@@ -11241,17 +11241,17 @@
       </c>
     </row>
     <row r="212" spans="1:7">
-      <c r="A212" s="87" t="s">
+      <c r="A212" s="79" t="s">
         <v>225</v>
       </c>
-      <c r="B212" s="74" t="s">
+      <c r="B212" s="81" t="s">
         <v>226</v>
       </c>
-      <c r="C212" s="73" t="s">
+      <c r="C212" s="82" t="s">
         <v>49</v>
       </c>
-      <c r="D212" s="74"/>
-      <c r="E212" s="74"/>
+      <c r="D212" s="81"/>
+      <c r="E212" s="81"/>
       <c r="F212" s="28" t="s">
         <v>214</v>
       </c>
@@ -11260,13 +11260,13 @@
       </c>
     </row>
     <row r="213" spans="1:7">
-      <c r="A213" s="87"/>
-      <c r="B213" s="74"/>
-      <c r="C213" s="74" t="s">
+      <c r="A213" s="79"/>
+      <c r="B213" s="81"/>
+      <c r="C213" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="D213" s="74"/>
-      <c r="E213" s="74"/>
+      <c r="D213" s="81"/>
+      <c r="E213" s="81"/>
       <c r="F213" s="28" t="s">
         <v>215</v>
       </c>
@@ -11275,15 +11275,15 @@
       </c>
     </row>
     <row r="214" spans="1:7">
-      <c r="A214" s="87"/>
-      <c r="B214" s="74" t="s">
+      <c r="A214" s="79"/>
+      <c r="B214" s="81" t="s">
         <v>227</v>
       </c>
-      <c r="C214" s="73" t="s">
+      <c r="C214" s="82" t="s">
         <v>228</v>
       </c>
-      <c r="D214" s="74"/>
-      <c r="E214" s="74"/>
+      <c r="D214" s="81"/>
+      <c r="E214" s="81"/>
       <c r="F214" s="28" t="s">
         <v>214</v>
       </c>
@@ -11291,14 +11291,14 @@
         <v>63</v>
       </c>
     </row>
-    <row r="215" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A215" s="98"/>
-      <c r="B215" s="99"/>
-      <c r="C215" s="99" t="s">
+    <row r="215" spans="1:7" ht="15" thickBot="1">
+      <c r="A215" s="80"/>
+      <c r="B215" s="83"/>
+      <c r="C215" s="83" t="s">
         <v>229</v>
       </c>
-      <c r="D215" s="99"/>
-      <c r="E215" s="99"/>
+      <c r="D215" s="83"/>
+      <c r="E215" s="83"/>
       <c r="F215" s="36" t="s">
         <v>215</v>
       </c>
@@ -11325,7 +11325,7 @@
       <c r="D218" s="37"/>
       <c r="E218" s="37"/>
     </row>
-    <row r="219" spans="1:7" ht="15.75" thickBot="1">
+    <row r="219" spans="1:7" ht="15" thickBot="1">
       <c r="A219" s="6" t="s">
         <v>231</v>
       </c>
@@ -11333,16 +11333,16 @@
       <c r="D219" s="37"/>
       <c r="E219" s="37"/>
     </row>
-    <row r="220" spans="1:7" ht="15.75" thickBot="1">
+    <row r="220" spans="1:7" ht="15" thickBot="1">
       <c r="A220" s="45" t="s">
         <v>232</v>
       </c>
-      <c r="B220" s="100" t="s">
+      <c r="B220" s="84" t="s">
         <v>52</v>
       </c>
-      <c r="C220" s="100"/>
-      <c r="D220" s="100"/>
-      <c r="E220" s="100"/>
+      <c r="C220" s="84"/>
+      <c r="D220" s="84"/>
+      <c r="E220" s="84"/>
       <c r="F220" s="46" t="s">
         <v>233</v>
       </c>
@@ -11354,12 +11354,12 @@
       <c r="A221" s="48" t="s">
         <v>235</v>
       </c>
-      <c r="B221" s="101" t="s">
+      <c r="B221" s="85" t="s">
         <v>236</v>
       </c>
-      <c r="C221" s="80"/>
-      <c r="D221" s="80"/>
-      <c r="E221" s="80"/>
+      <c r="C221" s="86"/>
+      <c r="D221" s="86"/>
+      <c r="E221" s="86"/>
       <c r="F221" s="49" t="s">
         <v>111</v>
       </c>
@@ -11371,12 +11371,12 @@
       <c r="A222" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="B222" s="102" t="s">
+      <c r="B222" s="87" t="s">
         <v>238</v>
       </c>
-      <c r="C222" s="103"/>
-      <c r="D222" s="103"/>
-      <c r="E222" s="104"/>
+      <c r="C222" s="88"/>
+      <c r="D222" s="88"/>
+      <c r="E222" s="89"/>
       <c r="F222" s="15" t="s">
         <v>63</v>
       </c>
@@ -11388,12 +11388,12 @@
       <c r="A223" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B223" s="102" t="s">
+      <c r="B223" s="87" t="s">
         <v>239</v>
       </c>
-      <c r="C223" s="103"/>
-      <c r="D223" s="103"/>
-      <c r="E223" s="104"/>
+      <c r="C223" s="88"/>
+      <c r="D223" s="88"/>
+      <c r="E223" s="89"/>
       <c r="F223" s="18" t="s">
         <v>63</v>
       </c>
@@ -11405,12 +11405,12 @@
       <c r="A224" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="B224" s="85" t="s">
+      <c r="B224" s="90" t="s">
         <v>241</v>
       </c>
-      <c r="C224" s="99"/>
-      <c r="D224" s="99"/>
-      <c r="E224" s="99"/>
+      <c r="C224" s="83"/>
+      <c r="D224" s="83"/>
+      <c r="E224" s="83"/>
       <c r="F224" s="21" t="s">
         <v>63</v>
       </c>
@@ -11421,12 +11421,12 @@
     <row r="225" spans="1:7">
       <c r="C225" s="51"/>
     </row>
-    <row r="227" spans="1:7" ht="15.75" thickBot="1">
+    <row r="227" spans="1:7" ht="15" thickBot="1">
       <c r="A227" s="6" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="228" spans="1:7" ht="15.75" thickBot="1">
+    <row r="228" spans="1:7" ht="15" thickBot="1">
       <c r="A228" s="9" t="s">
         <v>243</v>
       </c>
@@ -11455,11 +11455,11 @@
       <c r="C229" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D229" s="97" t="s">
+      <c r="D229" s="78" t="s">
         <v>54</v>
       </c>
-      <c r="E229" s="97"/>
-      <c r="F229" s="97"/>
+      <c r="E229" s="78"/>
+      <c r="F229" s="78"/>
       <c r="G229" s="57"/>
     </row>
     <row r="230" spans="1:7">
@@ -11472,11 +11472,11 @@
       <c r="C230" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D230" s="109" t="s">
+      <c r="D230" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="E230" s="109"/>
-      <c r="F230" s="109"/>
+      <c r="E230" s="77"/>
+      <c r="F230" s="77"/>
       <c r="G230" s="41"/>
     </row>
     <row r="231" spans="1:7">
@@ -11489,11 +11489,11 @@
       <c r="C231" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D231" s="109" t="s">
+      <c r="D231" s="77" t="s">
         <v>245</v>
       </c>
-      <c r="E231" s="109"/>
-      <c r="F231" s="109"/>
+      <c r="E231" s="77"/>
+      <c r="F231" s="77"/>
       <c r="G231" s="41"/>
     </row>
     <row r="232" spans="1:7">
@@ -11506,11 +11506,11 @@
       <c r="C232" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D232" s="109" t="s">
+      <c r="D232" s="77" t="s">
         <v>246</v>
       </c>
-      <c r="E232" s="109"/>
-      <c r="F232" s="109"/>
+      <c r="E232" s="77"/>
+      <c r="F232" s="77"/>
       <c r="G232" s="41"/>
     </row>
     <row r="233" spans="1:7">
@@ -11523,11 +11523,11 @@
       <c r="C233" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D233" s="109" t="s">
+      <c r="D233" s="77" t="s">
         <v>247</v>
       </c>
-      <c r="E233" s="109"/>
-      <c r="F233" s="109"/>
+      <c r="E233" s="77"/>
+      <c r="F233" s="77"/>
       <c r="G233" s="41"/>
     </row>
     <row r="234" spans="1:7">
@@ -11540,11 +11540,11 @@
       <c r="C234" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D234" s="109" t="s">
+      <c r="D234" s="77" t="s">
         <v>248</v>
       </c>
-      <c r="E234" s="109"/>
-      <c r="F234" s="109"/>
+      <c r="E234" s="77"/>
+      <c r="F234" s="77"/>
       <c r="G234" s="41"/>
     </row>
     <row r="235" spans="1:7">
@@ -11557,11 +11557,11 @@
       <c r="C235" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D235" s="105" t="s">
+      <c r="D235" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="E235" s="106"/>
-      <c r="F235" s="107"/>
+      <c r="E235" s="74"/>
+      <c r="F235" s="75"/>
       <c r="G235" s="43"/>
     </row>
     <row r="236" spans="1:7">
@@ -11574,11 +11574,11 @@
       <c r="C236" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D236" s="105" t="s">
+      <c r="D236" s="73" t="s">
         <v>65</v>
       </c>
-      <c r="E236" s="106"/>
-      <c r="F236" s="107"/>
+      <c r="E236" s="74"/>
+      <c r="F236" s="75"/>
       <c r="G236" s="43"/>
     </row>
     <row r="237" spans="1:7">
@@ -11591,11 +11591,11 @@
       <c r="C237" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D237" s="105" t="s">
+      <c r="D237" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="E237" s="106"/>
-      <c r="F237" s="107"/>
+      <c r="E237" s="74"/>
+      <c r="F237" s="75"/>
       <c r="G237" s="43"/>
     </row>
     <row r="238" spans="1:7">
@@ -11683,7 +11683,7 @@
       <c r="F242" s="64"/>
       <c r="G242" s="43"/>
     </row>
-    <row r="243" spans="1:7" ht="15.75" thickBot="1">
+    <row r="243" spans="1:7" ht="15" thickBot="1">
       <c r="A243" s="65">
         <v>44209</v>
       </c>
@@ -11693,56 +11693,33 @@
       <c r="C243" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="D243" s="108" t="s">
+      <c r="D243" s="76" t="s">
         <v>264</v>
       </c>
-      <c r="E243" s="108"/>
-      <c r="F243" s="108"/>
+      <c r="E243" s="76"/>
+      <c r="F243" s="76"/>
       <c r="G243" s="44"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
+    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" scale="115">
       <selection activeCell="C4" sqref="C4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" scale="115">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
       <selection activeCell="C4" sqref="C4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="51">
-    <mergeCell ref="D236:F236"/>
-    <mergeCell ref="D237:F237"/>
-    <mergeCell ref="D243:F243"/>
-    <mergeCell ref="D230:F230"/>
-    <mergeCell ref="D231:F231"/>
-    <mergeCell ref="D232:F232"/>
-    <mergeCell ref="D233:F233"/>
-    <mergeCell ref="D234:F234"/>
-    <mergeCell ref="D235:F235"/>
-    <mergeCell ref="D229:F229"/>
-    <mergeCell ref="A212:A215"/>
-    <mergeCell ref="B212:B213"/>
-    <mergeCell ref="C212:E212"/>
-    <mergeCell ref="C213:E213"/>
-    <mergeCell ref="B214:B215"/>
-    <mergeCell ref="C214:E214"/>
-    <mergeCell ref="C215:E215"/>
-    <mergeCell ref="B220:E220"/>
-    <mergeCell ref="B221:E221"/>
-    <mergeCell ref="B222:E222"/>
-    <mergeCell ref="B223:E223"/>
-    <mergeCell ref="B224:E224"/>
-    <mergeCell ref="A208:A211"/>
-    <mergeCell ref="B208:B209"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C209:E209"/>
-    <mergeCell ref="B210:B211"/>
-    <mergeCell ref="C210:E210"/>
-    <mergeCell ref="C211:E211"/>
+    <mergeCell ref="B174:B176"/>
+    <mergeCell ref="F111:N111"/>
+    <mergeCell ref="B148:B160"/>
+    <mergeCell ref="B161:B162"/>
+    <mergeCell ref="B163:B165"/>
+    <mergeCell ref="B166:B173"/>
     <mergeCell ref="B177:B178"/>
     <mergeCell ref="B179:B185"/>
     <mergeCell ref="C199:E199"/>
@@ -11759,12 +11736,35 @@
     <mergeCell ref="B206:B207"/>
     <mergeCell ref="C206:E206"/>
     <mergeCell ref="C207:E207"/>
-    <mergeCell ref="B174:B176"/>
-    <mergeCell ref="F111:N111"/>
-    <mergeCell ref="B148:B160"/>
-    <mergeCell ref="B161:B162"/>
-    <mergeCell ref="B163:B165"/>
-    <mergeCell ref="B166:B173"/>
+    <mergeCell ref="A208:A211"/>
+    <mergeCell ref="B208:B209"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C209:E209"/>
+    <mergeCell ref="B210:B211"/>
+    <mergeCell ref="C210:E210"/>
+    <mergeCell ref="C211:E211"/>
+    <mergeCell ref="D229:F229"/>
+    <mergeCell ref="A212:A215"/>
+    <mergeCell ref="B212:B213"/>
+    <mergeCell ref="C212:E212"/>
+    <mergeCell ref="C213:E213"/>
+    <mergeCell ref="B214:B215"/>
+    <mergeCell ref="C214:E214"/>
+    <mergeCell ref="C215:E215"/>
+    <mergeCell ref="B220:E220"/>
+    <mergeCell ref="B221:E221"/>
+    <mergeCell ref="B222:E222"/>
+    <mergeCell ref="B223:E223"/>
+    <mergeCell ref="B224:E224"/>
+    <mergeCell ref="D236:F236"/>
+    <mergeCell ref="D237:F237"/>
+    <mergeCell ref="D243:F243"/>
+    <mergeCell ref="D230:F230"/>
+    <mergeCell ref="D231:F231"/>
+    <mergeCell ref="D232:F232"/>
+    <mergeCell ref="D233:F233"/>
+    <mergeCell ref="D234:F234"/>
+    <mergeCell ref="D235:F235"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -11778,7 +11778,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -11787,18 +11787,18 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="E26" sqref="E26"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
i409--internal corescript warning msg added
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/radiant/silicon_07_apollo.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/radiant/silicon_07_apollo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\repository\tmp_client\doc\TMP_EIT_suites\radiant\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="pSvbrBtM5D7J1tTbaFvNMFAx+gsFF1+zjWgivCK1irAkzVtGcdIaviGYDMewqTuAFCctlIpswoSn4Z8ezPPc6w==" workbookSaltValue="fuR2EkRIGc7n0eTkIKsWWA==" workbookSpinCount="100000" lockStructure="1"/>
@@ -1155,9 +1155,6 @@
     <t>52</t>
   </si>
   <si>
-    <t>cmd = --check-conf=sim.conf --synthesis=synplify --sim-rtl --sim-syn-vlg  --sim-par-vlg  --run-ipgen</t>
-  </si>
-  <si>
     <t>22_softIP_Synp</t>
   </si>
   <si>
@@ -1780,6 +1777,9 @@
   </si>
   <si>
     <t xml:space="preserve">cmd = python DEV/bin/run_radiant.py  --run-map-trce --run-par-trce  --set-strategy="{par_disable_timing_driven=True}" </t>
+  </si>
+  <si>
+    <t>cmd = --check-conf=sim.conf --synthesis=synplify --sim-rtl --sim-syn-vlg  --sim-par-vlg  --run-ipgen  --check-smart</t>
   </si>
 </sst>
 </file>
@@ -6071,8 +6071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -6103,7 +6103,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -6111,12 +6111,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="B5" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -6129,7 +6129,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -6248,7 +6248,7 @@
         <v>5</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -6264,7 +6264,7 @@
         <v>114</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -6275,7 +6275,7 @@
         <v>93</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -6286,7 +6286,7 @@
         <v>5</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>362</v>
+        <v>570</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -6505,7 +6505,7 @@
         <v>296</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F3" s="2">
         <v>1</v>
@@ -6534,7 +6534,7 @@
         <v>296</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
@@ -6563,7 +6563,7 @@
         <v>296</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>40</v>
@@ -6592,7 +6592,7 @@
         <v>296</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>40</v>
@@ -6621,7 +6621,7 @@
         <v>296</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>40</v>
@@ -6650,7 +6650,7 @@
         <v>296</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>40</v>
@@ -6679,7 +6679,7 @@
         <v>296</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>40</v>
@@ -6708,7 +6708,7 @@
         <v>296</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>40</v>
@@ -6737,7 +6737,7 @@
         <v>296</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>40</v>
@@ -6766,7 +6766,7 @@
         <v>296</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>40</v>
@@ -6795,7 +6795,7 @@
         <v>296</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>40</v>
@@ -6824,7 +6824,7 @@
         <v>296</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>40</v>
@@ -6853,7 +6853,7 @@
         <v>296</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>40</v>
@@ -6882,7 +6882,7 @@
         <v>296</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>40</v>
@@ -6911,7 +6911,7 @@
         <v>296</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>40</v>
@@ -6940,7 +6940,7 @@
         <v>296</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>40</v>
@@ -6969,7 +6969,7 @@
         <v>296</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>40</v>
@@ -6998,7 +6998,7 @@
         <v>296</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>40</v>
@@ -7027,7 +7027,7 @@
         <v>296</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>40</v>
@@ -7056,7 +7056,7 @@
         <v>296</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>40</v>
@@ -7085,7 +7085,7 @@
         <v>296</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>40</v>
@@ -7114,7 +7114,7 @@
         <v>296</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>40</v>
@@ -7143,7 +7143,7 @@
         <v>327</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>40</v>
@@ -7172,7 +7172,7 @@
         <v>330</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>40</v>
@@ -7198,7 +7198,7 @@
         <v>330</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>40</v>
@@ -7224,7 +7224,7 @@
         <v>330</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>40</v>
@@ -7250,7 +7250,7 @@
         <v>330</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>40</v>
@@ -7276,7 +7276,7 @@
         <v>330</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>40</v>
@@ -7302,7 +7302,7 @@
         <v>330</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>40</v>
@@ -7328,7 +7328,7 @@
         <v>330</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>40</v>
@@ -7354,7 +7354,7 @@
         <v>329</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>40</v>
@@ -7377,7 +7377,7 @@
         <v>329</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>40</v>
@@ -7400,7 +7400,7 @@
         <v>329</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>40</v>
@@ -7423,7 +7423,7 @@
         <v>329</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>40</v>
@@ -7446,7 +7446,7 @@
         <v>343</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>40</v>
@@ -7469,7 +7469,7 @@
         <v>343</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>40</v>
@@ -7492,7 +7492,7 @@
         <v>343</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>40</v>
@@ -7515,7 +7515,7 @@
         <v>343</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>40</v>
@@ -7538,7 +7538,7 @@
         <v>343</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>40</v>
@@ -7561,7 +7561,7 @@
         <v>343</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>40</v>
@@ -7584,7 +7584,7 @@
         <v>343</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>40</v>
@@ -7607,7 +7607,7 @@
         <v>343</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>40</v>
@@ -7630,7 +7630,7 @@
         <v>343</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>40</v>
@@ -7653,7 +7653,7 @@
         <v>343</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>40</v>
@@ -7676,7 +7676,7 @@
         <v>343</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>40</v>
@@ -7699,7 +7699,7 @@
         <v>343</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>40</v>
@@ -7722,7 +7722,7 @@
         <v>343</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>40</v>
@@ -7745,7 +7745,7 @@
         <v>343</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>40</v>
@@ -7768,7 +7768,7 @@
         <v>343</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>40</v>
@@ -7791,7 +7791,7 @@
         <v>343</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>40</v>
@@ -7814,7 +7814,7 @@
         <v>343</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>40</v>
@@ -7837,7 +7837,7 @@
         <v>343</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>40</v>
@@ -7854,19 +7854,19 @@
     </row>
     <row r="55" spans="1:31">
       <c r="A55" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D55" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="G55" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="G55" s="2" t="s">
+      <c r="H55" s="2" t="s">
         <v>431</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>432</v>
       </c>
       <c r="S55" s="2" t="s">
         <v>301</v>
@@ -7880,19 +7880,19 @@
     </row>
     <row r="56" spans="1:31">
       <c r="A56" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E56" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="G56" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="G56" s="2" t="s">
+      <c r="H56" s="2" t="s">
         <v>434</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>435</v>
       </c>
       <c r="S56" s="2" t="s">
         <v>301</v>
@@ -7906,19 +7906,19 @@
     </row>
     <row r="57" spans="1:31">
       <c r="A57" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E57" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="G57" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="G57" s="2" t="s">
+      <c r="H57" s="2" t="s">
         <v>437</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>438</v>
       </c>
       <c r="S57" s="2" t="s">
         <v>301</v>
@@ -7932,19 +7932,19 @@
     </row>
     <row r="58" spans="1:31">
       <c r="A58" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E58" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="G58" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="G58" s="2" t="s">
+      <c r="H58" s="2" t="s">
         <v>440</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>441</v>
       </c>
       <c r="S58" s="2" t="s">
         <v>301</v>
@@ -7958,19 +7958,19 @@
     </row>
     <row r="59" spans="1:31">
       <c r="A59" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E59" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="G59" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="G59" s="2" t="s">
+      <c r="H59" s="2" t="s">
         <v>443</v>
-      </c>
-      <c r="H59" s="2" t="s">
-        <v>444</v>
       </c>
       <c r="S59" s="2" t="s">
         <v>301</v>
@@ -7984,19 +7984,19 @@
     </row>
     <row r="60" spans="1:31">
       <c r="A60" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E60" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="G60" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="G60" s="2" t="s">
+      <c r="H60" s="2" t="s">
         <v>446</v>
-      </c>
-      <c r="H60" s="2" t="s">
-        <v>447</v>
       </c>
       <c r="S60" s="2" t="s">
         <v>301</v>
@@ -8010,19 +8010,19 @@
     </row>
     <row r="61" spans="1:31">
       <c r="A61" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E61" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="G61" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="G61" s="2" t="s">
+      <c r="H61" s="2" t="s">
         <v>449</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>450</v>
       </c>
       <c r="S61" s="2" t="s">
         <v>301</v>
@@ -8036,19 +8036,19 @@
     </row>
     <row r="62" spans="1:31">
       <c r="A62" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E62" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="G62" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="G62" s="2" t="s">
+      <c r="H62" s="2" t="s">
         <v>452</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>453</v>
       </c>
       <c r="S62" s="2" t="s">
         <v>301</v>
@@ -8062,19 +8062,19 @@
     </row>
     <row r="63" spans="1:31">
       <c r="A63" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G63" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="H63" s="2" t="s">
         <v>431</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>432</v>
       </c>
       <c r="S63" s="2" t="s">
         <v>301</v>
@@ -8088,19 +8088,19 @@
     </row>
     <row r="64" spans="1:31">
       <c r="A64" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G64" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H64" s="2" t="s">
         <v>434</v>
-      </c>
-      <c r="H64" s="2" t="s">
-        <v>435</v>
       </c>
       <c r="S64" s="2" t="s">
         <v>301</v>
@@ -8114,19 +8114,19 @@
     </row>
     <row r="65" spans="1:31">
       <c r="A65" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E65" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="H65" s="2" t="s">
         <v>456</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="H65" s="2" t="s">
-        <v>457</v>
       </c>
       <c r="S65" s="2" t="s">
         <v>301</v>
@@ -8140,19 +8140,19 @@
     </row>
     <row r="66" spans="1:31">
       <c r="A66" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="D66" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="D66" s="2" t="s">
-        <v>429</v>
-      </c>
       <c r="E66" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="H66" s="2" t="s">
         <v>458</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="H66" s="2" t="s">
-        <v>459</v>
       </c>
       <c r="S66" s="2" t="s">
         <v>301</v>
@@ -8166,19 +8166,19 @@
     </row>
     <row r="67" spans="1:31">
       <c r="A67" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G67" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="H67" s="2" t="s">
         <v>443</v>
-      </c>
-      <c r="H67" s="2" t="s">
-        <v>444</v>
       </c>
       <c r="S67" s="2" t="s">
         <v>301</v>
@@ -8192,19 +8192,19 @@
     </row>
     <row r="68" spans="1:31">
       <c r="A68" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G68" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="H68" s="2" t="s">
         <v>446</v>
-      </c>
-      <c r="H68" s="2" t="s">
-        <v>447</v>
       </c>
       <c r="S68" s="2" t="s">
         <v>301</v>
@@ -8218,19 +8218,19 @@
     </row>
     <row r="69" spans="1:31">
       <c r="A69" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E69" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="H69" s="2" t="s">
         <v>462</v>
-      </c>
-      <c r="G69" s="2" t="s">
-        <v>449</v>
-      </c>
-      <c r="H69" s="2" t="s">
-        <v>463</v>
       </c>
       <c r="S69" s="2" t="s">
         <v>301</v>
@@ -8244,19 +8244,19 @@
     </row>
     <row r="70" spans="1:31">
       <c r="A70" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E70" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="H70" s="2" t="s">
         <v>464</v>
-      </c>
-      <c r="G70" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="H70" s="2" t="s">
-        <v>465</v>
       </c>
       <c r="S70" s="2" t="s">
         <v>301</v>
@@ -8270,16 +8270,16 @@
     </row>
     <row r="71" spans="1:31">
       <c r="A71" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>117</v>
       </c>
       <c r="E71" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="H71" s="2" t="s">
         <v>466</v>
-      </c>
-      <c r="H71" s="2" t="s">
-        <v>467</v>
       </c>
       <c r="S71" s="2" t="s">
         <v>301</v>
@@ -8293,16 +8293,16 @@
     </row>
     <row r="72" spans="1:31">
       <c r="A72" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>117</v>
       </c>
       <c r="E72" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="H72" s="2" t="s">
         <v>468</v>
-      </c>
-      <c r="H72" s="2" t="s">
-        <v>469</v>
       </c>
       <c r="S72" s="2" t="s">
         <v>301</v>
@@ -8316,19 +8316,19 @@
     </row>
     <row r="73" spans="1:31">
       <c r="A73" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>117</v>
       </c>
       <c r="E73" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="G73" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="G73" s="2" t="s">
+      <c r="H73" s="2" t="s">
         <v>471</v>
-      </c>
-      <c r="H73" s="2" t="s">
-        <v>472</v>
       </c>
       <c r="S73" s="2" t="s">
         <v>301</v>
@@ -8342,19 +8342,19 @@
     </row>
     <row r="74" spans="1:31">
       <c r="A74" s="2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>117</v>
       </c>
       <c r="E74" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="G74" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="G74" s="2" t="s">
+      <c r="H74" s="2" t="s">
         <v>475</v>
-      </c>
-      <c r="H74" s="2" t="s">
-        <v>476</v>
       </c>
       <c r="S74" s="2" t="s">
         <v>301</v>
@@ -8368,16 +8368,16 @@
     </row>
     <row r="75" spans="1:31">
       <c r="A75" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>117</v>
       </c>
       <c r="E75" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="H75" s="2" t="s">
         <v>477</v>
-      </c>
-      <c r="H75" s="2" t="s">
-        <v>478</v>
       </c>
       <c r="S75" s="2" t="s">
         <v>301</v>
@@ -8391,16 +8391,16 @@
     </row>
     <row r="76" spans="1:31">
       <c r="A76" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>117</v>
       </c>
       <c r="E76" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="H76" s="2" t="s">
         <v>480</v>
-      </c>
-      <c r="H76" s="2" t="s">
-        <v>481</v>
       </c>
       <c r="S76" s="2" t="s">
         <v>301</v>
@@ -8414,16 +8414,16 @@
     </row>
     <row r="77" spans="1:31">
       <c r="A77" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>117</v>
       </c>
       <c r="E77" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="H77" s="2" t="s">
         <v>482</v>
-      </c>
-      <c r="H77" s="2" t="s">
-        <v>483</v>
       </c>
       <c r="S77" s="2" t="s">
         <v>301</v>
@@ -8437,16 +8437,16 @@
     </row>
     <row r="78" spans="1:31">
       <c r="A78" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>117</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="S78" s="2" t="s">
         <v>301</v>
@@ -8460,19 +8460,19 @@
     </row>
     <row r="79" spans="1:31">
       <c r="A79" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>117</v>
       </c>
       <c r="E79" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="H79" s="2" t="s">
         <v>561</v>
-      </c>
-      <c r="G79" s="2" t="s">
-        <v>471</v>
-      </c>
-      <c r="H79" s="2" t="s">
-        <v>562</v>
       </c>
       <c r="S79" s="2" t="s">
         <v>301</v>
@@ -8486,19 +8486,19 @@
     </row>
     <row r="80" spans="1:31">
       <c r="A80" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>117</v>
       </c>
       <c r="E80" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="H80" s="2" t="s">
         <v>563</v>
-      </c>
-      <c r="G80" s="2" t="s">
-        <v>475</v>
-      </c>
-      <c r="H80" s="2" t="s">
-        <v>564</v>
       </c>
       <c r="S80" s="2" t="s">
         <v>301</v>
@@ -8512,16 +8512,16 @@
     </row>
     <row r="81" spans="1:31">
       <c r="A81" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>117</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="S81" s="2" t="s">
         <v>301</v>
@@ -8535,16 +8535,16 @@
     </row>
     <row r="82" spans="1:31">
       <c r="A82" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>117</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="S82" s="2" t="s">
         <v>301</v>
@@ -8558,13 +8558,13 @@
     </row>
     <row r="83" spans="1:31">
       <c r="A83" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="S83" s="2" t="s">
         <v>301</v>
@@ -8578,13 +8578,13 @@
     </row>
     <row r="84" spans="1:31">
       <c r="A84" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="S84" s="2" t="s">
         <v>301</v>
@@ -8598,13 +8598,13 @@
     </row>
     <row r="85" spans="1:31">
       <c r="A85" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="S85" s="2" t="s">
         <v>301</v>
@@ -8618,16 +8618,16 @@
     </row>
     <row r="86" spans="1:31">
       <c r="A86" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E86" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="H86" s="2" t="s">
         <v>487</v>
-      </c>
-      <c r="H86" s="2" t="s">
-        <v>488</v>
       </c>
       <c r="S86" s="2" t="s">
         <v>301</v>
@@ -8641,16 +8641,16 @@
     </row>
     <row r="87" spans="1:31">
       <c r="A87" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="S87" s="2" t="s">
         <v>301</v>
@@ -8664,13 +8664,13 @@
     </row>
     <row r="88" spans="1:31">
       <c r="A88" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="S88" s="2" t="s">
         <v>301</v>
@@ -8684,13 +8684,13 @@
     </row>
     <row r="89" spans="1:31">
       <c r="A89" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="S89" s="2" t="s">
         <v>301</v>
@@ -8704,13 +8704,13 @@
     </row>
     <row r="90" spans="1:31">
       <c r="A90" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="S90" s="2" t="s">
         <v>301</v>
@@ -8724,13 +8724,13 @@
     </row>
     <row r="91" spans="1:31">
       <c r="A91" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="S91" s="2" t="s">
         <v>301</v>
@@ -8744,16 +8744,16 @@
     </row>
     <row r="92" spans="1:31">
       <c r="A92" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E92" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="H92" s="2" t="s">
         <v>490</v>
-      </c>
-      <c r="H92" s="2" t="s">
-        <v>491</v>
       </c>
       <c r="S92" s="2" t="s">
         <v>301</v>
@@ -8767,16 +8767,16 @@
     </row>
     <row r="93" spans="1:31">
       <c r="A93" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="S93" s="2" t="s">
         <v>301</v>
@@ -8790,13 +8790,13 @@
     </row>
     <row r="94" spans="1:31">
       <c r="A94" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="S94" s="2" t="s">
         <v>301</v>
@@ -8810,16 +8810,16 @@
     </row>
     <row r="95" spans="1:31">
       <c r="A95" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>343</v>
       </c>
       <c r="E95" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="H95" s="2" t="s">
         <v>497</v>
-      </c>
-      <c r="H95" s="2" t="s">
-        <v>498</v>
       </c>
       <c r="S95" s="2" t="s">
         <v>343</v>
@@ -8833,16 +8833,16 @@
     </row>
     <row r="96" spans="1:31">
       <c r="A96" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>343</v>
       </c>
       <c r="E96" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="H96" s="2" t="s">
         <v>499</v>
-      </c>
-      <c r="H96" s="2" t="s">
-        <v>500</v>
       </c>
       <c r="S96" s="2" t="s">
         <v>343</v>
@@ -8856,16 +8856,16 @@
     </row>
     <row r="97" spans="1:31">
       <c r="A97" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>343</v>
       </c>
       <c r="E97" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="H97" s="2" t="s">
         <v>501</v>
-      </c>
-      <c r="H97" s="2" t="s">
-        <v>502</v>
       </c>
       <c r="S97" s="2" t="s">
         <v>343</v>
@@ -8879,16 +8879,16 @@
     </row>
     <row r="98" spans="1:31">
       <c r="A98" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>343</v>
       </c>
       <c r="E98" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="H98" s="2" t="s">
         <v>503</v>
-      </c>
-      <c r="H98" s="2" t="s">
-        <v>504</v>
       </c>
       <c r="S98" s="2" t="s">
         <v>343</v>
@@ -8902,16 +8902,16 @@
     </row>
     <row r="99" spans="1:31">
       <c r="A99" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>343</v>
       </c>
       <c r="E99" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="H99" s="2" t="s">
         <v>505</v>
-      </c>
-      <c r="H99" s="2" t="s">
-        <v>506</v>
       </c>
       <c r="S99" s="2" t="s">
         <v>343</v>
@@ -8925,16 +8925,16 @@
     </row>
     <row r="100" spans="1:31">
       <c r="A100" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>343</v>
       </c>
       <c r="E100" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="H100" s="2" t="s">
         <v>507</v>
-      </c>
-      <c r="H100" s="2" t="s">
-        <v>508</v>
       </c>
       <c r="S100" s="2" t="s">
         <v>343</v>
@@ -8948,16 +8948,16 @@
     </row>
     <row r="101" spans="1:31">
       <c r="A101" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>343</v>
       </c>
       <c r="E101" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="H101" s="2" t="s">
         <v>509</v>
-      </c>
-      <c r="H101" s="2" t="s">
-        <v>510</v>
       </c>
       <c r="S101" s="2" t="s">
         <v>343</v>
@@ -8971,13 +8971,13 @@
     </row>
     <row r="102" spans="1:31">
       <c r="A102" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>343</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="S102" s="2" t="s">
         <v>343</v>
@@ -8991,13 +8991,13 @@
     </row>
     <row r="103" spans="1:31">
       <c r="A103" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>343</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="S103" s="2" t="s">
         <v>343</v>
@@ -9011,13 +9011,13 @@
     </row>
     <row r="104" spans="1:31">
       <c r="A104" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>343</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="S104" s="2" t="s">
         <v>343</v>
@@ -9031,13 +9031,13 @@
     </row>
     <row r="105" spans="1:31">
       <c r="A105" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>343</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="S105" s="2" t="s">
         <v>343</v>
@@ -9051,13 +9051,13 @@
     </row>
     <row r="106" spans="1:31">
       <c r="A106" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>343</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="S106" s="2" t="s">
         <v>343</v>
@@ -9071,13 +9071,13 @@
     </row>
     <row r="107" spans="1:31">
       <c r="A107" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>343</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="S107" s="2" t="s">
         <v>343</v>
@@ -9091,13 +9091,13 @@
     </row>
     <row r="108" spans="1:31">
       <c r="A108" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>343</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="S108" s="2" t="s">
         <v>343</v>

</xml_diff>

<commit_message>
i431--Jedi-d6-100k suite file integrated
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/radiant/silicon_07_apollo.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/radiant/silicon_07_apollo.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\repository\tmp_client\doc\TMP_EIT_suites\radiant\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FE8270-508D-4937-AA01-85D61EE6AA86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6BDA2DD-74AD-4DE0-AE8B-2E5BE73A2394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="pSvbrBtM5D7J1tTbaFvNMFAx+gsFF1+zjWgivCK1irAkzVtGcdIaviGYDMewqTuAFCctlIpswoSn4Z8ezPPc6w==" workbookSaltValue="fuR2EkRIGc7n0eTkIKsWWA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="suite" sheetId="1" r:id="rId1"/>
@@ -1762,66 +1762,36 @@
     <t>primitive:IMONDELAY</t>
   </si>
   <si>
-    <t>ITR3/21_DDR/01_impl/10_DDRDPHY/101_DDRPHY16_impl</t>
-  </si>
-  <si>
     <t>primitive:DDRPHY16 implementation</t>
   </si>
   <si>
     <t>timeout=36000</t>
   </si>
   <si>
-    <t>ITR3/21_DDR/01_impl/10_DDRDPHY/102_DDRPHY32_impl</t>
-  </si>
-  <si>
     <t>primitive:DDRPHY32 implementation</t>
   </si>
   <si>
-    <t>ITR3/21_DDR/01_impl/10_DDRDPHY/103_DDRPHY40_impl</t>
-  </si>
-  <si>
     <t>primitive:DDRPHY40 implementation</t>
   </si>
   <si>
-    <t>ITR3/21_DDR/01_impl/10_DDRDPHY/104_DDRPHY64_impl</t>
-  </si>
-  <si>
     <t>primitive:DDRPHY64 implementation</t>
   </si>
   <si>
-    <t>ITR3/21_DDR/01_impl/10_DDRDPHY/105_DDRPHY72_impl</t>
-  </si>
-  <si>
     <t>primitive:DDRPHY72 implementation</t>
   </si>
   <si>
-    <t>ITR3/21_DDR/03_sim/10_DDRDPHY/101_DDRPHY16_sim</t>
-  </si>
-  <si>
     <t>primitive:DDRPHY16 sim flow</t>
   </si>
   <si>
-    <t>ITR3/21_DDR/03_sim/10_DDRDPHY/102_DDRPHY32_sim</t>
-  </si>
-  <si>
     <t>primitive:DDRPHY32sim flow</t>
   </si>
   <si>
-    <t>ITR3/21_DDR/03_sim/10_DDRDPHY/103_DDRPHY40_sim</t>
-  </si>
-  <si>
     <t>primitive:DDRPHY40 sim flow</t>
   </si>
   <si>
-    <t>ITR3/21_DDR/03_sim/10_DDRDPHY/104_DDRPHY64_sim</t>
-  </si>
-  <si>
     <t>primitive:DDRPHY64 sim flow</t>
   </si>
   <si>
-    <t>ITR3/21_DDR/03_sim/10_DDRDPHY/105_DDRPHY72_sim</t>
-  </si>
-  <si>
     <t>primitive:DDRPHY72 sim flow</t>
   </si>
   <si>
@@ -2101,27 +2071,18 @@
     <t>130</t>
   </si>
   <si>
-    <t>ITR3/21_DDR/01_impl/10_DDRDPHY/301_DDRPHY16B_impl</t>
-  </si>
-  <si>
     <t>primitive:DDRPHY16B implementation</t>
   </si>
   <si>
     <t>131</t>
   </si>
   <si>
-    <t>ITR3/21_DDR/01_impl/10_DDRDPHY/302_DDRPHY32B_impl</t>
-  </si>
-  <si>
     <t>primitive:DDRPHY32B implementation</t>
   </si>
   <si>
     <t>132</t>
   </si>
   <si>
-    <t>ITR3/21_DDR/01_impl/10_DDRDPHY/303_DDRPHY64B_impl</t>
-  </si>
-  <si>
     <t>primitive:DDRPHY64B implementation</t>
   </si>
   <si>
@@ -2161,21 +2122,12 @@
     <t>137</t>
   </si>
   <si>
-    <t>ITR3/21_DDR/03_sim/10_DDRDPHY/301_DDRPHY16B_sim</t>
-  </si>
-  <si>
     <t>138</t>
   </si>
   <si>
-    <t>ITR3/21_DDR/03_sim/10_DDRDPHY/302_DDRPHY32B_sim</t>
-  </si>
-  <si>
     <t>139</t>
   </si>
   <si>
-    <t>ITR3/21_DDR/03_sim/10_DDRDPHY/303_DDRPHY64B_sim</t>
-  </si>
-  <si>
     <t>140</t>
   </si>
   <si>
@@ -2414,6 +2366,54 @@
   </si>
   <si>
     <t>178</t>
+  </si>
+  <si>
+    <t>ITR3/21_DDR/03_sim/10_DDRPHY/301_DDRPHY16B_sim</t>
+  </si>
+  <si>
+    <t>ITR3/21_DDR/03_sim/10_DDRPHY/302_DDRPHY32B_sim</t>
+  </si>
+  <si>
+    <t>ITR3/21_DDR/03_sim/10_DDRPHY/303_DDRPHY64B_sim</t>
+  </si>
+  <si>
+    <t>ITR3/21_DDR/01_impl/10_DDRPHY/301_DDRPHY16B_impl</t>
+  </si>
+  <si>
+    <t>ITR3/21_DDR/01_impl/10_DDRPHY/302_DDRPHY32B_impl</t>
+  </si>
+  <si>
+    <t>ITR3/21_DDR/01_impl/10_DDRPHY/303_DDRPHY64B_impl</t>
+  </si>
+  <si>
+    <t>ITR3/21_DDR/03_sim/10_DDRPHY/105_DDRPHY72_sim</t>
+  </si>
+  <si>
+    <t>ITR3/21_DDR/03_sim/10_DDRPHY/104_DDRPHY64_sim</t>
+  </si>
+  <si>
+    <t>ITR3/21_DDR/03_sim/10_DDRPHY/103_DDRPHY40_sim</t>
+  </si>
+  <si>
+    <t>ITR3/21_DDR/03_sim/10_DDRPHY/102_DDRPHY32_sim</t>
+  </si>
+  <si>
+    <t>ITR3/21_DDR/03_sim/10_DDRPHY/101_DDRPHY16_sim</t>
+  </si>
+  <si>
+    <t>ITR3/21_DDR/01_impl/10_DDRPHY/105_DDRPHY72_impl</t>
+  </si>
+  <si>
+    <t>ITR3/21_DDR/01_impl/10_DDRPHY/104_DDRPHY64_impl</t>
+  </si>
+  <si>
+    <t>ITR3/21_DDR/01_impl/10_DDRPHY/103_DDRPHY40_impl</t>
+  </si>
+  <si>
+    <t>ITR3/21_DDR/01_impl/10_DDRPHY/102_DDRPHY32_impl</t>
+  </si>
+  <si>
+    <t>ITR3/21_DDR/01_impl/10_DDRPHY/101_DDRPHY16_impl</t>
   </si>
 </sst>
 </file>
@@ -6739,7 +6739,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -6803,7 +6803,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>739</v>
+        <v>723</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -6994,12 +6994,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AE180"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B150" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B96" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B181" sqref="B181"/>
+      <selection pane="bottomRight" activeCell="E135" sqref="E135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -9559,19 +9559,19 @@
         <v>531</v>
       </c>
       <c r="E90" s="2" t="s">
+        <v>781</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H90" s="2" t="s">
         <v>564</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H90" s="2" t="s">
-        <v>565</v>
       </c>
       <c r="L90" s="5" t="s">
         <v>35</v>
       </c>
       <c r="M90" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="S90" s="2" t="s">
         <v>301</v>
@@ -9591,19 +9591,19 @@
         <v>531</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>567</v>
+        <v>780</v>
       </c>
       <c r="F91" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="L91" s="5" t="s">
         <v>35</v>
       </c>
       <c r="M91" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="S91" s="2" t="s">
         <v>301</v>
@@ -9623,19 +9623,19 @@
         <v>531</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>569</v>
+        <v>779</v>
       </c>
       <c r="F92" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="L92" s="5" t="s">
         <v>35</v>
       </c>
       <c r="M92" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="S92" s="2" t="s">
         <v>301</v>
@@ -9655,19 +9655,19 @@
         <v>531</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>571</v>
+        <v>778</v>
       </c>
       <c r="F93" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="L93" s="5" t="s">
         <v>35</v>
       </c>
       <c r="M93" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="S93" s="2" t="s">
         <v>301</v>
@@ -9687,19 +9687,19 @@
         <v>531</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>573</v>
+        <v>777</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="L94" s="5" t="s">
         <v>35</v>
       </c>
       <c r="M94" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="S94" s="2" t="s">
         <v>301</v>
@@ -9719,19 +9719,19 @@
         <v>531</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>575</v>
+        <v>776</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="L95" s="5" t="s">
         <v>35</v>
       </c>
       <c r="M95" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="S95" s="2" t="s">
         <v>301</v>
@@ -9751,19 +9751,19 @@
         <v>531</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>577</v>
+        <v>775</v>
       </c>
       <c r="F96" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>578</v>
+        <v>571</v>
       </c>
       <c r="L96" s="5" t="s">
         <v>35</v>
       </c>
       <c r="M96" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="S96" s="2" t="s">
         <v>301</v>
@@ -9783,19 +9783,19 @@
         <v>531</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>579</v>
+        <v>774</v>
       </c>
       <c r="F97" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>580</v>
+        <v>572</v>
       </c>
       <c r="L97" s="5" t="s">
         <v>35</v>
       </c>
       <c r="M97" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="S97" s="2" t="s">
         <v>301</v>
@@ -9815,19 +9815,19 @@
         <v>531</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>581</v>
+        <v>773</v>
       </c>
       <c r="F98" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>582</v>
+        <v>573</v>
       </c>
       <c r="L98" s="5" t="s">
         <v>35</v>
       </c>
       <c r="M98" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="S98" s="2" t="s">
         <v>301</v>
@@ -9847,19 +9847,19 @@
         <v>531</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>583</v>
+        <v>772</v>
       </c>
       <c r="F99" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>584</v>
+        <v>574</v>
       </c>
       <c r="L99" s="5" t="s">
         <v>35</v>
       </c>
       <c r="M99" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="S99" s="2" t="s">
         <v>301</v>
@@ -9876,16 +9876,16 @@
         <v>509</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>740</v>
+        <v>724</v>
       </c>
       <c r="F100" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H100" s="2" t="s">
-        <v>586</v>
+        <v>576</v>
       </c>
       <c r="S100" s="2" t="s">
         <v>301</v>
@@ -9902,16 +9902,16 @@
         <v>510</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>587</v>
+        <v>577</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>588</v>
+        <v>578</v>
       </c>
       <c r="F101" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H101" s="2" t="s">
-        <v>589</v>
+        <v>579</v>
       </c>
       <c r="L101" s="5" t="s">
         <v>35</v>
@@ -9931,16 +9931,16 @@
         <v>511</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>587</v>
+        <v>577</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>590</v>
+        <v>580</v>
       </c>
       <c r="F102" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>591</v>
+        <v>581</v>
       </c>
       <c r="S102" s="2" t="s">
         <v>301</v>
@@ -9960,13 +9960,13 @@
         <v>531</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>592</v>
+        <v>582</v>
       </c>
       <c r="F103" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>593</v>
+        <v>583</v>
       </c>
       <c r="S103" s="2" t="s">
         <v>301</v>
@@ -9986,13 +9986,13 @@
         <v>531</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>594</v>
+        <v>584</v>
       </c>
       <c r="F104" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H104" s="2" t="s">
-        <v>595</v>
+        <v>585</v>
       </c>
       <c r="S104" s="2" t="s">
         <v>301</v>
@@ -10012,13 +10012,13 @@
         <v>531</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>596</v>
+        <v>586</v>
       </c>
       <c r="F105" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>597</v>
+        <v>587</v>
       </c>
       <c r="S105" s="2" t="s">
         <v>301</v>
@@ -10038,13 +10038,13 @@
         <v>531</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>598</v>
+        <v>588</v>
       </c>
       <c r="F106" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>599</v>
+        <v>589</v>
       </c>
       <c r="S106" s="2" t="s">
         <v>301</v>
@@ -10064,13 +10064,13 @@
         <v>531</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>600</v>
+        <v>590</v>
       </c>
       <c r="F107" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>601</v>
+        <v>591</v>
       </c>
       <c r="S107" s="2" t="s">
         <v>301</v>
@@ -10090,13 +10090,13 @@
         <v>531</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>602</v>
+        <v>592</v>
       </c>
       <c r="F108" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>603</v>
+        <v>593</v>
       </c>
       <c r="S108" s="2" t="s">
         <v>301</v>
@@ -10110,19 +10110,19 @@
     </row>
     <row r="109" spans="1:31">
       <c r="A109" s="2" t="s">
-        <v>604</v>
+        <v>594</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>531</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>605</v>
+        <v>595</v>
       </c>
       <c r="F109" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H109" s="2" t="s">
-        <v>606</v>
+        <v>596</v>
       </c>
       <c r="S109" s="2" t="s">
         <v>301</v>
@@ -10136,19 +10136,19 @@
     </row>
     <row r="110" spans="1:31">
       <c r="A110" s="2" t="s">
-        <v>607</v>
+        <v>597</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>531</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>608</v>
+        <v>598</v>
       </c>
       <c r="F110" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H110" s="2" t="s">
-        <v>609</v>
+        <v>599</v>
       </c>
       <c r="S110" s="2" t="s">
         <v>301</v>
@@ -10162,19 +10162,19 @@
     </row>
     <row r="111" spans="1:31">
       <c r="A111" s="2" t="s">
-        <v>610</v>
+        <v>600</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>116</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>611</v>
+        <v>601</v>
       </c>
       <c r="F111" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H111" s="2" t="s">
-        <v>612</v>
+        <v>602</v>
       </c>
       <c r="S111" s="2" t="s">
         <v>301</v>
@@ -10188,19 +10188,19 @@
     </row>
     <row r="112" spans="1:31">
       <c r="A112" s="2" t="s">
-        <v>613</v>
+        <v>603</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>614</v>
+        <v>604</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>615</v>
+        <v>605</v>
       </c>
       <c r="F112" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H112" s="2" t="s">
-        <v>616</v>
+        <v>606</v>
       </c>
       <c r="S112" s="2" t="s">
         <v>301</v>
@@ -10214,19 +10214,19 @@
     </row>
     <row r="113" spans="1:31">
       <c r="A113" s="2" t="s">
-        <v>617</v>
+        <v>607</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>614</v>
+        <v>604</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>618</v>
+        <v>608</v>
       </c>
       <c r="F113" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H113" s="2" t="s">
-        <v>619</v>
+        <v>609</v>
       </c>
       <c r="S113" s="2" t="s">
         <v>301</v>
@@ -10240,19 +10240,19 @@
     </row>
     <row r="114" spans="1:31">
       <c r="A114" s="2" t="s">
-        <v>620</v>
+        <v>610</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>614</v>
+        <v>604</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>621</v>
+        <v>611</v>
       </c>
       <c r="F114" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H114" s="2" t="s">
-        <v>622</v>
+        <v>612</v>
       </c>
       <c r="S114" s="2" t="s">
         <v>301</v>
@@ -10266,19 +10266,19 @@
     </row>
     <row r="115" spans="1:31">
       <c r="A115" s="2" t="s">
-        <v>623</v>
+        <v>613</v>
       </c>
       <c r="D115" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="E115" s="2" t="s">
         <v>614</v>
       </c>
-      <c r="E115" s="2" t="s">
-        <v>624</v>
-      </c>
       <c r="F115" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H115" s="2" t="s">
-        <v>625</v>
+        <v>615</v>
       </c>
       <c r="S115" s="2" t="s">
         <v>301</v>
@@ -10292,19 +10292,19 @@
     </row>
     <row r="116" spans="1:31">
       <c r="A116" s="2" t="s">
-        <v>626</v>
+        <v>616</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>614</v>
+        <v>604</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>627</v>
+        <v>617</v>
       </c>
       <c r="F116" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H116" s="2" t="s">
-        <v>628</v>
+        <v>618</v>
       </c>
       <c r="S116" s="2" t="s">
         <v>301</v>
@@ -10318,19 +10318,19 @@
     </row>
     <row r="117" spans="1:31">
       <c r="A117" s="2" t="s">
-        <v>629</v>
+        <v>619</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>614</v>
+        <v>604</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>630</v>
+        <v>620</v>
       </c>
       <c r="F117" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H117" s="2" t="s">
-        <v>631</v>
+        <v>621</v>
       </c>
       <c r="S117" s="2" t="s">
         <v>301</v>
@@ -10344,19 +10344,19 @@
     </row>
     <row r="118" spans="1:31">
       <c r="A118" s="2" t="s">
-        <v>632</v>
+        <v>622</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>614</v>
+        <v>604</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>633</v>
+        <v>623</v>
       </c>
       <c r="F118" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H118" s="2" t="s">
-        <v>634</v>
+        <v>624</v>
       </c>
       <c r="S118" s="2" t="s">
         <v>301</v>
@@ -10370,19 +10370,19 @@
     </row>
     <row r="119" spans="1:31">
       <c r="A119" s="2" t="s">
-        <v>635</v>
+        <v>625</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>614</v>
+        <v>604</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>636</v>
+        <v>626</v>
       </c>
       <c r="F119" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H119" s="2" t="s">
-        <v>637</v>
+        <v>627</v>
       </c>
       <c r="S119" s="2" t="s">
         <v>301</v>
@@ -10396,19 +10396,19 @@
     </row>
     <row r="120" spans="1:31">
       <c r="A120" s="2" t="s">
-        <v>638</v>
+        <v>628</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>531</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>639</v>
+        <v>629</v>
       </c>
       <c r="F120" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H120" s="2" t="s">
-        <v>640</v>
+        <v>630</v>
       </c>
       <c r="L120" s="5" t="s">
         <v>35</v>
@@ -10425,19 +10425,19 @@
     </row>
     <row r="121" spans="1:31">
       <c r="A121" s="2" t="s">
-        <v>641</v>
+        <v>631</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>531</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>642</v>
+        <v>632</v>
       </c>
       <c r="F121" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H121" s="2" t="s">
-        <v>643</v>
+        <v>633</v>
       </c>
       <c r="L121" s="5" t="s">
         <v>35</v>
@@ -10454,19 +10454,19 @@
     </row>
     <row r="122" spans="1:31">
       <c r="A122" s="2" t="s">
-        <v>644</v>
+        <v>634</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>531</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>645</v>
+        <v>635</v>
       </c>
       <c r="F122" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H122" s="2" t="s">
-        <v>646</v>
+        <v>636</v>
       </c>
       <c r="S122" s="2" t="s">
         <v>301</v>
@@ -10480,19 +10480,19 @@
     </row>
     <row r="123" spans="1:31">
       <c r="A123" s="2" t="s">
-        <v>647</v>
+        <v>637</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>531</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>648</v>
+        <v>638</v>
       </c>
       <c r="F123" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H123" s="2" t="s">
-        <v>649</v>
+        <v>639</v>
       </c>
       <c r="L123" s="5" t="s">
         <v>35</v>
@@ -10509,22 +10509,22 @@
     </row>
     <row r="124" spans="1:31">
       <c r="A124" s="2" t="s">
-        <v>650</v>
+        <v>640</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>531</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>651</v>
+        <v>641</v>
       </c>
       <c r="F124" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H124" s="2" t="s">
-        <v>652</v>
+        <v>642</v>
       </c>
       <c r="M124" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="S124" s="2" t="s">
         <v>301</v>
@@ -10538,22 +10538,22 @@
     </row>
     <row r="125" spans="1:31">
       <c r="A125" s="2" t="s">
-        <v>653</v>
+        <v>643</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>531</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>654</v>
+        <v>644</v>
       </c>
       <c r="F125" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>655</v>
+        <v>645</v>
       </c>
       <c r="M125" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="S125" s="2" t="s">
         <v>301</v>
@@ -10567,25 +10567,25 @@
     </row>
     <row r="126" spans="1:31">
       <c r="A126" s="2" t="s">
-        <v>656</v>
+        <v>646</v>
       </c>
       <c r="D126" s="2" t="s">
         <v>531</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>657</v>
+        <v>647</v>
       </c>
       <c r="F126" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H126" s="2" t="s">
-        <v>658</v>
+        <v>648</v>
       </c>
       <c r="L126" s="5" t="s">
         <v>35</v>
       </c>
       <c r="M126" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="S126" s="2" t="s">
         <v>301</v>
@@ -10599,25 +10599,25 @@
     </row>
     <row r="127" spans="1:31">
       <c r="A127" s="2" t="s">
-        <v>659</v>
+        <v>649</v>
       </c>
       <c r="D127" s="2" t="s">
         <v>531</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>660</v>
+        <v>650</v>
       </c>
       <c r="F127" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H127" s="2" t="s">
-        <v>661</v>
+        <v>651</v>
       </c>
       <c r="L127" s="5" t="s">
         <v>35</v>
       </c>
       <c r="M127" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="S127" s="2" t="s">
         <v>301</v>
@@ -10631,25 +10631,25 @@
     </row>
     <row r="128" spans="1:31">
       <c r="A128" s="2" t="s">
-        <v>662</v>
+        <v>652</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>663</v>
+        <v>653</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>664</v>
+        <v>654</v>
       </c>
       <c r="F128" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H128" s="2" t="s">
-        <v>665</v>
+        <v>655</v>
       </c>
       <c r="L128" s="5" t="s">
         <v>35</v>
       </c>
       <c r="O128" s="2" t="s">
-        <v>666</v>
+        <v>656</v>
       </c>
       <c r="S128" s="2" t="s">
         <v>301</v>
@@ -10663,22 +10663,22 @@
     </row>
     <row r="129" spans="1:31">
       <c r="A129" s="2" t="s">
-        <v>667</v>
+        <v>657</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>663</v>
+        <v>653</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>668</v>
+        <v>658</v>
       </c>
       <c r="F129" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H129" s="2" t="s">
-        <v>669</v>
+        <v>659</v>
       </c>
       <c r="O129" s="2" t="s">
-        <v>666</v>
+        <v>656</v>
       </c>
       <c r="S129" s="2" t="s">
         <v>301</v>
@@ -10692,19 +10692,19 @@
     </row>
     <row r="130" spans="1:31">
       <c r="A130" s="2" t="s">
-        <v>670</v>
+        <v>660</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>531</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>671</v>
+        <v>661</v>
       </c>
       <c r="F130" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H130" s="2" t="s">
-        <v>672</v>
+        <v>662</v>
       </c>
       <c r="S130" s="2" t="s">
         <v>301</v>
@@ -10718,19 +10718,19 @@
     </row>
     <row r="131" spans="1:31">
       <c r="A131" s="2" t="s">
-        <v>673</v>
+        <v>663</v>
       </c>
       <c r="D131" s="2" t="s">
         <v>531</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>674</v>
+        <v>664</v>
       </c>
       <c r="F131" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H131" s="2" t="s">
-        <v>675</v>
+        <v>665</v>
       </c>
       <c r="S131" s="2" t="s">
         <v>301</v>
@@ -10744,22 +10744,22 @@
     </row>
     <row r="132" spans="1:31">
       <c r="A132" s="2" t="s">
-        <v>676</v>
+        <v>666</v>
       </c>
       <c r="D132" s="2" t="s">
         <v>531</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>677</v>
+        <v>769</v>
       </c>
       <c r="F132" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H132" s="2" t="s">
-        <v>678</v>
+        <v>667</v>
       </c>
       <c r="M132" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="S132" s="2" t="s">
         <v>301</v>
@@ -10773,22 +10773,22 @@
     </row>
     <row r="133" spans="1:31">
       <c r="A133" s="2" t="s">
-        <v>679</v>
+        <v>668</v>
       </c>
       <c r="D133" s="2" t="s">
         <v>531</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>680</v>
+        <v>770</v>
       </c>
       <c r="F133" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H133" s="2" t="s">
-        <v>681</v>
+        <v>669</v>
       </c>
       <c r="M133" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="S133" s="2" t="s">
         <v>301</v>
@@ -10802,25 +10802,25 @@
     </row>
     <row r="134" spans="1:31">
       <c r="A134" s="2" t="s">
-        <v>682</v>
+        <v>670</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>531</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>683</v>
+        <v>771</v>
       </c>
       <c r="F134" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H134" s="2" t="s">
-        <v>684</v>
+        <v>671</v>
       </c>
       <c r="L134" s="5" t="s">
         <v>35</v>
       </c>
       <c r="M134" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="S134" s="2" t="s">
         <v>301</v>
@@ -10834,19 +10834,19 @@
     </row>
     <row r="135" spans="1:31">
       <c r="A135" s="2" t="s">
-        <v>685</v>
+        <v>672</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>531</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>686</v>
+        <v>673</v>
       </c>
       <c r="F135" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H135" s="2" t="s">
-        <v>687</v>
+        <v>674</v>
       </c>
       <c r="L135" s="5" t="s">
         <v>35</v>
@@ -10863,19 +10863,19 @@
     </row>
     <row r="136" spans="1:31">
       <c r="A136" s="2" t="s">
-        <v>688</v>
+        <v>675</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>531</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>689</v>
+        <v>676</v>
       </c>
       <c r="F136" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H136" s="2" t="s">
-        <v>690</v>
+        <v>677</v>
       </c>
       <c r="S136" s="2" t="s">
         <v>301</v>
@@ -10889,19 +10889,19 @@
     </row>
     <row r="137" spans="1:31">
       <c r="A137" s="2" t="s">
-        <v>691</v>
+        <v>678</v>
       </c>
       <c r="D137" s="2" t="s">
         <v>531</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>692</v>
+        <v>679</v>
       </c>
       <c r="F137" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H137" s="2" t="s">
-        <v>672</v>
+        <v>662</v>
       </c>
       <c r="S137" s="2" t="s">
         <v>301</v>
@@ -10915,19 +10915,19 @@
     </row>
     <row r="138" spans="1:31">
       <c r="A138" s="2" t="s">
-        <v>693</v>
+        <v>680</v>
       </c>
       <c r="D138" s="2" t="s">
         <v>531</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>694</v>
+        <v>681</v>
       </c>
       <c r="F138" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H138" s="2" t="s">
-        <v>695</v>
+        <v>682</v>
       </c>
       <c r="L138" s="5" t="s">
         <v>35</v>
@@ -10944,19 +10944,19 @@
     </row>
     <row r="139" spans="1:31">
       <c r="A139" s="2" t="s">
-        <v>696</v>
+        <v>683</v>
       </c>
       <c r="D139" s="2" t="s">
         <v>531</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>697</v>
+        <v>766</v>
       </c>
       <c r="F139" s="2" t="s">
         <v>40</v>
       </c>
       <c r="M139" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="S139" s="2" t="s">
         <v>301</v>
@@ -10970,19 +10970,19 @@
     </row>
     <row r="140" spans="1:31">
       <c r="A140" s="2" t="s">
-        <v>698</v>
+        <v>684</v>
       </c>
       <c r="D140" s="2" t="s">
         <v>531</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>699</v>
+        <v>767</v>
       </c>
       <c r="F140" s="2" t="s">
         <v>40</v>
       </c>
       <c r="M140" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="S140" s="2" t="s">
         <v>301</v>
@@ -10996,19 +10996,19 @@
     </row>
     <row r="141" spans="1:31">
       <c r="A141" s="2" t="s">
-        <v>700</v>
+        <v>685</v>
       </c>
       <c r="D141" s="2" t="s">
         <v>531</v>
       </c>
       <c r="E141" s="2" t="s">
-        <v>701</v>
+        <v>768</v>
       </c>
       <c r="F141" s="2" t="s">
         <v>40</v>
       </c>
       <c r="M141" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="S141" s="2" t="s">
         <v>301</v>
@@ -11022,13 +11022,13 @@
     </row>
     <row r="142" spans="1:31">
       <c r="A142" s="2" t="s">
-        <v>702</v>
+        <v>686</v>
       </c>
       <c r="D142" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>741</v>
+        <v>725</v>
       </c>
       <c r="F142" s="2" t="s">
         <v>40</v>
@@ -11045,13 +11045,13 @@
     </row>
     <row r="143" spans="1:31">
       <c r="A143" s="2" t="s">
-        <v>703</v>
+        <v>687</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E143" s="2" t="s">
-        <v>742</v>
+        <v>726</v>
       </c>
       <c r="F143" s="2" t="s">
         <v>40</v>
@@ -11068,13 +11068,13 @@
     </row>
     <row r="144" spans="1:31">
       <c r="A144" s="2" t="s">
-        <v>704</v>
+        <v>688</v>
       </c>
       <c r="D144" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E144" s="2" t="s">
-        <v>743</v>
+        <v>727</v>
       </c>
       <c r="F144" s="2" t="s">
         <v>40</v>
@@ -11091,13 +11091,13 @@
     </row>
     <row r="145" spans="1:31">
       <c r="A145" s="2" t="s">
-        <v>705</v>
+        <v>689</v>
       </c>
       <c r="D145" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>744</v>
+        <v>728</v>
       </c>
       <c r="F145" s="2" t="s">
         <v>40</v>
@@ -11114,13 +11114,13 @@
     </row>
     <row r="146" spans="1:31">
       <c r="A146" s="2" t="s">
-        <v>706</v>
+        <v>690</v>
       </c>
       <c r="D146" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>745</v>
+        <v>729</v>
       </c>
       <c r="F146" s="2" t="s">
         <v>40</v>
@@ -11137,13 +11137,13 @@
     </row>
     <row r="147" spans="1:31">
       <c r="A147" s="2" t="s">
-        <v>707</v>
+        <v>691</v>
       </c>
       <c r="D147" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E147" s="2" t="s">
-        <v>746</v>
+        <v>730</v>
       </c>
       <c r="F147" s="2" t="s">
         <v>40</v>
@@ -11160,13 +11160,13 @@
     </row>
     <row r="148" spans="1:31">
       <c r="A148" s="2" t="s">
-        <v>708</v>
+        <v>692</v>
       </c>
       <c r="D148" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E148" s="2" t="s">
-        <v>747</v>
+        <v>731</v>
       </c>
       <c r="F148" s="2" t="s">
         <v>40</v>
@@ -11183,13 +11183,13 @@
     </row>
     <row r="149" spans="1:31">
       <c r="A149" s="2" t="s">
-        <v>709</v>
+        <v>693</v>
       </c>
       <c r="D149" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E149" s="2" t="s">
-        <v>748</v>
+        <v>732</v>
       </c>
       <c r="F149" s="2" t="s">
         <v>40</v>
@@ -11206,13 +11206,13 @@
     </row>
     <row r="150" spans="1:31">
       <c r="A150" s="2" t="s">
-        <v>710</v>
+        <v>694</v>
       </c>
       <c r="D150" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E150" s="2" t="s">
-        <v>749</v>
+        <v>733</v>
       </c>
       <c r="F150" s="2" t="s">
         <v>40</v>
@@ -11229,13 +11229,13 @@
     </row>
     <row r="151" spans="1:31">
       <c r="A151" s="2" t="s">
-        <v>711</v>
+        <v>695</v>
       </c>
       <c r="D151" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E151" s="2" t="s">
-        <v>750</v>
+        <v>734</v>
       </c>
       <c r="F151" s="2" t="s">
         <v>40</v>
@@ -11252,13 +11252,13 @@
     </row>
     <row r="152" spans="1:31">
       <c r="A152" s="2" t="s">
-        <v>712</v>
+        <v>696</v>
       </c>
       <c r="D152" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E152" s="2" t="s">
-        <v>751</v>
+        <v>735</v>
       </c>
       <c r="F152" s="2" t="s">
         <v>40</v>
@@ -11275,13 +11275,13 @@
     </row>
     <row r="153" spans="1:31">
       <c r="A153" s="2" t="s">
-        <v>713</v>
+        <v>697</v>
       </c>
       <c r="D153" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E153" s="2" t="s">
-        <v>752</v>
+        <v>736</v>
       </c>
       <c r="F153" s="2" t="s">
         <v>40</v>
@@ -11298,13 +11298,13 @@
     </row>
     <row r="154" spans="1:31">
       <c r="A154" s="2" t="s">
-        <v>714</v>
+        <v>698</v>
       </c>
       <c r="D154" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E154" s="2" t="s">
-        <v>753</v>
+        <v>737</v>
       </c>
       <c r="F154" s="2" t="s">
         <v>40</v>
@@ -11321,13 +11321,13 @@
     </row>
     <row r="155" spans="1:31">
       <c r="A155" s="2" t="s">
-        <v>715</v>
+        <v>699</v>
       </c>
       <c r="D155" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E155" s="2" t="s">
-        <v>754</v>
+        <v>738</v>
       </c>
       <c r="F155" s="2" t="s">
         <v>40</v>
@@ -11344,13 +11344,13 @@
     </row>
     <row r="156" spans="1:31">
       <c r="A156" s="2" t="s">
-        <v>716</v>
+        <v>700</v>
       </c>
       <c r="D156" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E156" s="2" t="s">
-        <v>755</v>
+        <v>739</v>
       </c>
       <c r="F156" s="2" t="s">
         <v>40</v>
@@ -11367,13 +11367,13 @@
     </row>
     <row r="157" spans="1:31">
       <c r="A157" s="2" t="s">
-        <v>717</v>
+        <v>701</v>
       </c>
       <c r="D157" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E157" s="2" t="s">
-        <v>756</v>
+        <v>740</v>
       </c>
       <c r="F157" s="2" t="s">
         <v>40</v>
@@ -11390,13 +11390,13 @@
     </row>
     <row r="158" spans="1:31">
       <c r="A158" s="2" t="s">
-        <v>718</v>
+        <v>702</v>
       </c>
       <c r="D158" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E158" s="2" t="s">
-        <v>757</v>
+        <v>741</v>
       </c>
       <c r="F158" s="2" t="s">
         <v>40</v>
@@ -11413,13 +11413,13 @@
     </row>
     <row r="159" spans="1:31">
       <c r="A159" s="2" t="s">
-        <v>719</v>
+        <v>703</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E159" s="2" t="s">
-        <v>758</v>
+        <v>742</v>
       </c>
       <c r="F159" s="2" t="s">
         <v>40</v>
@@ -11436,13 +11436,13 @@
     </row>
     <row r="160" spans="1:31">
       <c r="A160" s="2" t="s">
-        <v>720</v>
+        <v>704</v>
       </c>
       <c r="D160" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E160" s="2" t="s">
-        <v>759</v>
+        <v>743</v>
       </c>
       <c r="F160" s="2" t="s">
         <v>40</v>
@@ -11459,13 +11459,13 @@
     </row>
     <row r="161" spans="1:31">
       <c r="A161" s="2" t="s">
-        <v>721</v>
+        <v>705</v>
       </c>
       <c r="D161" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E161" s="2" t="s">
-        <v>760</v>
+        <v>744</v>
       </c>
       <c r="F161" s="2" t="s">
         <v>40</v>
@@ -11482,13 +11482,13 @@
     </row>
     <row r="162" spans="1:31">
       <c r="A162" s="2" t="s">
-        <v>722</v>
+        <v>706</v>
       </c>
       <c r="D162" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E162" s="2" t="s">
-        <v>761</v>
+        <v>745</v>
       </c>
       <c r="F162" s="2" t="s">
         <v>40</v>
@@ -11505,13 +11505,13 @@
     </row>
     <row r="163" spans="1:31">
       <c r="A163" s="2" t="s">
-        <v>723</v>
+        <v>707</v>
       </c>
       <c r="D163" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E163" s="2" t="s">
-        <v>762</v>
+        <v>746</v>
       </c>
       <c r="F163" s="2" t="s">
         <v>40</v>
@@ -11528,13 +11528,13 @@
     </row>
     <row r="164" spans="1:31">
       <c r="A164" s="2" t="s">
-        <v>724</v>
+        <v>708</v>
       </c>
       <c r="D164" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E164" s="2" t="s">
-        <v>763</v>
+        <v>747</v>
       </c>
       <c r="F164" s="2" t="s">
         <v>40</v>
@@ -11551,13 +11551,13 @@
     </row>
     <row r="165" spans="1:31">
       <c r="A165" s="2" t="s">
-        <v>725</v>
+        <v>709</v>
       </c>
       <c r="D165" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E165" s="2" t="s">
-        <v>764</v>
+        <v>748</v>
       </c>
       <c r="F165" s="2" t="s">
         <v>40</v>
@@ -11574,13 +11574,13 @@
     </row>
     <row r="166" spans="1:31">
       <c r="A166" s="2" t="s">
-        <v>726</v>
+        <v>710</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E166" s="2" t="s">
-        <v>765</v>
+        <v>749</v>
       </c>
       <c r="F166" s="2" t="s">
         <v>40</v>
@@ -11597,13 +11597,13 @@
     </row>
     <row r="167" spans="1:31">
       <c r="A167" s="2" t="s">
-        <v>727</v>
+        <v>711</v>
       </c>
       <c r="D167" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E167" s="2" t="s">
-        <v>766</v>
+        <v>750</v>
       </c>
       <c r="F167" s="2" t="s">
         <v>40</v>
@@ -11620,13 +11620,13 @@
     </row>
     <row r="168" spans="1:31">
       <c r="A168" s="2" t="s">
-        <v>728</v>
+        <v>712</v>
       </c>
       <c r="D168" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E168" s="2" t="s">
-        <v>767</v>
+        <v>751</v>
       </c>
       <c r="F168" s="2" t="s">
         <v>40</v>
@@ -11643,13 +11643,13 @@
     </row>
     <row r="169" spans="1:31">
       <c r="A169" s="2" t="s">
-        <v>729</v>
+        <v>713</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E169" s="2" t="s">
-        <v>768</v>
+        <v>752</v>
       </c>
       <c r="F169" s="2" t="s">
         <v>40</v>
@@ -11666,13 +11666,13 @@
     </row>
     <row r="170" spans="1:31">
       <c r="A170" s="2" t="s">
-        <v>730</v>
+        <v>714</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E170" s="2" t="s">
-        <v>769</v>
+        <v>753</v>
       </c>
       <c r="F170" s="2" t="s">
         <v>40</v>
@@ -11689,13 +11689,13 @@
     </row>
     <row r="171" spans="1:31">
       <c r="A171" s="2" t="s">
-        <v>731</v>
+        <v>715</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E171" s="2" t="s">
-        <v>770</v>
+        <v>754</v>
       </c>
       <c r="F171" s="2" t="s">
         <v>40</v>
@@ -11712,13 +11712,13 @@
     </row>
     <row r="172" spans="1:31">
       <c r="A172" s="2" t="s">
-        <v>732</v>
+        <v>716</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E172" s="2" t="s">
-        <v>771</v>
+        <v>755</v>
       </c>
       <c r="F172" s="2" t="s">
         <v>40</v>
@@ -11735,13 +11735,13 @@
     </row>
     <row r="173" spans="1:31">
       <c r="A173" s="2" t="s">
-        <v>733</v>
+        <v>717</v>
       </c>
       <c r="D173" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E173" s="2" t="s">
-        <v>772</v>
+        <v>756</v>
       </c>
       <c r="F173" s="2" t="s">
         <v>40</v>
@@ -11758,13 +11758,13 @@
     </row>
     <row r="174" spans="1:31">
       <c r="A174" s="2" t="s">
-        <v>734</v>
+        <v>718</v>
       </c>
       <c r="D174" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E174" s="2" t="s">
-        <v>773</v>
+        <v>757</v>
       </c>
       <c r="F174" s="2" t="s">
         <v>40</v>
@@ -11781,7 +11781,7 @@
     </row>
     <row r="175" spans="1:31">
       <c r="A175" s="2" t="s">
-        <v>735</v>
+        <v>719</v>
       </c>
       <c r="B175" s="2" t="s">
         <v>35</v>
@@ -11790,7 +11790,7 @@
         <v>342</v>
       </c>
       <c r="E175" s="2" t="s">
-        <v>774</v>
+        <v>758</v>
       </c>
       <c r="F175" s="2" t="s">
         <v>40</v>
@@ -11807,13 +11807,13 @@
     </row>
     <row r="176" spans="1:31">
       <c r="A176" s="2" t="s">
-        <v>736</v>
+        <v>720</v>
       </c>
       <c r="D176" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E176" s="2" t="s">
-        <v>775</v>
+        <v>759</v>
       </c>
       <c r="F176" s="2" t="s">
         <v>40</v>
@@ -11830,13 +11830,13 @@
     </row>
     <row r="177" spans="1:31">
       <c r="A177" s="2" t="s">
-        <v>737</v>
+        <v>721</v>
       </c>
       <c r="D177" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E177" s="2" t="s">
-        <v>776</v>
+        <v>760</v>
       </c>
       <c r="F177" s="2" t="s">
         <v>40</v>
@@ -11853,13 +11853,13 @@
     </row>
     <row r="178" spans="1:31">
       <c r="A178" s="2" t="s">
-        <v>738</v>
+        <v>722</v>
       </c>
       <c r="D178" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E178" s="2" t="s">
-        <v>777</v>
+        <v>761</v>
       </c>
       <c r="F178" s="2" t="s">
         <v>40</v>
@@ -11876,13 +11876,13 @@
     </row>
     <row r="179" spans="1:31">
       <c r="A179" s="2" t="s">
-        <v>780</v>
+        <v>764</v>
       </c>
       <c r="D179" s="2" t="s">
         <v>342</v>
       </c>
       <c r="E179" s="2" t="s">
-        <v>778</v>
+        <v>762</v>
       </c>
       <c r="F179" s="2" t="s">
         <v>40</v>
@@ -11899,7 +11899,7 @@
     </row>
     <row r="180" spans="1:31">
       <c r="A180" s="2" t="s">
-        <v>781</v>
+        <v>765</v>
       </c>
       <c r="B180" s="2" t="s">
         <v>35</v>
@@ -11908,7 +11908,7 @@
         <v>342</v>
       </c>
       <c r="E180" s="2" t="s">
-        <v>779</v>
+        <v>763</v>
       </c>
       <c r="F180" s="2" t="s">
         <v>40</v>

</xml_diff>